<commit_message>
folders and .md files created
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -1,37 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24617"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_11df\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1248" documentId="11_ABF58B18D3B8FFB319BD2B146303C194C61A962A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D444A96F-937B-4844-8267-409C983A9AEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846BE123-0685-464C-ABFD-7A2DBABC6681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="562">
   <si>
     <t>Themen</t>
   </si>
@@ -1711,13 +1700,19 @@
   </si>
   <si>
     <t>Kanban_Swim_Lanes</t>
+  </si>
+  <si>
+    <t>Ishikawa_Methode</t>
+  </si>
+  <si>
+    <t>Projektmanagementhandbuch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2107,20 +2102,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="A350" sqref="A350"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="A208" sqref="A208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="83.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2136,7 +2131,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2144,7 +2139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2152,7 +2147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2161,7 +2156,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2169,7 +2164,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2177,7 +2172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2185,7 +2180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2193,7 +2188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2201,7 +2196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2209,7 +2204,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2217,7 +2212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2225,7 +2220,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2233,7 +2228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2241,7 +2236,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2249,7 +2244,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2257,7 +2252,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2265,7 +2260,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2273,7 +2268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2281,7 +2276,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2289,7 +2284,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2297,7 +2292,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2305,7 +2300,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2313,7 +2308,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2321,7 +2316,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2329,7 +2324,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2337,7 +2332,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2345,7 +2340,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2353,7 +2348,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2361,7 +2356,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -2369,7 +2364,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -2377,7 +2372,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -2385,7 +2380,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -2393,7 +2388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -2401,7 +2396,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -2409,7 +2404,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -2417,7 +2412,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2425,7 +2420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -2433,7 +2428,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2441,7 +2436,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2449,7 +2444,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -2457,7 +2452,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -2465,7 +2460,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -2474,7 +2469,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -2483,7 +2478,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2491,7 +2486,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2499,7 +2494,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2507,7 +2502,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -2515,7 +2510,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -2523,7 +2518,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -2531,7 +2526,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>96</v>
       </c>
@@ -2539,7 +2534,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>98</v>
       </c>
@@ -2547,7 +2542,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>100</v>
       </c>
@@ -2555,7 +2550,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>102</v>
       </c>
@@ -2563,7 +2558,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -2571,7 +2566,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -2579,7 +2574,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -2587,7 +2582,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -2595,7 +2590,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -2603,7 +2598,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>113</v>
       </c>
@@ -2611,7 +2606,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>115</v>
       </c>
@@ -2619,7 +2614,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -2627,7 +2622,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -2635,7 +2630,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>121</v>
       </c>
@@ -2643,7 +2638,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>122</v>
       </c>
@@ -2651,7 +2646,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>124</v>
       </c>
@@ -2659,7 +2654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>125</v>
       </c>
@@ -2667,7 +2662,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -2675,7 +2670,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -2683,7 +2678,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>131</v>
       </c>
@@ -2691,7 +2686,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -2699,7 +2694,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>134</v>
       </c>
@@ -2707,7 +2702,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>136</v>
       </c>
@@ -2715,7 +2710,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>138</v>
       </c>
@@ -2723,7 +2718,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>140</v>
       </c>
@@ -2731,7 +2726,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>141</v>
       </c>
@@ -2739,7 +2734,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>143</v>
       </c>
@@ -2747,7 +2742,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>144</v>
       </c>
@@ -2755,7 +2750,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>146</v>
       </c>
@@ -2763,7 +2758,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>148</v>
       </c>
@@ -2771,7 +2766,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>150</v>
       </c>
@@ -2779,7 +2774,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>152</v>
       </c>
@@ -2787,7 +2782,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>154</v>
       </c>
@@ -2795,7 +2790,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>156</v>
       </c>
@@ -2803,7 +2798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>157</v>
       </c>
@@ -2811,7 +2806,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>159</v>
       </c>
@@ -2819,7 +2814,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>161</v>
       </c>
@@ -2827,7 +2822,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>163</v>
       </c>
@@ -2835,7 +2830,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>165</v>
       </c>
@@ -2843,7 +2838,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>166</v>
       </c>
@@ -2851,7 +2846,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>168</v>
       </c>
@@ -2859,7 +2854,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>170</v>
       </c>
@@ -2867,7 +2862,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>172</v>
       </c>
@@ -2875,7 +2870,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>174</v>
       </c>
@@ -2883,7 +2878,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>176</v>
       </c>
@@ -2891,7 +2886,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>178</v>
       </c>
@@ -2899,7 +2894,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>180</v>
       </c>
@@ -2907,7 +2902,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>182</v>
       </c>
@@ -2915,7 +2910,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>184</v>
       </c>
@@ -2923,7 +2918,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>186</v>
       </c>
@@ -2931,7 +2926,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>188</v>
       </c>
@@ -2939,7 +2934,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>190</v>
       </c>
@@ -2947,7 +2942,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>192</v>
       </c>
@@ -2955,7 +2950,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>194</v>
       </c>
@@ -2963,7 +2958,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>196</v>
       </c>
@@ -2971,7 +2966,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>197</v>
       </c>
@@ -2980,7 +2975,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>198</v>
       </c>
@@ -2988,7 +2983,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>200</v>
       </c>
@@ -2996,7 +2991,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>202</v>
       </c>
@@ -3004,7 +2999,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>204</v>
       </c>
@@ -3012,7 +3007,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>206</v>
       </c>
@@ -3020,7 +3015,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>208</v>
       </c>
@@ -3028,7 +3023,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>210</v>
       </c>
@@ -3036,7 +3031,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>212</v>
       </c>
@@ -3044,7 +3039,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>214</v>
       </c>
@@ -3052,7 +3047,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>216</v>
       </c>
@@ -3060,7 +3055,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>218</v>
       </c>
@@ -3068,7 +3063,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>219</v>
       </c>
@@ -3076,7 +3071,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>220</v>
       </c>
@@ -3084,7 +3079,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>222</v>
       </c>
@@ -3092,7 +3087,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>224</v>
       </c>
@@ -3100,7 +3095,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>226</v>
       </c>
@@ -3108,7 +3103,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>228</v>
       </c>
@@ -3116,7 +3111,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>230</v>
       </c>
@@ -3124,7 +3119,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>232</v>
       </c>
@@ -3132,7 +3127,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>234</v>
       </c>
@@ -3140,7 +3135,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>236</v>
       </c>
@@ -3148,7 +3143,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>237</v>
       </c>
@@ -3156,7 +3151,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>238</v>
       </c>
@@ -3164,7 +3159,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>240</v>
       </c>
@@ -3172,7 +3167,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>241</v>
       </c>
@@ -3180,7 +3175,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>243</v>
       </c>
@@ -3188,7 +3183,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>245</v>
       </c>
@@ -3196,7 +3191,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>246</v>
       </c>
@@ -3204,7 +3199,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>248</v>
       </c>
@@ -3212,7 +3207,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>250</v>
       </c>
@@ -3220,7 +3215,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>252</v>
       </c>
@@ -3228,7 +3223,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>254</v>
       </c>
@@ -3236,7 +3231,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>256</v>
       </c>
@@ -3244,7 +3239,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>257</v>
       </c>
@@ -3252,7 +3247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>258</v>
       </c>
@@ -3260,7 +3255,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>260</v>
       </c>
@@ -3268,7 +3263,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>261</v>
       </c>
@@ -3276,7 +3271,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>262</v>
       </c>
@@ -3284,7 +3279,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>264</v>
       </c>
@@ -3292,7 +3287,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>265</v>
       </c>
@@ -3300,7 +3295,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>266</v>
       </c>
@@ -3308,7 +3303,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>267</v>
       </c>
@@ -3316,7 +3311,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>269</v>
       </c>
@@ -3324,7 +3319,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>271</v>
       </c>
@@ -3332,7 +3327,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>273</v>
       </c>
@@ -3340,7 +3335,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>275</v>
       </c>
@@ -3348,7 +3343,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>276</v>
       </c>
@@ -3356,7 +3351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>277</v>
       </c>
@@ -3364,7 +3359,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>278</v>
       </c>
@@ -3372,7 +3367,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>279</v>
       </c>
@@ -3380,7 +3375,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>280</v>
       </c>
@@ -3388,7 +3383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>281</v>
       </c>
@@ -3396,7 +3391,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>283</v>
       </c>
@@ -3404,7 +3399,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>285</v>
       </c>
@@ -3412,7 +3407,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>287</v>
       </c>
@@ -3420,7 +3415,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>289</v>
       </c>
@@ -3428,7 +3423,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>291</v>
       </c>
@@ -3436,7 +3431,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>293</v>
       </c>
@@ -3444,7 +3439,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>295</v>
       </c>
@@ -3452,7 +3447,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>296</v>
       </c>
@@ -3460,7 +3455,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>298</v>
       </c>
@@ -3468,7 +3463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>299</v>
       </c>
@@ -3476,7 +3471,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>300</v>
       </c>
@@ -3484,7 +3479,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>302</v>
       </c>
@@ -3492,7 +3487,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>304</v>
       </c>
@@ -3500,7 +3495,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>306</v>
       </c>
@@ -3508,7 +3503,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>307</v>
       </c>
@@ -3516,7 +3511,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>309</v>
       </c>
@@ -3524,7 +3519,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>311</v>
       </c>
@@ -3532,7 +3527,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>313</v>
       </c>
@@ -3540,7 +3535,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>315</v>
       </c>
@@ -3548,7 +3543,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>317</v>
       </c>
@@ -3556,7 +3551,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>318</v>
       </c>
@@ -3564,7 +3559,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>320</v>
       </c>
@@ -3572,7 +3567,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>322</v>
       </c>
@@ -3580,7 +3575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>323</v>
       </c>
@@ -3588,7 +3583,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>325</v>
       </c>
@@ -3596,7 +3591,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>327</v>
       </c>
@@ -3604,7 +3599,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>329</v>
       </c>
@@ -3612,7 +3607,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>331</v>
       </c>
@@ -3620,7 +3615,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>332</v>
       </c>
@@ -3628,7 +3623,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>333</v>
       </c>
@@ -3636,7 +3631,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>335</v>
       </c>
@@ -3644,7 +3639,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>337</v>
       </c>
@@ -3652,7 +3647,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>339</v>
       </c>
@@ -3660,7 +3655,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>340</v>
       </c>
@@ -3668,7 +3663,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>341</v>
       </c>
@@ -3676,7 +3671,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>343</v>
       </c>
@@ -3684,7 +3679,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>345</v>
       </c>
@@ -3692,7 +3687,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>347</v>
       </c>
@@ -3700,7 +3695,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>349</v>
       </c>
@@ -3708,7 +3703,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5">
+    <row r="198" spans="1:2" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
         <v>351</v>
       </c>
@@ -3716,7 +3711,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>353</v>
       </c>
@@ -3724,7 +3719,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>355</v>
       </c>
@@ -3732,7 +3727,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>357</v>
       </c>
@@ -3740,7 +3735,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>359</v>
       </c>
@@ -3748,7 +3743,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>361</v>
       </c>
@@ -3756,7 +3751,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>363</v>
       </c>
@@ -3764,7 +3759,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>365</v>
       </c>
@@ -3772,7 +3767,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>366</v>
       </c>
@@ -3780,7 +3775,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>368</v>
       </c>
@@ -3788,15 +3783,15 @@
         <v>369</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>109</v>
+        <v>561</v>
       </c>
       <c r="B208" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>370</v>
       </c>
@@ -3804,7 +3799,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>372</v>
       </c>
@@ -3812,7 +3807,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>374</v>
       </c>
@@ -3820,7 +3815,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>376</v>
       </c>
@@ -3828,7 +3823,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>378</v>
       </c>
@@ -3836,7 +3831,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>380</v>
       </c>
@@ -3844,7 +3839,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>382</v>
       </c>
@@ -3852,7 +3847,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>383</v>
       </c>
@@ -3860,7 +3855,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>385</v>
       </c>
@@ -3868,7 +3863,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>387</v>
       </c>
@@ -3876,7 +3871,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>389</v>
       </c>
@@ -3884,7 +3879,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>390</v>
       </c>
@@ -3892,7 +3887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>391</v>
       </c>
@@ -3900,7 +3895,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>393</v>
       </c>
@@ -3908,7 +3903,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>395</v>
       </c>
@@ -3916,7 +3911,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>397</v>
       </c>
@@ -3924,7 +3919,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>399</v>
       </c>
@@ -3932,7 +3927,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>401</v>
       </c>
@@ -3940,7 +3935,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>403</v>
       </c>
@@ -3948,7 +3943,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>405</v>
       </c>
@@ -3956,7 +3951,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>407</v>
       </c>
@@ -3964,7 +3959,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>409</v>
       </c>
@@ -3972,7 +3967,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>411</v>
       </c>
@@ -3980,7 +3975,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>412</v>
       </c>
@@ -3988,7 +3983,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>414</v>
       </c>
@@ -3996,7 +3991,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>415</v>
       </c>
@@ -4004,7 +3999,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>417</v>
       </c>
@@ -4012,7 +4007,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>419</v>
       </c>
@@ -4020,7 +4015,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>421</v>
       </c>
@@ -4028,7 +4023,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>423</v>
       </c>
@@ -4036,7 +4031,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>425</v>
       </c>
@@ -4044,7 +4039,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>427</v>
       </c>
@@ -4052,7 +4047,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>428</v>
       </c>
@@ -4060,7 +4055,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>430</v>
       </c>
@@ -4068,7 +4063,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>432</v>
       </c>
@@ -4076,7 +4071,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>433</v>
       </c>
@@ -4084,7 +4079,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>435</v>
       </c>
@@ -4092,7 +4087,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>437</v>
       </c>
@@ -4100,7 +4095,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>439</v>
       </c>
@@ -4108,7 +4103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>440</v>
       </c>
@@ -4116,7 +4111,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>441</v>
       </c>
@@ -4124,7 +4119,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>443</v>
       </c>
@@ -4132,7 +4127,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>445</v>
       </c>
@@ -4140,7 +4135,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>447</v>
       </c>
@@ -4148,7 +4143,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>448</v>
       </c>
@@ -4156,7 +4151,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>450</v>
       </c>
@@ -4164,7 +4159,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>451</v>
       </c>
@@ -4172,7 +4167,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>452</v>
       </c>
@@ -4180,7 +4175,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>453</v>
       </c>
@@ -4188,7 +4183,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>454</v>
       </c>
@@ -4196,7 +4191,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>455</v>
       </c>
@@ -4204,7 +4199,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>456</v>
       </c>
@@ -4212,7 +4207,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>458</v>
       </c>
@@ -4220,7 +4215,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>460</v>
       </c>
@@ -4228,7 +4223,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>462</v>
       </c>
@@ -4236,7 +4231,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>463</v>
       </c>
@@ -4244,7 +4239,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>465</v>
       </c>
@@ -4252,7 +4247,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>467</v>
       </c>
@@ -4260,7 +4255,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>469</v>
       </c>
@@ -4268,7 +4263,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>470</v>
       </c>
@@ -4276,7 +4271,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>471</v>
       </c>
@@ -4284,7 +4279,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>473</v>
       </c>
@@ -4292,7 +4287,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>474</v>
       </c>
@@ -4300,7 +4295,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>475</v>
       </c>
@@ -4308,7 +4303,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>476</v>
       </c>
@@ -4316,7 +4311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>477</v>
       </c>
@@ -4324,7 +4319,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>479</v>
       </c>
@@ -4332,7 +4327,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>480</v>
       </c>
@@ -4340,7 +4335,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>481</v>
       </c>
@@ -4348,7 +4343,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>483</v>
       </c>
@@ -4356,7 +4351,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>485</v>
       </c>
@@ -4364,7 +4359,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>486</v>
       </c>
@@ -4372,7 +4367,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>487</v>
       </c>
@@ -4380,7 +4375,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>489</v>
       </c>
@@ -4388,7 +4383,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>490</v>
       </c>
@@ -4396,7 +4391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>491</v>
       </c>
@@ -4404,7 +4399,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>492</v>
       </c>
@@ -4412,7 +4407,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>493</v>
       </c>
@@ -4420,7 +4415,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>494</v>
       </c>
@@ -4428,7 +4423,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>495</v>
       </c>
@@ -4436,7 +4431,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>496</v>
       </c>
@@ -4444,7 +4439,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>498</v>
       </c>
@@ -4452,7 +4447,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>500</v>
       </c>
@@ -4460,7 +4455,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>501</v>
       </c>
@@ -4468,7 +4463,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>502</v>
       </c>
@@ -4476,7 +4471,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>503</v>
       </c>
@@ -4484,7 +4479,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>504</v>
       </c>
@@ -4492,7 +4487,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>505</v>
       </c>
@@ -4500,7 +4495,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>506</v>
       </c>
@@ -4508,7 +4503,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>507</v>
       </c>
@@ -4516,7 +4511,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>508</v>
       </c>
@@ -4524,7 +4519,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>509</v>
       </c>
@@ -4532,7 +4527,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>511</v>
       </c>
@@ -4540,7 +4535,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>512</v>
       </c>
@@ -4548,7 +4543,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>513</v>
       </c>
@@ -4556,7 +4551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>514</v>
       </c>
@@ -4564,7 +4559,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>515</v>
       </c>
@@ -4572,7 +4567,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>516</v>
       </c>
@@ -4580,7 +4575,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>517</v>
       </c>
@@ -4588,7 +4583,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>518</v>
       </c>
@@ -4596,7 +4591,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>519</v>
       </c>
@@ -4604,7 +4599,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>520</v>
       </c>
@@ -4612,7 +4607,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>522</v>
       </c>
@@ -4620,7 +4615,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>523</v>
       </c>
@@ -4628,7 +4623,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>524</v>
       </c>
@@ -4636,7 +4631,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>525</v>
       </c>
@@ -4644,7 +4639,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>526</v>
       </c>
@@ -4652,7 +4647,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>527</v>
       </c>
@@ -4660,7 +4655,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>528</v>
       </c>
@@ -4668,7 +4663,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>529</v>
       </c>
@@ -4676,7 +4671,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>531</v>
       </c>
@@ -4684,7 +4679,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>532</v>
       </c>
@@ -4692,7 +4687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>533</v>
       </c>
@@ -4700,7 +4695,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>534</v>
       </c>
@@ -4708,7 +4703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>535</v>
       </c>
@@ -4716,7 +4711,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>537</v>
       </c>
@@ -4724,7 +4719,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>538</v>
       </c>
@@ -4732,7 +4727,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>539</v>
       </c>
@@ -4740,15 +4735,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>460</v>
+        <v>560</v>
       </c>
       <c r="B327" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>540</v>
       </c>
@@ -4756,7 +4751,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>541</v>
       </c>
@@ -4764,7 +4759,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
         <v>542</v>
       </c>
@@ -4772,7 +4767,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
         <v>544</v>
       </c>
@@ -4780,7 +4775,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
         <v>545</v>
       </c>
@@ -4788,7 +4783,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>546</v>
       </c>
@@ -4796,7 +4791,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>547</v>
       </c>
@@ -4804,7 +4799,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="335" spans="1:2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>548</v>
       </c>
@@ -4812,7 +4807,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="336" spans="1:2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>549</v>
       </c>
@@ -4820,7 +4815,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="337" spans="1:2">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>551</v>
       </c>
@@ -4828,7 +4823,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="338" spans="1:2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>553</v>
       </c>
@@ -4836,7 +4831,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="339" spans="1:2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>555</v>
       </c>
@@ -4844,7 +4839,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="340" spans="1:2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>557</v>
       </c>
@@ -4852,7 +4847,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="341" spans="1:2">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>559</v>
       </c>
@@ -4866,6 +4861,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CDD89E2A6189134493471C3B1248FFEC" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f8c835211e191b604f15d9c196fd702e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73be11ab-4534-422f-8ab6-049e22ac882d" xmlns:ns3="142bc323-bc41-43fc-a839-79fc38759c0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e35637ed6ab77bc02eb788b6a909f82" ns2:_="" ns3:_="">
     <xsd:import namespace="73be11ab-4534-422f-8ab6-049e22ac882d"/>
@@ -5068,29 +5078,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A5431A-F902-4554-AE88-9292CACE75EC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A5431A-F902-4554-AE88-9292CACE75EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="73be11ab-4534-422f-8ab6-049e22ac882d"/>
+    <ds:schemaRef ds:uri="142bc323-bc41-43fc-a839-79fc38759c0e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update beschreibung + template
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -2237,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H369"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5361,18 +5361,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5395,18 +5395,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added gitignore + einige NachzüglerInnen
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="611">
   <si>
     <t>Themen</t>
   </si>
@@ -1819,13 +1819,49 @@
   </si>
   <si>
     <t>domirow-fau</t>
+  </si>
+  <si>
+    <t>Adaye1e</t>
+  </si>
+  <si>
+    <t>enesmvlt</t>
+  </si>
+  <si>
+    <t>tkessler94</t>
+  </si>
+  <si>
+    <t>AmrouHasan</t>
+  </si>
+  <si>
+    <t>juliwebair</t>
+  </si>
+  <si>
+    <t>Irishcoffee09</t>
+  </si>
+  <si>
+    <t>bilgesb</t>
+  </si>
+  <si>
+    <t>TobiasZuerrlein</t>
+  </si>
+  <si>
+    <t>lukasheinrich9</t>
+  </si>
+  <si>
+    <t>fe94fiqy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaskiaHe </t>
+  </si>
+  <si>
+    <t>EuleW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1876,8 +1912,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1888,6 +1931,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1918,7 +1967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1933,6 +1982,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2235,10 +2286,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2266,7 +2318,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2274,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2282,7 +2334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2291,7 +2343,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2299,7 +2351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2307,7 +2359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2315,7 +2367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2323,7 +2375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2331,7 +2383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2339,7 +2391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2347,7 +2399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2355,7 +2407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2363,7 +2415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2371,7 +2423,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2379,7 +2431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2387,7 +2439,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" hidden="1">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2395,7 +2447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" hidden="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2403,7 +2455,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" hidden="1">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2411,7 +2463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" hidden="1">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2419,7 +2471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" hidden="1">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2427,7 +2479,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" hidden="1">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2435,7 +2487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" hidden="1">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2443,7 +2495,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" hidden="1">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2451,7 +2503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" hidden="1">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2459,7 +2511,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" hidden="1">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2467,7 +2519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" hidden="1">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2475,7 +2527,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" hidden="1">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2492,8 +2544,11 @@
       <c r="A30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="B30" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2501,7 +2556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" hidden="1">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2509,7 +2564,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2517,7 +2572,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2525,7 +2580,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" hidden="1">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2533,7 +2588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" hidden="1">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2541,7 +2596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2554,7 +2609,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2562,7 +2617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2570,7 +2625,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2578,7 +2633,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2586,7 +2641,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2595,7 +2650,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2604,7 +2659,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2612,7 +2667,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2624,8 +2679,11 @@
       <c r="A47" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="B47" s="10" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" hidden="1">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -2633,7 +2691,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" hidden="1">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -2641,7 +2699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" hidden="1">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -2649,7 +2707,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" hidden="1">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2657,7 +2715,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" hidden="1">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2665,7 +2723,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" hidden="1">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2673,7 +2731,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" hidden="1">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2681,7 +2739,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" hidden="1">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2689,7 +2747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" hidden="1">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2697,7 +2755,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" hidden="1">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2705,7 +2763,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" hidden="1">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2713,7 +2771,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" hidden="1">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2721,7 +2779,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" hidden="1">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2729,7 +2787,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" hidden="1">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -2737,7 +2795,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" hidden="1">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -2745,7 +2803,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" hidden="1">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -2753,7 +2811,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" hidden="1">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -2761,7 +2819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" hidden="1">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -2769,7 +2827,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" hidden="1">
       <c r="A66" t="s">
         <v>123</v>
       </c>
@@ -2777,7 +2835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" hidden="1">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -2785,7 +2843,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -2793,7 +2851,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" hidden="1">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -2801,7 +2859,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" hidden="1">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -2813,8 +2871,11 @@
       <c r="A71" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="B71" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -2822,7 +2883,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" hidden="1">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -2830,7 +2891,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" hidden="1">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -2838,7 +2899,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" hidden="1">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -2846,7 +2907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" hidden="1">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -2854,7 +2915,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" hidden="1">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2862,7 +2923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" hidden="1">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2870,7 +2931,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" hidden="1">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2878,7 +2939,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" hidden="1">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2886,7 +2947,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" hidden="1">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2894,7 +2955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" hidden="1">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -2902,7 +2963,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" hidden="1">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -2910,7 +2971,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" hidden="1">
       <c r="A84" t="s">
         <v>155</v>
       </c>
@@ -2918,7 +2979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" hidden="1">
       <c r="A85" t="s">
         <v>156</v>
       </c>
@@ -2926,7 +2987,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" hidden="1">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -2934,7 +2995,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" hidden="1">
       <c r="A87" t="s">
         <v>160</v>
       </c>
@@ -2942,7 +3003,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" hidden="1">
       <c r="A88" t="s">
         <v>162</v>
       </c>
@@ -2950,7 +3011,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" hidden="1">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -2958,7 +3019,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" hidden="1">
       <c r="A90" t="s">
         <v>165</v>
       </c>
@@ -2966,7 +3027,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" hidden="1">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -2974,7 +3035,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" hidden="1">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -2982,7 +3043,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" hidden="1">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -2990,7 +3051,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" hidden="1">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -2998,7 +3059,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" hidden="1">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -3006,7 +3067,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" hidden="1">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3014,7 +3075,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" hidden="1">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -3022,7 +3083,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" hidden="1">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -3030,7 +3091,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" hidden="1">
       <c r="A99" t="s">
         <v>183</v>
       </c>
@@ -3038,7 +3099,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" hidden="1">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -3046,7 +3107,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" hidden="1">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -3054,7 +3115,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" hidden="1">
       <c r="A102" t="s">
         <v>189</v>
       </c>
@@ -3062,7 +3123,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" hidden="1">
       <c r="A103" t="s">
         <v>191</v>
       </c>
@@ -3070,7 +3131,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" hidden="1">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -3078,7 +3139,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" hidden="1">
       <c r="A105" t="s">
         <v>195</v>
       </c>
@@ -3086,7 +3147,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" hidden="1">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -3095,7 +3156,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" hidden="1">
       <c r="A107" t="s">
         <v>197</v>
       </c>
@@ -3103,7 +3164,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" hidden="1">
       <c r="A108" t="s">
         <v>199</v>
       </c>
@@ -3111,7 +3172,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" hidden="1">
       <c r="A109" t="s">
         <v>201</v>
       </c>
@@ -3119,7 +3180,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1">
       <c r="A110" t="s">
         <v>203</v>
       </c>
@@ -3127,7 +3188,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" hidden="1">
       <c r="A111" t="s">
         <v>205</v>
       </c>
@@ -3135,7 +3196,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" hidden="1">
       <c r="A112" t="s">
         <v>207</v>
       </c>
@@ -3143,7 +3204,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" hidden="1">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -3151,7 +3212,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" hidden="1">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -3159,7 +3220,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" hidden="1">
       <c r="A115" t="s">
         <v>213</v>
       </c>
@@ -3167,7 +3228,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" hidden="1">
       <c r="A116" t="s">
         <v>215</v>
       </c>
@@ -3175,7 +3236,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" hidden="1">
       <c r="A117" t="s">
         <v>217</v>
       </c>
@@ -3183,7 +3244,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" hidden="1">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3191,7 +3252,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" hidden="1">
       <c r="A119" t="s">
         <v>219</v>
       </c>
@@ -3199,7 +3260,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" hidden="1">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -3207,7 +3268,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" hidden="1">
       <c r="A121" t="s">
         <v>223</v>
       </c>
@@ -3215,7 +3276,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" hidden="1">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -3223,7 +3284,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" hidden="1">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -3231,7 +3292,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" hidden="1">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -3239,7 +3300,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" hidden="1">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -3247,7 +3308,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" hidden="1">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -3255,7 +3316,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" hidden="1">
       <c r="A127" t="s">
         <v>235</v>
       </c>
@@ -3263,7 +3324,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" hidden="1">
       <c r="A128" t="s">
         <v>236</v>
       </c>
@@ -3276,7 +3337,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" hidden="1">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -3284,7 +3345,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" hidden="1">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -3292,7 +3353,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" hidden="1">
       <c r="A132" t="s">
         <v>242</v>
       </c>
@@ -3300,7 +3361,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" hidden="1">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -3308,7 +3369,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" hidden="1">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -3316,7 +3377,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" hidden="1">
       <c r="A135" t="s">
         <v>247</v>
       </c>
@@ -3324,7 +3385,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" hidden="1">
       <c r="A136" t="s">
         <v>249</v>
       </c>
@@ -3332,7 +3393,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" hidden="1">
       <c r="A137" t="s">
         <v>251</v>
       </c>
@@ -3340,7 +3401,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" hidden="1">
       <c r="A138" t="s">
         <v>253</v>
       </c>
@@ -3352,13 +3413,19 @@
       <c r="A139" t="s">
         <v>255</v>
       </c>
+      <c r="B139" s="10" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="B140" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" hidden="1">
       <c r="A141" t="s">
         <v>257</v>
       </c>
@@ -3366,7 +3433,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" hidden="1">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -3374,7 +3441,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" hidden="1">
       <c r="A143" t="s">
         <v>260</v>
       </c>
@@ -3382,7 +3449,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" hidden="1">
       <c r="A144" t="s">
         <v>261</v>
       </c>
@@ -3390,7 +3457,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" hidden="1">
       <c r="A145" t="s">
         <v>263</v>
       </c>
@@ -3398,7 +3465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" hidden="1">
       <c r="A146" t="s">
         <v>264</v>
       </c>
@@ -3406,7 +3473,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" hidden="1">
       <c r="A147" t="s">
         <v>265</v>
       </c>
@@ -3414,7 +3481,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" hidden="1">
       <c r="A148" t="s">
         <v>266</v>
       </c>
@@ -3422,7 +3489,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" hidden="1">
       <c r="A149" t="s">
         <v>268</v>
       </c>
@@ -3430,7 +3497,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" hidden="1">
       <c r="A150" t="s">
         <v>270</v>
       </c>
@@ -3438,7 +3505,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" hidden="1">
       <c r="A151" t="s">
         <v>272</v>
       </c>
@@ -3446,7 +3513,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" hidden="1">
       <c r="A152" t="s">
         <v>274</v>
       </c>
@@ -3454,7 +3521,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" hidden="1">
       <c r="A153" t="s">
         <v>275</v>
       </c>
@@ -3462,7 +3529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" hidden="1">
       <c r="A154" t="s">
         <v>276</v>
       </c>
@@ -3470,7 +3537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" hidden="1">
       <c r="A155" t="s">
         <v>277</v>
       </c>
@@ -3478,7 +3545,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" hidden="1">
       <c r="A156" t="s">
         <v>278</v>
       </c>
@@ -3490,8 +3557,11 @@
       <c r="A157" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="158" spans="1:2">
+      <c r="B157" s="10" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" hidden="1">
       <c r="A158" t="s">
         <v>280</v>
       </c>
@@ -3499,7 +3569,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" hidden="1">
       <c r="A159" t="s">
         <v>282</v>
       </c>
@@ -3507,7 +3577,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" hidden="1">
       <c r="A160" t="s">
         <v>284</v>
       </c>
@@ -3515,7 +3585,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" hidden="1">
       <c r="A161" t="s">
         <v>286</v>
       </c>
@@ -3523,7 +3593,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" hidden="1">
       <c r="A162" t="s">
         <v>288</v>
       </c>
@@ -3531,7 +3601,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" hidden="1">
       <c r="A163" s="4" t="s">
         <v>289</v>
       </c>
@@ -3539,7 +3609,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" hidden="1">
       <c r="A164" t="s">
         <v>291</v>
       </c>
@@ -3547,7 +3617,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" hidden="1">
       <c r="A165" t="s">
         <v>293</v>
       </c>
@@ -3555,7 +3625,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" hidden="1">
       <c r="A166" t="s">
         <v>294</v>
       </c>
@@ -3563,7 +3633,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" hidden="1">
       <c r="A167" t="s">
         <v>296</v>
       </c>
@@ -3571,7 +3641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" hidden="1">
       <c r="A168" t="s">
         <v>297</v>
       </c>
@@ -3579,7 +3649,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" hidden="1">
       <c r="A169" t="s">
         <v>298</v>
       </c>
@@ -3587,7 +3657,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" hidden="1">
       <c r="A170" t="s">
         <v>300</v>
       </c>
@@ -3595,7 +3665,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" hidden="1">
       <c r="A171" t="s">
         <v>302</v>
       </c>
@@ -3603,7 +3673,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" hidden="1">
       <c r="A172" t="s">
         <v>304</v>
       </c>
@@ -3611,7 +3681,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" hidden="1">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -3619,7 +3689,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" hidden="1">
       <c r="A174" t="s">
         <v>307</v>
       </c>
@@ -3627,7 +3697,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" hidden="1">
       <c r="A175" t="s">
         <v>309</v>
       </c>
@@ -3635,7 +3705,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" hidden="1">
       <c r="A176" t="s">
         <v>311</v>
       </c>
@@ -3643,7 +3713,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" hidden="1">
       <c r="A177" t="s">
         <v>313</v>
       </c>
@@ -3651,7 +3721,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" hidden="1">
       <c r="A178" t="s">
         <v>315</v>
       </c>
@@ -3659,7 +3729,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" hidden="1">
       <c r="A179" t="s">
         <v>316</v>
       </c>
@@ -3667,7 +3737,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" hidden="1">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -3680,7 +3750,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" hidden="1">
       <c r="A182" t="s">
         <v>321</v>
       </c>
@@ -3688,7 +3758,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" hidden="1">
       <c r="A183" t="s">
         <v>323</v>
       </c>
@@ -3696,7 +3766,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" hidden="1">
       <c r="A184" t="s">
         <v>325</v>
       </c>
@@ -3704,7 +3774,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" hidden="1">
       <c r="A185" t="s">
         <v>327</v>
       </c>
@@ -3712,7 +3782,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" hidden="1">
       <c r="A186" t="s">
         <v>329</v>
       </c>
@@ -3720,7 +3790,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" hidden="1">
       <c r="A187" t="s">
         <v>330</v>
       </c>
@@ -3728,7 +3798,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" hidden="1">
       <c r="A188" t="s">
         <v>331</v>
       </c>
@@ -3736,7 +3806,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" hidden="1">
       <c r="A189" t="s">
         <v>333</v>
       </c>
@@ -3744,7 +3814,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" hidden="1">
       <c r="A190" t="s">
         <v>335</v>
       </c>
@@ -3756,8 +3826,11 @@
       <c r="A191" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="192" spans="1:2">
+      <c r="B191" s="10" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" hidden="1">
       <c r="A192" t="s">
         <v>338</v>
       </c>
@@ -3765,7 +3838,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" hidden="1">
       <c r="A193" t="s">
         <v>339</v>
       </c>
@@ -3773,7 +3846,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" hidden="1">
       <c r="A194" t="s">
         <v>341</v>
       </c>
@@ -3781,7 +3854,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" hidden="1">
       <c r="A195" t="s">
         <v>343</v>
       </c>
@@ -3789,7 +3862,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" hidden="1">
       <c r="A196" t="s">
         <v>345</v>
       </c>
@@ -3797,7 +3870,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" hidden="1">
       <c r="A197" t="s">
         <v>347</v>
       </c>
@@ -3805,7 +3878,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5">
+    <row r="198" spans="1:2" ht="16.5" hidden="1">
       <c r="A198" t="s">
         <v>349</v>
       </c>
@@ -3813,7 +3886,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" hidden="1">
       <c r="A199" t="s">
         <v>351</v>
       </c>
@@ -3821,7 +3894,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" hidden="1">
       <c r="A200" t="s">
         <v>353</v>
       </c>
@@ -3829,7 +3902,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" hidden="1">
       <c r="A201" t="s">
         <v>355</v>
       </c>
@@ -3837,7 +3910,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" hidden="1">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -3845,7 +3918,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" hidden="1">
       <c r="A203" t="s">
         <v>359</v>
       </c>
@@ -3853,7 +3926,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" hidden="1">
       <c r="A204" t="s">
         <v>361</v>
       </c>
@@ -3861,7 +3934,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" hidden="1">
       <c r="A205" t="s">
         <v>363</v>
       </c>
@@ -3869,7 +3942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" hidden="1">
       <c r="A206" t="s">
         <v>364</v>
       </c>
@@ -3877,7 +3950,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" hidden="1">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -3885,7 +3958,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" hidden="1">
       <c r="A208" t="s">
         <v>559</v>
       </c>
@@ -3893,7 +3966,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" hidden="1">
       <c r="A209" t="s">
         <v>368</v>
       </c>
@@ -3901,7 +3974,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" hidden="1">
       <c r="A210" t="s">
         <v>370</v>
       </c>
@@ -3909,7 +3982,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" hidden="1">
       <c r="A211" t="s">
         <v>372</v>
       </c>
@@ -3917,7 +3990,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" hidden="1">
       <c r="A212" t="s">
         <v>374</v>
       </c>
@@ -3925,7 +3998,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" hidden="1">
       <c r="A213" t="s">
         <v>376</v>
       </c>
@@ -3933,7 +4006,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" hidden="1">
       <c r="A214" t="s">
         <v>378</v>
       </c>
@@ -3941,7 +4014,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" hidden="1">
       <c r="A215" t="s">
         <v>380</v>
       </c>
@@ -3949,7 +4022,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" hidden="1">
       <c r="A216" t="s">
         <v>381</v>
       </c>
@@ -3957,7 +4030,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" hidden="1">
       <c r="A217" t="s">
         <v>383</v>
       </c>
@@ -3965,7 +4038,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" hidden="1">
       <c r="A218" t="s">
         <v>385</v>
       </c>
@@ -3973,7 +4046,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" hidden="1">
       <c r="A219" t="s">
         <v>387</v>
       </c>
@@ -3985,8 +4058,11 @@
       <c r="A220" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="221" spans="1:2">
+      <c r="B220" s="10" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" hidden="1">
       <c r="A221" t="s">
         <v>389</v>
       </c>
@@ -3994,7 +4070,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" hidden="1">
       <c r="A222" t="s">
         <v>391</v>
       </c>
@@ -4002,7 +4078,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" hidden="1">
       <c r="A223" t="s">
         <v>393</v>
       </c>
@@ -4010,7 +4086,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" hidden="1">
       <c r="A224" t="s">
         <v>395</v>
       </c>
@@ -4018,7 +4094,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" hidden="1">
       <c r="A225" t="s">
         <v>397</v>
       </c>
@@ -4026,7 +4102,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" hidden="1">
       <c r="A226" t="s">
         <v>399</v>
       </c>
@@ -4034,7 +4110,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" hidden="1">
       <c r="A227" t="s">
         <v>401</v>
       </c>
@@ -4042,7 +4118,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" hidden="1">
       <c r="A228" t="s">
         <v>403</v>
       </c>
@@ -4050,7 +4126,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" hidden="1">
       <c r="A229" t="s">
         <v>405</v>
       </c>
@@ -4058,7 +4134,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" hidden="1">
       <c r="A230" t="s">
         <v>407</v>
       </c>
@@ -4066,7 +4142,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" hidden="1">
       <c r="A231" t="s">
         <v>409</v>
       </c>
@@ -4074,7 +4150,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" hidden="1">
       <c r="A232" t="s">
         <v>410</v>
       </c>
@@ -4082,7 +4158,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" hidden="1">
       <c r="A233" t="s">
         <v>412</v>
       </c>
@@ -4090,7 +4166,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" hidden="1">
       <c r="A234" t="s">
         <v>413</v>
       </c>
@@ -4098,7 +4174,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" hidden="1">
       <c r="A235" t="s">
         <v>415</v>
       </c>
@@ -4106,7 +4182,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" hidden="1">
       <c r="A236" t="s">
         <v>417</v>
       </c>
@@ -4114,7 +4190,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" hidden="1">
       <c r="A237" t="s">
         <v>419</v>
       </c>
@@ -4122,7 +4198,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" hidden="1">
       <c r="A238" t="s">
         <v>421</v>
       </c>
@@ -4130,7 +4206,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" hidden="1">
       <c r="A239" t="s">
         <v>423</v>
       </c>
@@ -4138,7 +4214,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" hidden="1">
       <c r="A240" t="s">
         <v>425</v>
       </c>
@@ -4146,7 +4222,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" hidden="1">
       <c r="A241" t="s">
         <v>426</v>
       </c>
@@ -4154,7 +4230,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" hidden="1">
       <c r="A242" t="s">
         <v>428</v>
       </c>
@@ -4167,7 +4243,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" hidden="1">
       <c r="A244" t="s">
         <v>431</v>
       </c>
@@ -4175,7 +4251,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" hidden="1">
       <c r="A245" t="s">
         <v>433</v>
       </c>
@@ -4183,7 +4259,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" hidden="1">
       <c r="A246" t="s">
         <v>435</v>
       </c>
@@ -4191,7 +4267,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" hidden="1">
       <c r="A247" t="s">
         <v>437</v>
       </c>
@@ -4204,7 +4280,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" hidden="1">
       <c r="A249" t="s">
         <v>439</v>
       </c>
@@ -4212,7 +4288,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" hidden="1">
       <c r="A250" t="s">
         <v>441</v>
       </c>
@@ -4220,7 +4296,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" hidden="1">
       <c r="A251" t="s">
         <v>443</v>
       </c>
@@ -4233,7 +4309,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" hidden="1">
       <c r="A253" t="s">
         <v>446</v>
       </c>
@@ -4245,13 +4321,19 @@
       <c r="A254" t="s">
         <v>448</v>
       </c>
+      <c r="B254" s="10" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="256" spans="1:2">
+      <c r="B255" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" hidden="1">
       <c r="A256" t="s">
         <v>450</v>
       </c>
@@ -4259,7 +4341,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" hidden="1">
       <c r="A257" t="s">
         <v>451</v>
       </c>
@@ -4267,7 +4349,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" hidden="1">
       <c r="A258" t="s">
         <v>452</v>
       </c>
@@ -4275,7 +4357,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" hidden="1">
       <c r="A259" t="s">
         <v>453</v>
       </c>
@@ -4283,7 +4365,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" hidden="1">
       <c r="A260" t="s">
         <v>454</v>
       </c>
@@ -4291,7 +4373,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" hidden="1">
       <c r="A261" t="s">
         <v>456</v>
       </c>
@@ -4299,7 +4381,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" hidden="1">
       <c r="A262" t="s">
         <v>458</v>
       </c>
@@ -4307,7 +4389,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" hidden="1">
       <c r="A263" t="s">
         <v>460</v>
       </c>
@@ -4315,7 +4397,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" hidden="1">
       <c r="A264" t="s">
         <v>461</v>
       </c>
@@ -4323,7 +4405,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" hidden="1">
       <c r="A265" t="s">
         <v>463</v>
       </c>
@@ -4331,7 +4413,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" hidden="1">
       <c r="A266" t="s">
         <v>465</v>
       </c>
@@ -4339,7 +4421,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" hidden="1">
       <c r="A267" t="s">
         <v>467</v>
       </c>
@@ -4347,7 +4429,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" hidden="1">
       <c r="A268" t="s">
         <v>468</v>
       </c>
@@ -4355,7 +4437,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" hidden="1">
       <c r="A269" t="s">
         <v>469</v>
       </c>
@@ -4377,13 +4459,16 @@
       <c r="A272" t="s">
         <v>473</v>
       </c>
+      <c r="B272" s="10" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" hidden="1">
       <c r="A274" t="s">
         <v>475</v>
       </c>
@@ -4391,7 +4476,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" hidden="1">
       <c r="A275" t="s">
         <v>477</v>
       </c>
@@ -4404,7 +4489,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" hidden="1">
       <c r="A277" t="s">
         <v>479</v>
       </c>
@@ -4412,7 +4497,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" hidden="1">
       <c r="A278" t="s">
         <v>481</v>
       </c>
@@ -4420,7 +4505,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" hidden="1">
       <c r="A279" t="s">
         <v>483</v>
       </c>
@@ -4428,7 +4513,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" hidden="1">
       <c r="A280" t="s">
         <v>484</v>
       </c>
@@ -4436,7 +4521,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" hidden="1">
       <c r="A281" t="s">
         <v>485</v>
       </c>
@@ -4444,7 +4529,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" hidden="1">
       <c r="A282" t="s">
         <v>487</v>
       </c>
@@ -4452,7 +4537,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" hidden="1">
       <c r="A283" t="s">
         <v>488</v>
       </c>
@@ -4460,7 +4545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" hidden="1">
       <c r="A284" t="s">
         <v>489</v>
       </c>
@@ -4468,7 +4553,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" hidden="1">
       <c r="A285" t="s">
         <v>490</v>
       </c>
@@ -4476,7 +4561,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" hidden="1">
       <c r="A286" t="s">
         <v>491</v>
       </c>
@@ -4484,7 +4569,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" hidden="1">
       <c r="A287" t="s">
         <v>492</v>
       </c>
@@ -4492,7 +4577,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" hidden="1">
       <c r="A288" t="s">
         <v>493</v>
       </c>
@@ -4500,7 +4585,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" hidden="1">
       <c r="A289" t="s">
         <v>494</v>
       </c>
@@ -4508,7 +4593,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" hidden="1">
       <c r="A290" t="s">
         <v>496</v>
       </c>
@@ -4516,7 +4601,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" hidden="1">
       <c r="A291" t="s">
         <v>498</v>
       </c>
@@ -4524,7 +4609,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" hidden="1">
       <c r="A292" t="s">
         <v>499</v>
       </c>
@@ -4532,7 +4617,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" hidden="1">
       <c r="A293" t="s">
         <v>500</v>
       </c>
@@ -4540,7 +4625,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" hidden="1">
       <c r="A294" t="s">
         <v>501</v>
       </c>
@@ -4548,7 +4633,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" hidden="1">
       <c r="A295" t="s">
         <v>502</v>
       </c>
@@ -4556,7 +4641,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" hidden="1">
       <c r="A296" t="s">
         <v>503</v>
       </c>
@@ -4564,7 +4649,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" hidden="1">
       <c r="A297" t="s">
         <v>504</v>
       </c>
@@ -4572,7 +4657,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" hidden="1">
       <c r="A298" t="s">
         <v>505</v>
       </c>
@@ -4580,7 +4665,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" hidden="1">
       <c r="A299" t="s">
         <v>506</v>
       </c>
@@ -4588,7 +4673,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" hidden="1">
       <c r="A300" t="s">
         <v>507</v>
       </c>
@@ -4596,7 +4681,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" hidden="1">
       <c r="A301" t="s">
         <v>509</v>
       </c>
@@ -4604,7 +4689,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" hidden="1">
       <c r="A302" t="s">
         <v>510</v>
       </c>
@@ -4617,7 +4702,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" hidden="1">
       <c r="A304" t="s">
         <v>512</v>
       </c>
@@ -4625,7 +4710,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:5" hidden="1">
       <c r="A305" t="s">
         <v>513</v>
       </c>
@@ -4633,7 +4718,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="306" spans="1:5">
+    <row r="306" spans="1:5" hidden="1">
       <c r="A306" t="s">
         <v>514</v>
       </c>
@@ -4644,7 +4729,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="307" spans="1:5">
+    <row r="307" spans="1:5" hidden="1">
       <c r="A307" t="s">
         <v>515</v>
       </c>
@@ -4652,7 +4737,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:5" hidden="1">
       <c r="A308" t="s">
         <v>516</v>
       </c>
@@ -4660,7 +4745,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:5">
+    <row r="309" spans="1:5" hidden="1">
       <c r="A309" t="s">
         <v>517</v>
       </c>
@@ -4668,7 +4753,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="310" spans="1:5">
+    <row r="310" spans="1:5" hidden="1">
       <c r="A310" t="s">
         <v>518</v>
       </c>
@@ -4676,7 +4761,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="311" spans="1:5">
+    <row r="311" spans="1:5" hidden="1">
       <c r="A311" t="s">
         <v>520</v>
       </c>
@@ -4684,7 +4769,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="312" spans="1:5">
+    <row r="312" spans="1:5" hidden="1">
       <c r="A312" t="s">
         <v>521</v>
       </c>
@@ -4692,7 +4777,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="313" spans="1:5">
+    <row r="313" spans="1:5" hidden="1">
       <c r="A313" t="s">
         <v>522</v>
       </c>
@@ -4700,7 +4785,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="314" spans="1:5">
+    <row r="314" spans="1:5" hidden="1">
       <c r="A314" t="s">
         <v>523</v>
       </c>
@@ -4708,7 +4793,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="315" spans="1:5">
+    <row r="315" spans="1:5" hidden="1">
       <c r="A315" t="s">
         <v>524</v>
       </c>
@@ -4716,7 +4801,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="316" spans="1:5">
+    <row r="316" spans="1:5" hidden="1">
       <c r="A316" t="s">
         <v>525</v>
       </c>
@@ -4724,7 +4809,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="317" spans="1:5">
+    <row r="317" spans="1:5" hidden="1">
       <c r="A317" t="s">
         <v>526</v>
       </c>
@@ -4732,7 +4817,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="318" spans="1:5">
+    <row r="318" spans="1:5" hidden="1">
       <c r="A318" t="s">
         <v>527</v>
       </c>
@@ -4740,7 +4825,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="319" spans="1:5">
+    <row r="319" spans="1:5" hidden="1">
       <c r="A319" t="s">
         <v>529</v>
       </c>
@@ -4753,7 +4838,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" hidden="1">
       <c r="A321" t="s">
         <v>531</v>
       </c>
@@ -4761,7 +4846,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" hidden="1">
       <c r="A322" t="s">
         <v>532</v>
       </c>
@@ -4769,7 +4854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" hidden="1">
       <c r="A323" t="s">
         <v>533</v>
       </c>
@@ -4777,7 +4862,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" hidden="1">
       <c r="A324" t="s">
         <v>535</v>
       </c>
@@ -4785,7 +4870,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" hidden="1">
       <c r="A325" t="s">
         <v>536</v>
       </c>
@@ -4793,7 +4878,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" hidden="1">
       <c r="A326" t="s">
         <v>537</v>
       </c>
@@ -4806,7 +4891,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" hidden="1">
       <c r="A328" t="s">
         <v>538</v>
       </c>
@@ -4814,7 +4899,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" hidden="1">
       <c r="A329" t="s">
         <v>539</v>
       </c>
@@ -4822,7 +4907,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" hidden="1">
       <c r="A330" s="4" t="s">
         <v>540</v>
       </c>
@@ -4830,7 +4915,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" hidden="1">
       <c r="A331" s="4" t="s">
         <v>542</v>
       </c>
@@ -4838,7 +4923,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" hidden="1">
       <c r="A332" s="4" t="s">
         <v>543</v>
       </c>
@@ -4846,7 +4931,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" hidden="1">
       <c r="A333" t="s">
         <v>544</v>
       </c>
@@ -4854,7 +4939,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" hidden="1">
       <c r="A334" t="s">
         <v>545</v>
       </c>
@@ -4866,8 +4951,11 @@
       <c r="A335" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="336" spans="1:2">
+      <c r="B335" s="10" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" hidden="1">
       <c r="A336" t="s">
         <v>547</v>
       </c>
@@ -4875,7 +4963,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1">
       <c r="A337" t="s">
         <v>549</v>
       </c>
@@ -4883,7 +4971,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" hidden="1">
       <c r="A338" t="s">
         <v>551</v>
       </c>
@@ -4891,7 +4979,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" t="s">
         <v>553</v>
       </c>
@@ -4899,7 +4987,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" t="s">
         <v>555</v>
       </c>
@@ -4907,7 +4995,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" t="s">
         <v>557</v>
       </c>
@@ -4915,7 +5003,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" t="s">
         <v>581</v>
       </c>
@@ -4923,7 +5011,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" t="s">
         <v>576</v>
       </c>
@@ -4931,7 +5019,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" t="s">
         <v>580</v>
       </c>
@@ -4939,7 +5027,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" t="s">
         <v>577</v>
       </c>
@@ -4947,7 +5035,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1">
       <c r="A346" t="s">
         <v>578</v>
       </c>
@@ -4955,7 +5043,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1">
       <c r="A347" t="s">
         <v>579</v>
       </c>
@@ -4963,7 +5051,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1">
       <c r="A348" t="s">
         <v>582</v>
       </c>
@@ -4971,7 +5059,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1">
       <c r="A349" t="s">
         <v>583</v>
       </c>
@@ -4979,7 +5067,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="17.25">
+    <row r="350" spans="1:7" ht="17.25" hidden="1">
       <c r="A350" t="s">
         <v>584</v>
       </c>
@@ -4991,7 +5079,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1">
       <c r="A351" t="s">
         <v>585</v>
       </c>
@@ -5016,12 +5104,14 @@
       <c r="A353" t="s">
         <v>587</v>
       </c>
-      <c r="B353" s="7"/>
+      <c r="B353" s="10" t="s">
+        <v>609</v>
+      </c>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:7" hidden="1">
       <c r="A354" t="s">
         <v>588</v>
       </c>
@@ -5032,7 +5122,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:7" hidden="1">
       <c r="A355" t="s">
         <v>589</v>
       </c>
@@ -5043,7 +5133,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5">
+    <row r="356" spans="1:7" ht="19.5" hidden="1">
       <c r="A356" t="s">
         <v>590</v>
       </c>
@@ -5055,7 +5145,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1">
       <c r="A357" t="s">
         <v>591</v>
       </c>
@@ -5067,7 +5157,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1">
       <c r="A358" t="s">
         <v>592</v>
       </c>
@@ -5078,7 +5168,7 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1">
       <c r="A359" t="s">
         <v>593</v>
       </c>
@@ -5151,7 +5241,11 @@
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362"/>
+  <autoFilter ref="A1:H362">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5361,18 +5455,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5395,18 +5489,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "added gitignore + einige NachzüglerInnen"
This reverts commit f75d3b6ef507e2e31328f02aa2dbc2ff2a543459.
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="599">
   <si>
     <t>Themen</t>
   </si>
@@ -1819,49 +1819,13 @@
   </si>
   <si>
     <t>domirow-fau</t>
-  </si>
-  <si>
-    <t>Adaye1e</t>
-  </si>
-  <si>
-    <t>enesmvlt</t>
-  </si>
-  <si>
-    <t>tkessler94</t>
-  </si>
-  <si>
-    <t>AmrouHasan</t>
-  </si>
-  <si>
-    <t>juliwebair</t>
-  </si>
-  <si>
-    <t>Irishcoffee09</t>
-  </si>
-  <si>
-    <t>bilgesb</t>
-  </si>
-  <si>
-    <t>TobiasZuerrlein</t>
-  </si>
-  <si>
-    <t>lukasheinrich9</t>
-  </si>
-  <si>
-    <t>fe94fiqy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SaskiaHe </t>
-  </si>
-  <si>
-    <t>EuleW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1912,15 +1876,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1931,12 +1888,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1967,7 +1918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1982,8 +1933,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2286,11 +2235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2318,7 +2266,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2326,7 +2274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2334,7 +2282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2343,7 +2291,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2351,7 +2299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2359,7 +2307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2367,7 +2315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2375,7 +2323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2383,7 +2331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2391,7 +2339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2399,7 +2347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2407,7 +2355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2415,7 +2363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2423,7 +2371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2431,7 +2379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2439,7 +2387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2447,7 +2395,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2455,7 +2403,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2463,7 +2411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2471,7 +2419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2479,7 +2427,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2487,7 +2435,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2495,7 +2443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2503,7 +2451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2511,7 +2459,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2519,7 +2467,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2527,7 +2475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2544,11 +2492,8 @@
       <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" hidden="1">
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2556,7 +2501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2564,7 +2509,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2572,7 +2517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2580,7 +2525,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2588,7 +2533,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2596,7 +2541,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2609,7 +2554,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2617,7 +2562,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2625,7 +2570,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2633,7 +2578,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2641,7 +2586,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2650,7 +2595,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2659,7 +2604,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2667,7 +2612,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2679,11 +2624,8 @@
       <c r="A47" t="s">
         <v>89</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" hidden="1">
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -2691,7 +2633,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -2699,7 +2641,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -2707,7 +2649,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2715,7 +2657,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2723,7 +2665,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2731,7 +2673,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2739,7 +2681,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2747,7 +2689,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2755,7 +2697,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2763,7 +2705,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2771,7 +2713,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2779,7 +2721,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2787,7 +2729,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -2795,7 +2737,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -2803,7 +2745,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -2811,7 +2753,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -2819,7 +2761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -2827,7 +2769,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>123</v>
       </c>
@@ -2835,7 +2777,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -2843,7 +2785,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" customHeight="1">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -2851,7 +2793,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -2859,7 +2801,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -2871,11 +2813,8 @@
       <c r="A71" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="10" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" hidden="1">
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -2883,7 +2822,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -2891,7 +2830,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -2899,7 +2838,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -2907,7 +2846,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -2915,7 +2854,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2923,7 +2862,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2931,7 +2870,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2939,7 +2878,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2947,7 +2886,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2955,7 +2894,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -2963,7 +2902,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -2971,7 +2910,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>155</v>
       </c>
@@ -2979,7 +2918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>156</v>
       </c>
@@ -2987,7 +2926,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -2995,7 +2934,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>160</v>
       </c>
@@ -3003,7 +2942,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>162</v>
       </c>
@@ -3011,7 +2950,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -3019,7 +2958,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>165</v>
       </c>
@@ -3027,7 +2966,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1">
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -3035,7 +2974,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -3043,7 +2982,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1">
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -3051,7 +2990,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1">
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -3059,7 +2998,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1">
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -3067,7 +3006,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1">
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3075,7 +3014,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -3083,7 +3022,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -3091,7 +3030,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>183</v>
       </c>
@@ -3099,7 +3038,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -3107,7 +3046,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -3115,7 +3054,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>189</v>
       </c>
@@ -3123,7 +3062,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>191</v>
       </c>
@@ -3131,7 +3070,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -3139,7 +3078,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>195</v>
       </c>
@@ -3147,7 +3086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -3156,7 +3095,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" hidden="1">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>197</v>
       </c>
@@ -3164,7 +3103,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>199</v>
       </c>
@@ -3172,7 +3111,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>201</v>
       </c>
@@ -3180,7 +3119,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>203</v>
       </c>
@@ -3188,7 +3127,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>205</v>
       </c>
@@ -3196,7 +3135,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>207</v>
       </c>
@@ -3204,7 +3143,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1">
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -3212,7 +3151,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1">
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -3220,7 +3159,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1">
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>213</v>
       </c>
@@ -3228,7 +3167,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1">
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>215</v>
       </c>
@@ -3236,7 +3175,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1">
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>217</v>
       </c>
@@ -3244,7 +3183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1">
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3252,7 +3191,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1">
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>219</v>
       </c>
@@ -3260,7 +3199,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1">
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -3268,7 +3207,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1">
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>223</v>
       </c>
@@ -3276,7 +3215,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1">
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -3284,7 +3223,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1">
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -3292,7 +3231,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1">
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -3300,7 +3239,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1">
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -3308,7 +3247,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1">
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -3316,7 +3255,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1">
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>235</v>
       </c>
@@ -3324,7 +3263,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1">
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>236</v>
       </c>
@@ -3337,7 +3276,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1">
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -3345,7 +3284,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1">
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -3353,7 +3292,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1">
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>242</v>
       </c>
@@ -3361,7 +3300,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1">
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -3369,7 +3308,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1">
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -3377,7 +3316,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1">
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>247</v>
       </c>
@@ -3385,7 +3324,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1">
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>249</v>
       </c>
@@ -3393,7 +3332,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1">
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>251</v>
       </c>
@@ -3401,7 +3340,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1">
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>253</v>
       </c>
@@ -3413,19 +3352,13 @@
       <c r="A139" t="s">
         <v>255</v>
       </c>
-      <c r="B139" s="10" t="s">
-        <v>601</v>
-      </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>256</v>
       </c>
-      <c r="B140" s="10" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" hidden="1">
+    </row>
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>257</v>
       </c>
@@ -3433,7 +3366,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1">
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -3441,7 +3374,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1">
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
         <v>260</v>
       </c>
@@ -3449,7 +3382,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1">
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
         <v>261</v>
       </c>
@@ -3457,7 +3390,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1">
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
         <v>263</v>
       </c>
@@ -3465,7 +3398,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1">
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
         <v>264</v>
       </c>
@@ -3473,7 +3406,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1">
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
         <v>265</v>
       </c>
@@ -3481,7 +3414,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1">
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
         <v>266</v>
       </c>
@@ -3489,7 +3422,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1">
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
         <v>268</v>
       </c>
@@ -3497,7 +3430,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1">
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>270</v>
       </c>
@@ -3505,7 +3438,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1">
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
         <v>272</v>
       </c>
@@ -3513,7 +3446,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1">
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
         <v>274</v>
       </c>
@@ -3521,7 +3454,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1">
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
         <v>275</v>
       </c>
@@ -3529,7 +3462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1">
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
         <v>276</v>
       </c>
@@ -3537,7 +3470,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1">
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
         <v>277</v>
       </c>
@@ -3545,7 +3478,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1">
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
         <v>278</v>
       </c>
@@ -3557,11 +3490,8 @@
       <c r="A157" t="s">
         <v>279</v>
       </c>
-      <c r="B157" s="10" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" hidden="1">
+    </row>
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
         <v>280</v>
       </c>
@@ -3569,7 +3499,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1">
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>282</v>
       </c>
@@ -3577,7 +3507,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1">
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
         <v>284</v>
       </c>
@@ -3585,7 +3515,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1">
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>286</v>
       </c>
@@ -3593,7 +3523,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1">
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>288</v>
       </c>
@@ -3601,7 +3531,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1">
+    <row r="163" spans="1:2">
       <c r="A163" s="4" t="s">
         <v>289</v>
       </c>
@@ -3609,7 +3539,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1">
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>291</v>
       </c>
@@ -3617,7 +3547,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1">
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>293</v>
       </c>
@@ -3625,7 +3555,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1">
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>294</v>
       </c>
@@ -3633,7 +3563,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1">
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
         <v>296</v>
       </c>
@@ -3641,7 +3571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1">
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
         <v>297</v>
       </c>
@@ -3649,7 +3579,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1">
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
         <v>298</v>
       </c>
@@ -3657,7 +3587,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1">
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>300</v>
       </c>
@@ -3665,7 +3595,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1">
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>302</v>
       </c>
@@ -3673,7 +3603,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1">
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>304</v>
       </c>
@@ -3681,7 +3611,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1">
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -3689,7 +3619,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1">
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>307</v>
       </c>
@@ -3697,7 +3627,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1">
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>309</v>
       </c>
@@ -3705,7 +3635,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1">
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>311</v>
       </c>
@@ -3713,7 +3643,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1">
+    <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>313</v>
       </c>
@@ -3721,7 +3651,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1">
+    <row r="178" spans="1:2">
       <c r="A178" t="s">
         <v>315</v>
       </c>
@@ -3729,7 +3659,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1">
+    <row r="179" spans="1:2">
       <c r="A179" t="s">
         <v>316</v>
       </c>
@@ -3737,7 +3667,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1">
+    <row r="180" spans="1:2">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -3750,7 +3680,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1">
+    <row r="182" spans="1:2">
       <c r="A182" t="s">
         <v>321</v>
       </c>
@@ -3758,7 +3688,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1">
+    <row r="183" spans="1:2">
       <c r="A183" t="s">
         <v>323</v>
       </c>
@@ -3766,7 +3696,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1">
+    <row r="184" spans="1:2">
       <c r="A184" t="s">
         <v>325</v>
       </c>
@@ -3774,7 +3704,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1">
+    <row r="185" spans="1:2">
       <c r="A185" t="s">
         <v>327</v>
       </c>
@@ -3782,7 +3712,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1">
+    <row r="186" spans="1:2">
       <c r="A186" t="s">
         <v>329</v>
       </c>
@@ -3790,7 +3720,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1">
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>330</v>
       </c>
@@ -3798,7 +3728,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1">
+    <row r="188" spans="1:2">
       <c r="A188" t="s">
         <v>331</v>
       </c>
@@ -3806,7 +3736,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1">
+    <row r="189" spans="1:2">
       <c r="A189" t="s">
         <v>333</v>
       </c>
@@ -3814,7 +3744,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1">
+    <row r="190" spans="1:2">
       <c r="A190" t="s">
         <v>335</v>
       </c>
@@ -3826,11 +3756,8 @@
       <c r="A191" t="s">
         <v>337</v>
       </c>
-      <c r="B191" s="10" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" hidden="1">
+    </row>
+    <row r="192" spans="1:2">
       <c r="A192" t="s">
         <v>338</v>
       </c>
@@ -3838,7 +3765,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1">
+    <row r="193" spans="1:2">
       <c r="A193" t="s">
         <v>339</v>
       </c>
@@ -3846,7 +3773,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1">
+    <row r="194" spans="1:2">
       <c r="A194" t="s">
         <v>341</v>
       </c>
@@ -3854,7 +3781,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1">
+    <row r="195" spans="1:2">
       <c r="A195" t="s">
         <v>343</v>
       </c>
@@ -3862,7 +3789,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1">
+    <row r="196" spans="1:2">
       <c r="A196" t="s">
         <v>345</v>
       </c>
@@ -3870,7 +3797,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1">
+    <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>347</v>
       </c>
@@ -3878,7 +3805,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5" hidden="1">
+    <row r="198" spans="1:2" ht="16.5">
       <c r="A198" t="s">
         <v>349</v>
       </c>
@@ -3886,7 +3813,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1">
+    <row r="199" spans="1:2">
       <c r="A199" t="s">
         <v>351</v>
       </c>
@@ -3894,7 +3821,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1">
+    <row r="200" spans="1:2">
       <c r="A200" t="s">
         <v>353</v>
       </c>
@@ -3902,7 +3829,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1">
+    <row r="201" spans="1:2">
       <c r="A201" t="s">
         <v>355</v>
       </c>
@@ -3910,7 +3837,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1">
+    <row r="202" spans="1:2">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -3918,7 +3845,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1">
+    <row r="203" spans="1:2">
       <c r="A203" t="s">
         <v>359</v>
       </c>
@@ -3926,7 +3853,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1">
+    <row r="204" spans="1:2">
       <c r="A204" t="s">
         <v>361</v>
       </c>
@@ -3934,7 +3861,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1">
+    <row r="205" spans="1:2">
       <c r="A205" t="s">
         <v>363</v>
       </c>
@@ -3942,7 +3869,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1">
+    <row r="206" spans="1:2">
       <c r="A206" t="s">
         <v>364</v>
       </c>
@@ -3950,7 +3877,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1">
+    <row r="207" spans="1:2">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -3958,7 +3885,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1">
+    <row r="208" spans="1:2">
       <c r="A208" t="s">
         <v>559</v>
       </c>
@@ -3966,7 +3893,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1">
+    <row r="209" spans="1:2">
       <c r="A209" t="s">
         <v>368</v>
       </c>
@@ -3974,7 +3901,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1">
+    <row r="210" spans="1:2">
       <c r="A210" t="s">
         <v>370</v>
       </c>
@@ -3982,7 +3909,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1">
+    <row r="211" spans="1:2">
       <c r="A211" t="s">
         <v>372</v>
       </c>
@@ -3990,7 +3917,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1">
+    <row r="212" spans="1:2">
       <c r="A212" t="s">
         <v>374</v>
       </c>
@@ -3998,7 +3925,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1">
+    <row r="213" spans="1:2">
       <c r="A213" t="s">
         <v>376</v>
       </c>
@@ -4006,7 +3933,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1">
+    <row r="214" spans="1:2">
       <c r="A214" t="s">
         <v>378</v>
       </c>
@@ -4014,7 +3941,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1">
+    <row r="215" spans="1:2">
       <c r="A215" t="s">
         <v>380</v>
       </c>
@@ -4022,7 +3949,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1">
+    <row r="216" spans="1:2">
       <c r="A216" t="s">
         <v>381</v>
       </c>
@@ -4030,7 +3957,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1">
+    <row r="217" spans="1:2">
       <c r="A217" t="s">
         <v>383</v>
       </c>
@@ -4038,7 +3965,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1">
+    <row r="218" spans="1:2">
       <c r="A218" t="s">
         <v>385</v>
       </c>
@@ -4046,7 +3973,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1">
+    <row r="219" spans="1:2">
       <c r="A219" t="s">
         <v>387</v>
       </c>
@@ -4058,11 +3985,8 @@
       <c r="A220" t="s">
         <v>388</v>
       </c>
-      <c r="B220" s="10" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" hidden="1">
+    </row>
+    <row r="221" spans="1:2">
       <c r="A221" t="s">
         <v>389</v>
       </c>
@@ -4070,7 +3994,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1">
+    <row r="222" spans="1:2">
       <c r="A222" t="s">
         <v>391</v>
       </c>
@@ -4078,7 +4002,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1">
+    <row r="223" spans="1:2">
       <c r="A223" t="s">
         <v>393</v>
       </c>
@@ -4086,7 +4010,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1">
+    <row r="224" spans="1:2">
       <c r="A224" t="s">
         <v>395</v>
       </c>
@@ -4094,7 +4018,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1">
+    <row r="225" spans="1:2">
       <c r="A225" t="s">
         <v>397</v>
       </c>
@@ -4102,7 +4026,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1">
+    <row r="226" spans="1:2">
       <c r="A226" t="s">
         <v>399</v>
       </c>
@@ -4110,7 +4034,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1">
+    <row r="227" spans="1:2">
       <c r="A227" t="s">
         <v>401</v>
       </c>
@@ -4118,7 +4042,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1">
+    <row r="228" spans="1:2">
       <c r="A228" t="s">
         <v>403</v>
       </c>
@@ -4126,7 +4050,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1">
+    <row r="229" spans="1:2">
       <c r="A229" t="s">
         <v>405</v>
       </c>
@@ -4134,7 +4058,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1">
+    <row r="230" spans="1:2">
       <c r="A230" t="s">
         <v>407</v>
       </c>
@@ -4142,7 +4066,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1">
+    <row r="231" spans="1:2">
       <c r="A231" t="s">
         <v>409</v>
       </c>
@@ -4150,7 +4074,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1">
+    <row r="232" spans="1:2">
       <c r="A232" t="s">
         <v>410</v>
       </c>
@@ -4158,7 +4082,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1">
+    <row r="233" spans="1:2">
       <c r="A233" t="s">
         <v>412</v>
       </c>
@@ -4166,7 +4090,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1">
+    <row r="234" spans="1:2">
       <c r="A234" t="s">
         <v>413</v>
       </c>
@@ -4174,7 +4098,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1">
+    <row r="235" spans="1:2">
       <c r="A235" t="s">
         <v>415</v>
       </c>
@@ -4182,7 +4106,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1">
+    <row r="236" spans="1:2">
       <c r="A236" t="s">
         <v>417</v>
       </c>
@@ -4190,7 +4114,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1">
+    <row r="237" spans="1:2">
       <c r="A237" t="s">
         <v>419</v>
       </c>
@@ -4198,7 +4122,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1">
+    <row r="238" spans="1:2">
       <c r="A238" t="s">
         <v>421</v>
       </c>
@@ -4206,7 +4130,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1">
+    <row r="239" spans="1:2">
       <c r="A239" t="s">
         <v>423</v>
       </c>
@@ -4214,7 +4138,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1">
+    <row r="240" spans="1:2">
       <c r="A240" t="s">
         <v>425</v>
       </c>
@@ -4222,7 +4146,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1">
+    <row r="241" spans="1:2">
       <c r="A241" t="s">
         <v>426</v>
       </c>
@@ -4230,7 +4154,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1">
+    <row r="242" spans="1:2">
       <c r="A242" t="s">
         <v>428</v>
       </c>
@@ -4243,7 +4167,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1">
+    <row r="244" spans="1:2">
       <c r="A244" t="s">
         <v>431</v>
       </c>
@@ -4251,7 +4175,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1">
+    <row r="245" spans="1:2">
       <c r="A245" t="s">
         <v>433</v>
       </c>
@@ -4259,7 +4183,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1">
+    <row r="246" spans="1:2">
       <c r="A246" t="s">
         <v>435</v>
       </c>
@@ -4267,7 +4191,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1">
+    <row r="247" spans="1:2">
       <c r="A247" t="s">
         <v>437</v>
       </c>
@@ -4280,7 +4204,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1">
+    <row r="249" spans="1:2">
       <c r="A249" t="s">
         <v>439</v>
       </c>
@@ -4288,7 +4212,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1">
+    <row r="250" spans="1:2">
       <c r="A250" t="s">
         <v>441</v>
       </c>
@@ -4296,7 +4220,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1">
+    <row r="251" spans="1:2">
       <c r="A251" t="s">
         <v>443</v>
       </c>
@@ -4309,7 +4233,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1">
+    <row r="253" spans="1:2">
       <c r="A253" t="s">
         <v>446</v>
       </c>
@@ -4321,19 +4245,13 @@
       <c r="A254" t="s">
         <v>448</v>
       </c>
-      <c r="B254" s="10" t="s">
-        <v>605</v>
-      </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
         <v>449</v>
       </c>
-      <c r="B255" s="11" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" hidden="1">
+    </row>
+    <row r="256" spans="1:2">
       <c r="A256" t="s">
         <v>450</v>
       </c>
@@ -4341,7 +4259,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1">
+    <row r="257" spans="1:2">
       <c r="A257" t="s">
         <v>451</v>
       </c>
@@ -4349,7 +4267,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1">
+    <row r="258" spans="1:2">
       <c r="A258" t="s">
         <v>452</v>
       </c>
@@ -4357,7 +4275,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1">
+    <row r="259" spans="1:2">
       <c r="A259" t="s">
         <v>453</v>
       </c>
@@ -4365,7 +4283,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1">
+    <row r="260" spans="1:2">
       <c r="A260" t="s">
         <v>454</v>
       </c>
@@ -4373,7 +4291,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1">
+    <row r="261" spans="1:2">
       <c r="A261" t="s">
         <v>456</v>
       </c>
@@ -4381,7 +4299,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1">
+    <row r="262" spans="1:2">
       <c r="A262" t="s">
         <v>458</v>
       </c>
@@ -4389,7 +4307,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1">
+    <row r="263" spans="1:2">
       <c r="A263" t="s">
         <v>460</v>
       </c>
@@ -4397,7 +4315,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1">
+    <row r="264" spans="1:2">
       <c r="A264" t="s">
         <v>461</v>
       </c>
@@ -4405,7 +4323,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1">
+    <row r="265" spans="1:2">
       <c r="A265" t="s">
         <v>463</v>
       </c>
@@ -4413,7 +4331,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1">
+    <row r="266" spans="1:2">
       <c r="A266" t="s">
         <v>465</v>
       </c>
@@ -4421,7 +4339,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1">
+    <row r="267" spans="1:2">
       <c r="A267" t="s">
         <v>467</v>
       </c>
@@ -4429,7 +4347,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="268" spans="1:2" hidden="1">
+    <row r="268" spans="1:2">
       <c r="A268" t="s">
         <v>468</v>
       </c>
@@ -4437,7 +4355,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1">
+    <row r="269" spans="1:2">
       <c r="A269" t="s">
         <v>469</v>
       </c>
@@ -4459,16 +4377,13 @@
       <c r="A272" t="s">
         <v>473</v>
       </c>
-      <c r="B272" s="10" t="s">
-        <v>606</v>
-      </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1">
+    <row r="274" spans="1:2">
       <c r="A274" t="s">
         <v>475</v>
       </c>
@@ -4476,7 +4391,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1">
+    <row r="275" spans="1:2">
       <c r="A275" t="s">
         <v>477</v>
       </c>
@@ -4489,7 +4404,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1">
+    <row r="277" spans="1:2">
       <c r="A277" t="s">
         <v>479</v>
       </c>
@@ -4497,7 +4412,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1">
+    <row r="278" spans="1:2">
       <c r="A278" t="s">
         <v>481</v>
       </c>
@@ -4505,7 +4420,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1">
+    <row r="279" spans="1:2">
       <c r="A279" t="s">
         <v>483</v>
       </c>
@@ -4513,7 +4428,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1">
+    <row r="280" spans="1:2">
       <c r="A280" t="s">
         <v>484</v>
       </c>
@@ -4521,7 +4436,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1">
+    <row r="281" spans="1:2">
       <c r="A281" t="s">
         <v>485</v>
       </c>
@@ -4529,7 +4444,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1">
+    <row r="282" spans="1:2">
       <c r="A282" t="s">
         <v>487</v>
       </c>
@@ -4537,7 +4452,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1">
+    <row r="283" spans="1:2">
       <c r="A283" t="s">
         <v>488</v>
       </c>
@@ -4545,7 +4460,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1">
+    <row r="284" spans="1:2">
       <c r="A284" t="s">
         <v>489</v>
       </c>
@@ -4553,7 +4468,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1">
+    <row r="285" spans="1:2">
       <c r="A285" t="s">
         <v>490</v>
       </c>
@@ -4561,7 +4476,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1">
+    <row r="286" spans="1:2">
       <c r="A286" t="s">
         <v>491</v>
       </c>
@@ -4569,7 +4484,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1">
+    <row r="287" spans="1:2">
       <c r="A287" t="s">
         <v>492</v>
       </c>
@@ -4577,7 +4492,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1">
+    <row r="288" spans="1:2">
       <c r="A288" t="s">
         <v>493</v>
       </c>
@@ -4585,7 +4500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="289" spans="1:2" hidden="1">
+    <row r="289" spans="1:2">
       <c r="A289" t="s">
         <v>494</v>
       </c>
@@ -4593,7 +4508,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1">
+    <row r="290" spans="1:2">
       <c r="A290" t="s">
         <v>496</v>
       </c>
@@ -4601,7 +4516,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1">
+    <row r="291" spans="1:2">
       <c r="A291" t="s">
         <v>498</v>
       </c>
@@ -4609,7 +4524,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="292" spans="1:2" hidden="1">
+    <row r="292" spans="1:2">
       <c r="A292" t="s">
         <v>499</v>
       </c>
@@ -4617,7 +4532,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1">
+    <row r="293" spans="1:2">
       <c r="A293" t="s">
         <v>500</v>
       </c>
@@ -4625,7 +4540,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1">
+    <row r="294" spans="1:2">
       <c r="A294" t="s">
         <v>501</v>
       </c>
@@ -4633,7 +4548,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1">
+    <row r="295" spans="1:2">
       <c r="A295" t="s">
         <v>502</v>
       </c>
@@ -4641,7 +4556,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1">
+    <row r="296" spans="1:2">
       <c r="A296" t="s">
         <v>503</v>
       </c>
@@ -4649,7 +4564,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1">
+    <row r="297" spans="1:2">
       <c r="A297" t="s">
         <v>504</v>
       </c>
@@ -4657,7 +4572,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1">
+    <row r="298" spans="1:2">
       <c r="A298" t="s">
         <v>505</v>
       </c>
@@ -4665,7 +4580,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1">
+    <row r="299" spans="1:2">
       <c r="A299" t="s">
         <v>506</v>
       </c>
@@ -4673,7 +4588,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1">
+    <row r="300" spans="1:2">
       <c r="A300" t="s">
         <v>507</v>
       </c>
@@ -4681,7 +4596,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1">
+    <row r="301" spans="1:2">
       <c r="A301" t="s">
         <v>509</v>
       </c>
@@ -4689,7 +4604,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1">
+    <row r="302" spans="1:2">
       <c r="A302" t="s">
         <v>510</v>
       </c>
@@ -4702,7 +4617,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1">
+    <row r="304" spans="1:2">
       <c r="A304" t="s">
         <v>512</v>
       </c>
@@ -4710,7 +4625,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1">
+    <row r="305" spans="1:5">
       <c r="A305" t="s">
         <v>513</v>
       </c>
@@ -4718,7 +4633,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1">
+    <row r="306" spans="1:5">
       <c r="A306" t="s">
         <v>514</v>
       </c>
@@ -4729,7 +4644,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1">
+    <row r="307" spans="1:5">
       <c r="A307" t="s">
         <v>515</v>
       </c>
@@ -4737,7 +4652,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1">
+    <row r="308" spans="1:5">
       <c r="A308" t="s">
         <v>516</v>
       </c>
@@ -4745,7 +4660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1">
+    <row r="309" spans="1:5">
       <c r="A309" t="s">
         <v>517</v>
       </c>
@@ -4753,7 +4668,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1">
+    <row r="310" spans="1:5">
       <c r="A310" t="s">
         <v>518</v>
       </c>
@@ -4761,7 +4676,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1">
+    <row r="311" spans="1:5">
       <c r="A311" t="s">
         <v>520</v>
       </c>
@@ -4769,7 +4684,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1">
+    <row r="312" spans="1:5">
       <c r="A312" t="s">
         <v>521</v>
       </c>
@@ -4777,7 +4692,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1">
+    <row r="313" spans="1:5">
       <c r="A313" t="s">
         <v>522</v>
       </c>
@@ -4785,7 +4700,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1">
+    <row r="314" spans="1:5">
       <c r="A314" t="s">
         <v>523</v>
       </c>
@@ -4793,7 +4708,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1">
+    <row r="315" spans="1:5">
       <c r="A315" t="s">
         <v>524</v>
       </c>
@@ -4801,7 +4716,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1">
+    <row r="316" spans="1:5">
       <c r="A316" t="s">
         <v>525</v>
       </c>
@@ -4809,7 +4724,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1">
+    <row r="317" spans="1:5">
       <c r="A317" t="s">
         <v>526</v>
       </c>
@@ -4817,7 +4732,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1">
+    <row r="318" spans="1:5">
       <c r="A318" t="s">
         <v>527</v>
       </c>
@@ -4825,7 +4740,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1">
+    <row r="319" spans="1:5">
       <c r="A319" t="s">
         <v>529</v>
       </c>
@@ -4838,7 +4753,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1">
+    <row r="321" spans="1:2">
       <c r="A321" t="s">
         <v>531</v>
       </c>
@@ -4846,7 +4761,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1">
+    <row r="322" spans="1:2">
       <c r="A322" t="s">
         <v>532</v>
       </c>
@@ -4854,7 +4769,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1">
+    <row r="323" spans="1:2">
       <c r="A323" t="s">
         <v>533</v>
       </c>
@@ -4862,7 +4777,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1">
+    <row r="324" spans="1:2">
       <c r="A324" t="s">
         <v>535</v>
       </c>
@@ -4870,7 +4785,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1">
+    <row r="325" spans="1:2">
       <c r="A325" t="s">
         <v>536</v>
       </c>
@@ -4878,7 +4793,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1">
+    <row r="326" spans="1:2">
       <c r="A326" t="s">
         <v>537</v>
       </c>
@@ -4891,7 +4806,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1">
+    <row r="328" spans="1:2">
       <c r="A328" t="s">
         <v>538</v>
       </c>
@@ -4899,7 +4814,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1">
+    <row r="329" spans="1:2">
       <c r="A329" t="s">
         <v>539</v>
       </c>
@@ -4907,7 +4822,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1">
+    <row r="330" spans="1:2">
       <c r="A330" s="4" t="s">
         <v>540</v>
       </c>
@@ -4915,7 +4830,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1">
+    <row r="331" spans="1:2">
       <c r="A331" s="4" t="s">
         <v>542</v>
       </c>
@@ -4923,7 +4838,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="332" spans="1:2" hidden="1">
+    <row r="332" spans="1:2">
       <c r="A332" s="4" t="s">
         <v>543</v>
       </c>
@@ -4931,7 +4846,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1">
+    <row r="333" spans="1:2">
       <c r="A333" t="s">
         <v>544</v>
       </c>
@@ -4939,7 +4854,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="334" spans="1:2" hidden="1">
+    <row r="334" spans="1:2">
       <c r="A334" t="s">
         <v>545</v>
       </c>
@@ -4951,11 +4866,8 @@
       <c r="A335" t="s">
         <v>546</v>
       </c>
-      <c r="B335" s="10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" hidden="1">
+    </row>
+    <row r="336" spans="1:2">
       <c r="A336" t="s">
         <v>547</v>
       </c>
@@ -4963,7 +4875,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="337" spans="1:7" hidden="1">
+    <row r="337" spans="1:7">
       <c r="A337" t="s">
         <v>549</v>
       </c>
@@ -4971,7 +4883,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1">
+    <row r="338" spans="1:7">
       <c r="A338" t="s">
         <v>551</v>
       </c>
@@ -4979,7 +4891,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="339" spans="1:7" hidden="1">
+    <row r="339" spans="1:7">
       <c r="A339" t="s">
         <v>553</v>
       </c>
@@ -4987,7 +4899,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="340" spans="1:7" hidden="1">
+    <row r="340" spans="1:7">
       <c r="A340" t="s">
         <v>555</v>
       </c>
@@ -4995,7 +4907,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="341" spans="1:7" hidden="1">
+    <row r="341" spans="1:7">
       <c r="A341" t="s">
         <v>557</v>
       </c>
@@ -5003,7 +4915,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1">
+    <row r="342" spans="1:7">
       <c r="A342" t="s">
         <v>581</v>
       </c>
@@ -5011,7 +4923,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="343" spans="1:7" hidden="1">
+    <row r="343" spans="1:7">
       <c r="A343" t="s">
         <v>576</v>
       </c>
@@ -5019,7 +4931,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="344" spans="1:7" hidden="1">
+    <row r="344" spans="1:7">
       <c r="A344" t="s">
         <v>580</v>
       </c>
@@ -5027,7 +4939,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1">
+    <row r="345" spans="1:7">
       <c r="A345" t="s">
         <v>577</v>
       </c>
@@ -5035,7 +4947,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1">
+    <row r="346" spans="1:7">
       <c r="A346" t="s">
         <v>578</v>
       </c>
@@ -5043,7 +4955,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1">
+    <row r="347" spans="1:7">
       <c r="A347" t="s">
         <v>579</v>
       </c>
@@ -5051,7 +4963,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1">
+    <row r="348" spans="1:7">
       <c r="A348" t="s">
         <v>582</v>
       </c>
@@ -5059,7 +4971,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1">
+    <row r="349" spans="1:7">
       <c r="A349" t="s">
         <v>583</v>
       </c>
@@ -5067,7 +4979,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="17.25" hidden="1">
+    <row r="350" spans="1:7" ht="17.25">
       <c r="A350" t="s">
         <v>584</v>
       </c>
@@ -5079,7 +4991,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7" hidden="1">
+    <row r="351" spans="1:7">
       <c r="A351" t="s">
         <v>585</v>
       </c>
@@ -5104,14 +5016,12 @@
       <c r="A353" t="s">
         <v>587</v>
       </c>
-      <c r="B353" s="10" t="s">
-        <v>609</v>
-      </c>
+      <c r="B353" s="7"/>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7" hidden="1">
+    <row r="354" spans="1:7">
       <c r="A354" t="s">
         <v>588</v>
       </c>
@@ -5122,7 +5032,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7" hidden="1">
+    <row r="355" spans="1:7">
       <c r="A355" t="s">
         <v>589</v>
       </c>
@@ -5133,7 +5043,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5" hidden="1">
+    <row r="356" spans="1:7" ht="19.5">
       <c r="A356" t="s">
         <v>590</v>
       </c>
@@ -5145,7 +5055,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7" hidden="1">
+    <row r="357" spans="1:7">
       <c r="A357" t="s">
         <v>591</v>
       </c>
@@ -5157,7 +5067,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7" hidden="1">
+    <row r="358" spans="1:7">
       <c r="A358" t="s">
         <v>592</v>
       </c>
@@ -5168,7 +5078,7 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7" hidden="1">
+    <row r="359" spans="1:7">
       <c r="A359" t="s">
         <v>593</v>
       </c>
@@ -5241,11 +5151,7 @@
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362">
-    <filterColumn colId="1">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H362"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5455,18 +5361,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5489,18 +5395,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
.gitignore added, update themenzuordnung
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="611">
   <si>
     <t>Themen</t>
   </si>
@@ -1819,13 +1819,49 @@
   </si>
   <si>
     <t>domirow-fau</t>
+  </si>
+  <si>
+    <t>Adaye1e</t>
+  </si>
+  <si>
+    <t>enesmvlt</t>
+  </si>
+  <si>
+    <t>tkessler94</t>
+  </si>
+  <si>
+    <t>AmrouHasan</t>
+  </si>
+  <si>
+    <t>juliwebair</t>
+  </si>
+  <si>
+    <t>Irishcoffee09</t>
+  </si>
+  <si>
+    <t>bilgesb</t>
+  </si>
+  <si>
+    <t>TobiasZuerrlein</t>
+  </si>
+  <si>
+    <t>lukasheinrich9</t>
+  </si>
+  <si>
+    <t>fe94fiqy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SaskiaHe </t>
+  </si>
+  <si>
+    <t>EuleW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1876,8 +1912,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1888,6 +1931,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1918,7 +1967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1933,6 +1982,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2235,10 +2286,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2266,7 +2318,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2274,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2282,7 +2334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2291,7 +2343,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2299,7 +2351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2307,7 +2359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2315,7 +2367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2323,7 +2375,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2331,7 +2383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2339,7 +2391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2347,7 +2399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2355,7 +2407,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2363,7 +2415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2371,7 +2423,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2379,7 +2431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2387,7 +2439,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" hidden="1">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2395,7 +2447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" hidden="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2403,7 +2455,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" hidden="1">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2411,7 +2463,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" hidden="1">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2419,7 +2471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" hidden="1">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2427,7 +2479,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" hidden="1">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2435,7 +2487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" hidden="1">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2443,7 +2495,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" hidden="1">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2451,7 +2503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" hidden="1">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2459,7 +2511,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" hidden="1">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2467,7 +2519,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" hidden="1">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2475,7 +2527,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" hidden="1">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2492,8 +2544,11 @@
       <c r="A30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="B30" s="10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2501,7 +2556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" hidden="1">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2509,7 +2564,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2517,7 +2572,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2525,7 +2580,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" hidden="1">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2533,7 +2588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" hidden="1">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2541,7 +2596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2554,7 +2609,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2562,7 +2617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2570,7 +2625,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2578,7 +2633,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2586,7 +2641,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2595,7 +2650,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2604,7 +2659,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2612,7 +2667,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2624,8 +2679,11 @@
       <c r="A47" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="B47" s="10" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" hidden="1">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -2633,7 +2691,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" hidden="1">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -2641,7 +2699,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" hidden="1">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -2649,7 +2707,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" hidden="1">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2657,7 +2715,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" hidden="1">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2665,7 +2723,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" hidden="1">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2673,7 +2731,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" hidden="1">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2681,7 +2739,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" hidden="1">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2689,7 +2747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" hidden="1">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2697,7 +2755,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" hidden="1">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2705,7 +2763,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" hidden="1">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2713,7 +2771,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" hidden="1">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2721,7 +2779,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" hidden="1">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2729,7 +2787,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" hidden="1">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -2737,7 +2795,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" hidden="1">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -2745,7 +2803,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" hidden="1">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -2753,7 +2811,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" hidden="1">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -2761,7 +2819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" hidden="1">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -2769,7 +2827,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" hidden="1">
       <c r="A66" t="s">
         <v>123</v>
       </c>
@@ -2777,7 +2835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" hidden="1">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -2785,7 +2843,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -2793,7 +2851,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" hidden="1">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -2801,7 +2859,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" hidden="1">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -2813,8 +2871,11 @@
       <c r="A71" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="B71" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -2822,7 +2883,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" hidden="1">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -2830,7 +2891,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" hidden="1">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -2838,7 +2899,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" hidden="1">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -2846,7 +2907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" hidden="1">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -2854,7 +2915,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" hidden="1">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2862,7 +2923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" hidden="1">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2870,7 +2931,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" hidden="1">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2878,7 +2939,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" hidden="1">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2886,7 +2947,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" hidden="1">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2894,7 +2955,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" hidden="1">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -2902,7 +2963,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" hidden="1">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -2910,7 +2971,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" hidden="1">
       <c r="A84" t="s">
         <v>155</v>
       </c>
@@ -2918,7 +2979,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" hidden="1">
       <c r="A85" t="s">
         <v>156</v>
       </c>
@@ -2926,7 +2987,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" hidden="1">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -2934,7 +2995,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" hidden="1">
       <c r="A87" t="s">
         <v>160</v>
       </c>
@@ -2942,7 +3003,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" hidden="1">
       <c r="A88" t="s">
         <v>162</v>
       </c>
@@ -2950,7 +3011,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" hidden="1">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -2958,7 +3019,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" hidden="1">
       <c r="A90" t="s">
         <v>165</v>
       </c>
@@ -2966,7 +3027,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" hidden="1">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -2974,7 +3035,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" hidden="1">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -2982,7 +3043,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" hidden="1">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -2990,7 +3051,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" hidden="1">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -2998,7 +3059,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" hidden="1">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -3006,7 +3067,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" hidden="1">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3014,7 +3075,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" hidden="1">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -3022,7 +3083,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" hidden="1">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -3030,7 +3091,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" hidden="1">
       <c r="A99" t="s">
         <v>183</v>
       </c>
@@ -3038,7 +3099,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" hidden="1">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -3046,7 +3107,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" hidden="1">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -3054,7 +3115,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" hidden="1">
       <c r="A102" t="s">
         <v>189</v>
       </c>
@@ -3062,7 +3123,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" hidden="1">
       <c r="A103" t="s">
         <v>191</v>
       </c>
@@ -3070,7 +3131,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" hidden="1">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -3078,7 +3139,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" hidden="1">
       <c r="A105" t="s">
         <v>195</v>
       </c>
@@ -3086,7 +3147,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" hidden="1">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -3095,7 +3156,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" hidden="1">
       <c r="A107" t="s">
         <v>197</v>
       </c>
@@ -3103,7 +3164,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" hidden="1">
       <c r="A108" t="s">
         <v>199</v>
       </c>
@@ -3111,7 +3172,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" hidden="1">
       <c r="A109" t="s">
         <v>201</v>
       </c>
@@ -3119,7 +3180,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1">
       <c r="A110" t="s">
         <v>203</v>
       </c>
@@ -3127,7 +3188,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" hidden="1">
       <c r="A111" t="s">
         <v>205</v>
       </c>
@@ -3135,7 +3196,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" hidden="1">
       <c r="A112" t="s">
         <v>207</v>
       </c>
@@ -3143,7 +3204,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" hidden="1">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -3151,7 +3212,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" hidden="1">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -3159,7 +3220,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" hidden="1">
       <c r="A115" t="s">
         <v>213</v>
       </c>
@@ -3167,7 +3228,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" hidden="1">
       <c r="A116" t="s">
         <v>215</v>
       </c>
@@ -3175,7 +3236,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" hidden="1">
       <c r="A117" t="s">
         <v>217</v>
       </c>
@@ -3183,7 +3244,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" hidden="1">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3191,7 +3252,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" hidden="1">
       <c r="A119" t="s">
         <v>219</v>
       </c>
@@ -3199,7 +3260,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" hidden="1">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -3207,7 +3268,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" hidden="1">
       <c r="A121" t="s">
         <v>223</v>
       </c>
@@ -3215,7 +3276,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" hidden="1">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -3223,7 +3284,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" hidden="1">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -3231,7 +3292,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" hidden="1">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -3239,7 +3300,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" hidden="1">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -3247,7 +3308,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" hidden="1">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -3255,7 +3316,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" hidden="1">
       <c r="A127" t="s">
         <v>235</v>
       </c>
@@ -3263,7 +3324,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" hidden="1">
       <c r="A128" t="s">
         <v>236</v>
       </c>
@@ -3276,7 +3337,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" hidden="1">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -3284,7 +3345,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" hidden="1">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -3292,7 +3353,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" hidden="1">
       <c r="A132" t="s">
         <v>242</v>
       </c>
@@ -3300,7 +3361,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" hidden="1">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -3308,7 +3369,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" hidden="1">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -3316,7 +3377,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" hidden="1">
       <c r="A135" t="s">
         <v>247</v>
       </c>
@@ -3324,7 +3385,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" hidden="1">
       <c r="A136" t="s">
         <v>249</v>
       </c>
@@ -3332,7 +3393,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" hidden="1">
       <c r="A137" t="s">
         <v>251</v>
       </c>
@@ -3340,7 +3401,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" hidden="1">
       <c r="A138" t="s">
         <v>253</v>
       </c>
@@ -3352,13 +3413,19 @@
       <c r="A139" t="s">
         <v>255</v>
       </c>
+      <c r="B139" s="10" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="B140" s="10" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" hidden="1">
       <c r="A141" t="s">
         <v>257</v>
       </c>
@@ -3366,7 +3433,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" hidden="1">
       <c r="A142" t="s">
         <v>259</v>
       </c>
@@ -3374,7 +3441,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" hidden="1">
       <c r="A143" t="s">
         <v>260</v>
       </c>
@@ -3382,7 +3449,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" hidden="1">
       <c r="A144" t="s">
         <v>261</v>
       </c>
@@ -3390,7 +3457,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" hidden="1">
       <c r="A145" t="s">
         <v>263</v>
       </c>
@@ -3398,7 +3465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" hidden="1">
       <c r="A146" t="s">
         <v>264</v>
       </c>
@@ -3406,7 +3473,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" hidden="1">
       <c r="A147" t="s">
         <v>265</v>
       </c>
@@ -3414,7 +3481,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" hidden="1">
       <c r="A148" t="s">
         <v>266</v>
       </c>
@@ -3422,7 +3489,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" hidden="1">
       <c r="A149" t="s">
         <v>268</v>
       </c>
@@ -3430,7 +3497,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" hidden="1">
       <c r="A150" t="s">
         <v>270</v>
       </c>
@@ -3438,7 +3505,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" hidden="1">
       <c r="A151" t="s">
         <v>272</v>
       </c>
@@ -3446,7 +3513,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" hidden="1">
       <c r="A152" t="s">
         <v>274</v>
       </c>
@@ -3454,7 +3521,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" hidden="1">
       <c r="A153" t="s">
         <v>275</v>
       </c>
@@ -3462,7 +3529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" hidden="1">
       <c r="A154" t="s">
         <v>276</v>
       </c>
@@ -3470,7 +3537,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" hidden="1">
       <c r="A155" t="s">
         <v>277</v>
       </c>
@@ -3478,7 +3545,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" hidden="1">
       <c r="A156" t="s">
         <v>278</v>
       </c>
@@ -3490,8 +3557,11 @@
       <c r="A157" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="158" spans="1:2">
+      <c r="B157" s="10" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" hidden="1">
       <c r="A158" t="s">
         <v>280</v>
       </c>
@@ -3499,7 +3569,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" hidden="1">
       <c r="A159" t="s">
         <v>282</v>
       </c>
@@ -3507,7 +3577,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" hidden="1">
       <c r="A160" t="s">
         <v>284</v>
       </c>
@@ -3515,7 +3585,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" hidden="1">
       <c r="A161" t="s">
         <v>286</v>
       </c>
@@ -3523,7 +3593,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" hidden="1">
       <c r="A162" t="s">
         <v>288</v>
       </c>
@@ -3531,7 +3601,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" hidden="1">
       <c r="A163" s="4" t="s">
         <v>289</v>
       </c>
@@ -3539,7 +3609,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" hidden="1">
       <c r="A164" t="s">
         <v>291</v>
       </c>
@@ -3547,7 +3617,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" hidden="1">
       <c r="A165" t="s">
         <v>293</v>
       </c>
@@ -3555,7 +3625,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" hidden="1">
       <c r="A166" t="s">
         <v>294</v>
       </c>
@@ -3563,7 +3633,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" hidden="1">
       <c r="A167" t="s">
         <v>296</v>
       </c>
@@ -3571,7 +3641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" hidden="1">
       <c r="A168" t="s">
         <v>297</v>
       </c>
@@ -3579,7 +3649,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" hidden="1">
       <c r="A169" t="s">
         <v>298</v>
       </c>
@@ -3587,7 +3657,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" hidden="1">
       <c r="A170" t="s">
         <v>300</v>
       </c>
@@ -3595,7 +3665,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" hidden="1">
       <c r="A171" t="s">
         <v>302</v>
       </c>
@@ -3603,7 +3673,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" hidden="1">
       <c r="A172" t="s">
         <v>304</v>
       </c>
@@ -3611,7 +3681,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" hidden="1">
       <c r="A173" t="s">
         <v>305</v>
       </c>
@@ -3619,7 +3689,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" hidden="1">
       <c r="A174" t="s">
         <v>307</v>
       </c>
@@ -3627,7 +3697,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" hidden="1">
       <c r="A175" t="s">
         <v>309</v>
       </c>
@@ -3635,7 +3705,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" hidden="1">
       <c r="A176" t="s">
         <v>311</v>
       </c>
@@ -3643,7 +3713,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" hidden="1">
       <c r="A177" t="s">
         <v>313</v>
       </c>
@@ -3651,7 +3721,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" hidden="1">
       <c r="A178" t="s">
         <v>315</v>
       </c>
@@ -3659,7 +3729,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" hidden="1">
       <c r="A179" t="s">
         <v>316</v>
       </c>
@@ -3667,7 +3737,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" hidden="1">
       <c r="A180" t="s">
         <v>318</v>
       </c>
@@ -3680,7 +3750,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" hidden="1">
       <c r="A182" t="s">
         <v>321</v>
       </c>
@@ -3688,7 +3758,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" hidden="1">
       <c r="A183" t="s">
         <v>323</v>
       </c>
@@ -3696,7 +3766,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" hidden="1">
       <c r="A184" t="s">
         <v>325</v>
       </c>
@@ -3704,7 +3774,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" hidden="1">
       <c r="A185" t="s">
         <v>327</v>
       </c>
@@ -3712,7 +3782,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" hidden="1">
       <c r="A186" t="s">
         <v>329</v>
       </c>
@@ -3720,7 +3790,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" hidden="1">
       <c r="A187" t="s">
         <v>330</v>
       </c>
@@ -3728,7 +3798,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" hidden="1">
       <c r="A188" t="s">
         <v>331</v>
       </c>
@@ -3736,7 +3806,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" hidden="1">
       <c r="A189" t="s">
         <v>333</v>
       </c>
@@ -3744,7 +3814,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" hidden="1">
       <c r="A190" t="s">
         <v>335</v>
       </c>
@@ -3756,8 +3826,11 @@
       <c r="A191" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="192" spans="1:2">
+      <c r="B191" s="10" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" hidden="1">
       <c r="A192" t="s">
         <v>338</v>
       </c>
@@ -3765,7 +3838,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" hidden="1">
       <c r="A193" t="s">
         <v>339</v>
       </c>
@@ -3773,7 +3846,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" hidden="1">
       <c r="A194" t="s">
         <v>341</v>
       </c>
@@ -3781,7 +3854,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" hidden="1">
       <c r="A195" t="s">
         <v>343</v>
       </c>
@@ -3789,7 +3862,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" hidden="1">
       <c r="A196" t="s">
         <v>345</v>
       </c>
@@ -3797,7 +3870,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" hidden="1">
       <c r="A197" t="s">
         <v>347</v>
       </c>
@@ -3805,7 +3878,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5">
+    <row r="198" spans="1:2" ht="16.5" hidden="1">
       <c r="A198" t="s">
         <v>349</v>
       </c>
@@ -3813,7 +3886,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" hidden="1">
       <c r="A199" t="s">
         <v>351</v>
       </c>
@@ -3821,7 +3894,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" hidden="1">
       <c r="A200" t="s">
         <v>353</v>
       </c>
@@ -3829,7 +3902,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" hidden="1">
       <c r="A201" t="s">
         <v>355</v>
       </c>
@@ -3837,7 +3910,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" hidden="1">
       <c r="A202" t="s">
         <v>357</v>
       </c>
@@ -3845,7 +3918,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" hidden="1">
       <c r="A203" t="s">
         <v>359</v>
       </c>
@@ -3853,7 +3926,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" hidden="1">
       <c r="A204" t="s">
         <v>361</v>
       </c>
@@ -3861,7 +3934,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" hidden="1">
       <c r="A205" t="s">
         <v>363</v>
       </c>
@@ -3869,7 +3942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" hidden="1">
       <c r="A206" t="s">
         <v>364</v>
       </c>
@@ -3877,7 +3950,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" hidden="1">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -3885,7 +3958,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" hidden="1">
       <c r="A208" t="s">
         <v>559</v>
       </c>
@@ -3893,7 +3966,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" hidden="1">
       <c r="A209" t="s">
         <v>368</v>
       </c>
@@ -3901,7 +3974,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" hidden="1">
       <c r="A210" t="s">
         <v>370</v>
       </c>
@@ -3909,7 +3982,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" hidden="1">
       <c r="A211" t="s">
         <v>372</v>
       </c>
@@ -3917,7 +3990,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" hidden="1">
       <c r="A212" t="s">
         <v>374</v>
       </c>
@@ -3925,7 +3998,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" hidden="1">
       <c r="A213" t="s">
         <v>376</v>
       </c>
@@ -3933,7 +4006,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" hidden="1">
       <c r="A214" t="s">
         <v>378</v>
       </c>
@@ -3941,7 +4014,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" hidden="1">
       <c r="A215" t="s">
         <v>380</v>
       </c>
@@ -3949,7 +4022,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" hidden="1">
       <c r="A216" t="s">
         <v>381</v>
       </c>
@@ -3957,7 +4030,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" hidden="1">
       <c r="A217" t="s">
         <v>383</v>
       </c>
@@ -3965,7 +4038,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" hidden="1">
       <c r="A218" t="s">
         <v>385</v>
       </c>
@@ -3973,7 +4046,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" hidden="1">
       <c r="A219" t="s">
         <v>387</v>
       </c>
@@ -3985,8 +4058,11 @@
       <c r="A220" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="221" spans="1:2">
+      <c r="B220" s="10" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" hidden="1">
       <c r="A221" t="s">
         <v>389</v>
       </c>
@@ -3994,7 +4070,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" hidden="1">
       <c r="A222" t="s">
         <v>391</v>
       </c>
@@ -4002,7 +4078,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" hidden="1">
       <c r="A223" t="s">
         <v>393</v>
       </c>
@@ -4010,7 +4086,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" hidden="1">
       <c r="A224" t="s">
         <v>395</v>
       </c>
@@ -4018,7 +4094,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" hidden="1">
       <c r="A225" t="s">
         <v>397</v>
       </c>
@@ -4026,7 +4102,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" hidden="1">
       <c r="A226" t="s">
         <v>399</v>
       </c>
@@ -4034,7 +4110,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" hidden="1">
       <c r="A227" t="s">
         <v>401</v>
       </c>
@@ -4042,7 +4118,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" hidden="1">
       <c r="A228" t="s">
         <v>403</v>
       </c>
@@ -4050,7 +4126,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" hidden="1">
       <c r="A229" t="s">
         <v>405</v>
       </c>
@@ -4058,7 +4134,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" hidden="1">
       <c r="A230" t="s">
         <v>407</v>
       </c>
@@ -4066,7 +4142,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" hidden="1">
       <c r="A231" t="s">
         <v>409</v>
       </c>
@@ -4074,7 +4150,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" hidden="1">
       <c r="A232" t="s">
         <v>410</v>
       </c>
@@ -4082,7 +4158,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" hidden="1">
       <c r="A233" t="s">
         <v>412</v>
       </c>
@@ -4090,7 +4166,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" hidden="1">
       <c r="A234" t="s">
         <v>413</v>
       </c>
@@ -4098,7 +4174,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" hidden="1">
       <c r="A235" t="s">
         <v>415</v>
       </c>
@@ -4106,7 +4182,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" hidden="1">
       <c r="A236" t="s">
         <v>417</v>
       </c>
@@ -4114,7 +4190,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" hidden="1">
       <c r="A237" t="s">
         <v>419</v>
       </c>
@@ -4122,7 +4198,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" hidden="1">
       <c r="A238" t="s">
         <v>421</v>
       </c>
@@ -4130,7 +4206,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" hidden="1">
       <c r="A239" t="s">
         <v>423</v>
       </c>
@@ -4138,7 +4214,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" hidden="1">
       <c r="A240" t="s">
         <v>425</v>
       </c>
@@ -4146,7 +4222,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" hidden="1">
       <c r="A241" t="s">
         <v>426</v>
       </c>
@@ -4154,7 +4230,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" hidden="1">
       <c r="A242" t="s">
         <v>428</v>
       </c>
@@ -4167,7 +4243,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" hidden="1">
       <c r="A244" t="s">
         <v>431</v>
       </c>
@@ -4175,7 +4251,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" hidden="1">
       <c r="A245" t="s">
         <v>433</v>
       </c>
@@ -4183,7 +4259,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" hidden="1">
       <c r="A246" t="s">
         <v>435</v>
       </c>
@@ -4191,7 +4267,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" hidden="1">
       <c r="A247" t="s">
         <v>437</v>
       </c>
@@ -4204,7 +4280,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" hidden="1">
       <c r="A249" t="s">
         <v>439</v>
       </c>
@@ -4212,7 +4288,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" hidden="1">
       <c r="A250" t="s">
         <v>441</v>
       </c>
@@ -4220,7 +4296,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" hidden="1">
       <c r="A251" t="s">
         <v>443</v>
       </c>
@@ -4233,7 +4309,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" hidden="1">
       <c r="A253" t="s">
         <v>446</v>
       </c>
@@ -4245,13 +4321,19 @@
       <c r="A254" t="s">
         <v>448</v>
       </c>
+      <c r="B254" s="10" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="256" spans="1:2">
+      <c r="B255" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" hidden="1">
       <c r="A256" t="s">
         <v>450</v>
       </c>
@@ -4259,7 +4341,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" hidden="1">
       <c r="A257" t="s">
         <v>451</v>
       </c>
@@ -4267,7 +4349,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" hidden="1">
       <c r="A258" t="s">
         <v>452</v>
       </c>
@@ -4275,7 +4357,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" hidden="1">
       <c r="A259" t="s">
         <v>453</v>
       </c>
@@ -4283,7 +4365,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" hidden="1">
       <c r="A260" t="s">
         <v>454</v>
       </c>
@@ -4291,7 +4373,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" hidden="1">
       <c r="A261" t="s">
         <v>456</v>
       </c>
@@ -4299,7 +4381,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" hidden="1">
       <c r="A262" t="s">
         <v>458</v>
       </c>
@@ -4307,7 +4389,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" hidden="1">
       <c r="A263" t="s">
         <v>460</v>
       </c>
@@ -4315,7 +4397,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" hidden="1">
       <c r="A264" t="s">
         <v>461</v>
       </c>
@@ -4323,7 +4405,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" hidden="1">
       <c r="A265" t="s">
         <v>463</v>
       </c>
@@ -4331,7 +4413,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" hidden="1">
       <c r="A266" t="s">
         <v>465</v>
       </c>
@@ -4339,7 +4421,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" hidden="1">
       <c r="A267" t="s">
         <v>467</v>
       </c>
@@ -4347,7 +4429,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" hidden="1">
       <c r="A268" t="s">
         <v>468</v>
       </c>
@@ -4355,7 +4437,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" hidden="1">
       <c r="A269" t="s">
         <v>469</v>
       </c>
@@ -4377,13 +4459,16 @@
       <c r="A272" t="s">
         <v>473</v>
       </c>
+      <c r="B272" s="10" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" hidden="1">
       <c r="A274" t="s">
         <v>475</v>
       </c>
@@ -4391,7 +4476,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" hidden="1">
       <c r="A275" t="s">
         <v>477</v>
       </c>
@@ -4404,7 +4489,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" hidden="1">
       <c r="A277" t="s">
         <v>479</v>
       </c>
@@ -4412,7 +4497,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" hidden="1">
       <c r="A278" t="s">
         <v>481</v>
       </c>
@@ -4420,7 +4505,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" hidden="1">
       <c r="A279" t="s">
         <v>483</v>
       </c>
@@ -4428,7 +4513,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" hidden="1">
       <c r="A280" t="s">
         <v>484</v>
       </c>
@@ -4436,7 +4521,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" hidden="1">
       <c r="A281" t="s">
         <v>485</v>
       </c>
@@ -4444,7 +4529,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" hidden="1">
       <c r="A282" t="s">
         <v>487</v>
       </c>
@@ -4452,7 +4537,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" hidden="1">
       <c r="A283" t="s">
         <v>488</v>
       </c>
@@ -4460,7 +4545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" hidden="1">
       <c r="A284" t="s">
         <v>489</v>
       </c>
@@ -4468,7 +4553,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" hidden="1">
       <c r="A285" t="s">
         <v>490</v>
       </c>
@@ -4476,7 +4561,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" hidden="1">
       <c r="A286" t="s">
         <v>491</v>
       </c>
@@ -4484,7 +4569,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" hidden="1">
       <c r="A287" t="s">
         <v>492</v>
       </c>
@@ -4492,7 +4577,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" hidden="1">
       <c r="A288" t="s">
         <v>493</v>
       </c>
@@ -4500,7 +4585,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" hidden="1">
       <c r="A289" t="s">
         <v>494</v>
       </c>
@@ -4508,7 +4593,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" hidden="1">
       <c r="A290" t="s">
         <v>496</v>
       </c>
@@ -4516,7 +4601,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" hidden="1">
       <c r="A291" t="s">
         <v>498</v>
       </c>
@@ -4524,7 +4609,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" hidden="1">
       <c r="A292" t="s">
         <v>499</v>
       </c>
@@ -4532,7 +4617,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" hidden="1">
       <c r="A293" t="s">
         <v>500</v>
       </c>
@@ -4540,7 +4625,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" hidden="1">
       <c r="A294" t="s">
         <v>501</v>
       </c>
@@ -4548,7 +4633,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" hidden="1">
       <c r="A295" t="s">
         <v>502</v>
       </c>
@@ -4556,7 +4641,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" hidden="1">
       <c r="A296" t="s">
         <v>503</v>
       </c>
@@ -4564,7 +4649,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" hidden="1">
       <c r="A297" t="s">
         <v>504</v>
       </c>
@@ -4572,7 +4657,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" hidden="1">
       <c r="A298" t="s">
         <v>505</v>
       </c>
@@ -4580,7 +4665,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" hidden="1">
       <c r="A299" t="s">
         <v>506</v>
       </c>
@@ -4588,7 +4673,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" hidden="1">
       <c r="A300" t="s">
         <v>507</v>
       </c>
@@ -4596,7 +4681,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" hidden="1">
       <c r="A301" t="s">
         <v>509</v>
       </c>
@@ -4604,7 +4689,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" hidden="1">
       <c r="A302" t="s">
         <v>510</v>
       </c>
@@ -4617,7 +4702,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" hidden="1">
       <c r="A304" t="s">
         <v>512</v>
       </c>
@@ -4625,7 +4710,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:5" hidden="1">
       <c r="A305" t="s">
         <v>513</v>
       </c>
@@ -4633,7 +4718,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="306" spans="1:5">
+    <row r="306" spans="1:5" hidden="1">
       <c r="A306" t="s">
         <v>514</v>
       </c>
@@ -4644,7 +4729,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="307" spans="1:5">
+    <row r="307" spans="1:5" hidden="1">
       <c r="A307" t="s">
         <v>515</v>
       </c>
@@ -4652,7 +4737,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:5" hidden="1">
       <c r="A308" t="s">
         <v>516</v>
       </c>
@@ -4660,7 +4745,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:5">
+    <row r="309" spans="1:5" hidden="1">
       <c r="A309" t="s">
         <v>517</v>
       </c>
@@ -4668,7 +4753,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="310" spans="1:5">
+    <row r="310" spans="1:5" hidden="1">
       <c r="A310" t="s">
         <v>518</v>
       </c>
@@ -4676,7 +4761,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="311" spans="1:5">
+    <row r="311" spans="1:5" hidden="1">
       <c r="A311" t="s">
         <v>520</v>
       </c>
@@ -4684,7 +4769,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="312" spans="1:5">
+    <row r="312" spans="1:5" hidden="1">
       <c r="A312" t="s">
         <v>521</v>
       </c>
@@ -4692,7 +4777,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="313" spans="1:5">
+    <row r="313" spans="1:5" hidden="1">
       <c r="A313" t="s">
         <v>522</v>
       </c>
@@ -4700,7 +4785,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="314" spans="1:5">
+    <row r="314" spans="1:5" hidden="1">
       <c r="A314" t="s">
         <v>523</v>
       </c>
@@ -4708,7 +4793,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="315" spans="1:5">
+    <row r="315" spans="1:5" hidden="1">
       <c r="A315" t="s">
         <v>524</v>
       </c>
@@ -4716,7 +4801,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="316" spans="1:5">
+    <row r="316" spans="1:5" hidden="1">
       <c r="A316" t="s">
         <v>525</v>
       </c>
@@ -4724,7 +4809,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="317" spans="1:5">
+    <row r="317" spans="1:5" hidden="1">
       <c r="A317" t="s">
         <v>526</v>
       </c>
@@ -4732,7 +4817,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="318" spans="1:5">
+    <row r="318" spans="1:5" hidden="1">
       <c r="A318" t="s">
         <v>527</v>
       </c>
@@ -4740,7 +4825,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="319" spans="1:5">
+    <row r="319" spans="1:5" hidden="1">
       <c r="A319" t="s">
         <v>529</v>
       </c>
@@ -4753,7 +4838,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" hidden="1">
       <c r="A321" t="s">
         <v>531</v>
       </c>
@@ -4761,7 +4846,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" hidden="1">
       <c r="A322" t="s">
         <v>532</v>
       </c>
@@ -4769,7 +4854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" hidden="1">
       <c r="A323" t="s">
         <v>533</v>
       </c>
@@ -4777,7 +4862,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" hidden="1">
       <c r="A324" t="s">
         <v>535</v>
       </c>
@@ -4785,7 +4870,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" hidden="1">
       <c r="A325" t="s">
         <v>536</v>
       </c>
@@ -4793,7 +4878,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" hidden="1">
       <c r="A326" t="s">
         <v>537</v>
       </c>
@@ -4806,7 +4891,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" hidden="1">
       <c r="A328" t="s">
         <v>538</v>
       </c>
@@ -4814,7 +4899,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" hidden="1">
       <c r="A329" t="s">
         <v>539</v>
       </c>
@@ -4822,7 +4907,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" hidden="1">
       <c r="A330" s="4" t="s">
         <v>540</v>
       </c>
@@ -4830,7 +4915,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" hidden="1">
       <c r="A331" s="4" t="s">
         <v>542</v>
       </c>
@@ -4838,7 +4923,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" hidden="1">
       <c r="A332" s="4" t="s">
         <v>543</v>
       </c>
@@ -4846,7 +4931,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" hidden="1">
       <c r="A333" t="s">
         <v>544</v>
       </c>
@@ -4854,7 +4939,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" hidden="1">
       <c r="A334" t="s">
         <v>545</v>
       </c>
@@ -4866,8 +4951,11 @@
       <c r="A335" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="336" spans="1:2">
+      <c r="B335" s="10" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" hidden="1">
       <c r="A336" t="s">
         <v>547</v>
       </c>
@@ -4875,7 +4963,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1">
       <c r="A337" t="s">
         <v>549</v>
       </c>
@@ -4883,7 +4971,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" hidden="1">
       <c r="A338" t="s">
         <v>551</v>
       </c>
@@ -4891,7 +4979,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" t="s">
         <v>553</v>
       </c>
@@ -4899,7 +4987,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" t="s">
         <v>555</v>
       </c>
@@ -4907,7 +4995,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" t="s">
         <v>557</v>
       </c>
@@ -4915,7 +5003,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" t="s">
         <v>581</v>
       </c>
@@ -4923,7 +5011,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" t="s">
         <v>576</v>
       </c>
@@ -4931,7 +5019,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" t="s">
         <v>580</v>
       </c>
@@ -4939,7 +5027,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" t="s">
         <v>577</v>
       </c>
@@ -4947,7 +5035,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1">
       <c r="A346" t="s">
         <v>578</v>
       </c>
@@ -4955,7 +5043,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1">
       <c r="A347" t="s">
         <v>579</v>
       </c>
@@ -4963,7 +5051,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1">
       <c r="A348" t="s">
         <v>582</v>
       </c>
@@ -4971,7 +5059,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1">
       <c r="A349" t="s">
         <v>583</v>
       </c>
@@ -4979,7 +5067,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="17.25">
+    <row r="350" spans="1:7" ht="17.25" hidden="1">
       <c r="A350" t="s">
         <v>584</v>
       </c>
@@ -4991,7 +5079,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1">
       <c r="A351" t="s">
         <v>585</v>
       </c>
@@ -5016,12 +5104,14 @@
       <c r="A353" t="s">
         <v>587</v>
       </c>
-      <c r="B353" s="7"/>
+      <c r="B353" s="10" t="s">
+        <v>609</v>
+      </c>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:7" hidden="1">
       <c r="A354" t="s">
         <v>588</v>
       </c>
@@ -5032,7 +5122,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:7" hidden="1">
       <c r="A355" t="s">
         <v>589</v>
       </c>
@@ -5043,7 +5133,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5">
+    <row r="356" spans="1:7" ht="19.5" hidden="1">
       <c r="A356" t="s">
         <v>590</v>
       </c>
@@ -5055,7 +5145,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1">
       <c r="A357" t="s">
         <v>591</v>
       </c>
@@ -5067,7 +5157,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1">
       <c r="A358" t="s">
         <v>592</v>
       </c>
@@ -5078,7 +5168,7 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1">
       <c r="A359" t="s">
         <v>593</v>
       </c>
@@ -5151,7 +5241,11 @@
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362"/>
+  <autoFilter ref="A1:H362">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
correction of github username
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="610">
   <si>
     <t>Themen</t>
   </si>
@@ -778,9 +778,6 @@
   </si>
   <si>
     <t>Kanban_Work_in_Progress</t>
-  </si>
-  <si>
-    <t>ri26hugy</t>
   </si>
   <si>
     <t>Kanban_Karten</t>
@@ -2290,7 +2287,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+      <selection activeCell="B363" sqref="B363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2535,17 +2532,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" hidden="1">
       <c r="A29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" hidden="1">
       <c r="A30" t="s">
         <v>57</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="31" spans="1:2" hidden="1">
@@ -2604,7 +2601,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" hidden="1">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2638,7 +2635,7 @@
         <v>81</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="43" spans="1:3" hidden="1">
@@ -2675,12 +2672,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1">
       <c r="A47" t="s">
         <v>89</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1">
@@ -2867,12 +2864,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" hidden="1">
       <c r="A71" t="s">
         <v>132</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="72" spans="1:2" hidden="1">
@@ -3332,7 +3329,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" hidden="1">
       <c r="A129" t="s">
         <v>237</v>
       </c>
@@ -3393,49 +3390,49 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1">
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>251</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
+        <v>385</v>
       </c>
     </row>
     <row r="138" spans="1:2" hidden="1">
       <c r="A138" t="s">
+        <v>252</v>
+      </c>
+      <c r="B138" t="s">
         <v>253</v>
       </c>
-      <c r="B138" t="s">
+    </row>
+    <row r="139" spans="1:2" hidden="1">
+      <c r="A139" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
-      <c r="A139" t="s">
+      <c r="B139" s="10" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" hidden="1">
+      <c r="A140" t="s">
         <v>255</v>
       </c>
-      <c r="B139" s="10" t="s">
+      <c r="B140" s="10" t="s">
         <v>601</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
-      <c r="A140" t="s">
-        <v>256</v>
-      </c>
-      <c r="B140" s="10" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="141" spans="1:2" hidden="1">
       <c r="A141" t="s">
+        <v>256</v>
+      </c>
+      <c r="B141" t="s">
         <v>257</v>
-      </c>
-      <c r="B141" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:2" hidden="1">
       <c r="A142" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B142" t="s">
         <v>208</v>
@@ -3443,7 +3440,7 @@
     </row>
     <row r="143" spans="1:2" hidden="1">
       <c r="A143" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B143" t="s">
         <v>232</v>
@@ -3451,15 +3448,15 @@
     </row>
     <row r="144" spans="1:2" hidden="1">
       <c r="A144" t="s">
+        <v>260</v>
+      </c>
+      <c r="B144" t="s">
         <v>261</v>
-      </c>
-      <c r="B144" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="145" spans="1:2" hidden="1">
       <c r="A145" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B145" t="s">
         <v>58</v>
@@ -3467,55 +3464,55 @@
     </row>
     <row r="146" spans="1:2" hidden="1">
       <c r="A146" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B146" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1">
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B147" t="s">
-        <v>252</v>
+        <v>385</v>
       </c>
     </row>
     <row r="148" spans="1:2" hidden="1">
       <c r="A148" t="s">
+        <v>265</v>
+      </c>
+      <c r="B148" t="s">
         <v>266</v>
-      </c>
-      <c r="B148" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:2" hidden="1">
       <c r="A149" t="s">
+        <v>267</v>
+      </c>
+      <c r="B149" t="s">
         <v>268</v>
-      </c>
-      <c r="B149" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="150" spans="1:2" hidden="1">
       <c r="A150" t="s">
+        <v>269</v>
+      </c>
+      <c r="B150" t="s">
         <v>270</v>
-      </c>
-      <c r="B150" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:2" hidden="1">
       <c r="A151" t="s">
+        <v>271</v>
+      </c>
+      <c r="B151" t="s">
         <v>272</v>
-      </c>
-      <c r="B151" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="152" spans="1:2" hidden="1">
       <c r="A152" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B152" t="s">
         <v>91</v>
@@ -3523,7 +3520,7 @@
     </row>
     <row r="153" spans="1:2" hidden="1">
       <c r="A153" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B153" t="s">
         <v>17</v>
@@ -3531,7 +3528,7 @@
     </row>
     <row r="154" spans="1:2" hidden="1">
       <c r="A154" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B154" t="s">
         <v>94</v>
@@ -3539,7 +3536,7 @@
     </row>
     <row r="155" spans="1:2" hidden="1">
       <c r="A155" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B155" t="s">
         <v>119</v>
@@ -3547,79 +3544,79 @@
     </row>
     <row r="156" spans="1:2" hidden="1">
       <c r="A156" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B156" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" hidden="1">
       <c r="A157" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="158" spans="1:2" hidden="1">
       <c r="A158" t="s">
+        <v>279</v>
+      </c>
+      <c r="B158" t="s">
         <v>280</v>
-      </c>
-      <c r="B158" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="159" spans="1:2" hidden="1">
       <c r="A159" t="s">
+        <v>281</v>
+      </c>
+      <c r="B159" t="s">
         <v>282</v>
-      </c>
-      <c r="B159" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="160" spans="1:2" hidden="1">
       <c r="A160" t="s">
+        <v>283</v>
+      </c>
+      <c r="B160" t="s">
         <v>284</v>
-      </c>
-      <c r="B160" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="161" spans="1:2" hidden="1">
       <c r="A161" t="s">
+        <v>285</v>
+      </c>
+      <c r="B161" t="s">
         <v>286</v>
-      </c>
-      <c r="B161" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="162" spans="1:2" hidden="1">
       <c r="A162" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B162" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="163" spans="1:2" hidden="1">
       <c r="A163" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B163" t="s">
         <v>289</v>
-      </c>
-      <c r="B163" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="164" spans="1:2" hidden="1">
       <c r="A164" t="s">
+        <v>290</v>
+      </c>
+      <c r="B164" t="s">
         <v>291</v>
-      </c>
-      <c r="B164" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="165" spans="1:2" hidden="1">
       <c r="A165" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B165" t="s">
         <v>96</v>
@@ -3627,15 +3624,15 @@
     </row>
     <row r="166" spans="1:2" hidden="1">
       <c r="A166" t="s">
+        <v>293</v>
+      </c>
+      <c r="B166" t="s">
         <v>294</v>
-      </c>
-      <c r="B166" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="167" spans="1:2" hidden="1">
       <c r="A167" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
@@ -3643,7 +3640,7 @@
     </row>
     <row r="168" spans="1:2" hidden="1">
       <c r="A168" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B168" t="s">
         <v>190</v>
@@ -3651,140 +3648,140 @@
     </row>
     <row r="169" spans="1:2" hidden="1">
       <c r="A169" t="s">
+        <v>297</v>
+      </c>
+      <c r="B169" t="s">
         <v>298</v>
-      </c>
-      <c r="B169" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="170" spans="1:2" hidden="1">
       <c r="A170" t="s">
+        <v>299</v>
+      </c>
+      <c r="B170" t="s">
         <v>300</v>
-      </c>
-      <c r="B170" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="171" spans="1:2" hidden="1">
       <c r="A171" t="s">
+        <v>301</v>
+      </c>
+      <c r="B171" t="s">
         <v>302</v>
-      </c>
-      <c r="B171" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="172" spans="1:2" hidden="1">
       <c r="A172" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B172" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="173" spans="1:2" hidden="1">
       <c r="A173" t="s">
+        <v>304</v>
+      </c>
+      <c r="B173" t="s">
         <v>305</v>
-      </c>
-      <c r="B173" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="174" spans="1:2" hidden="1">
       <c r="A174" t="s">
+        <v>306</v>
+      </c>
+      <c r="B174" t="s">
         <v>307</v>
-      </c>
-      <c r="B174" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="175" spans="1:2" hidden="1">
       <c r="A175" t="s">
+        <v>308</v>
+      </c>
+      <c r="B175" t="s">
         <v>309</v>
-      </c>
-      <c r="B175" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="176" spans="1:2" hidden="1">
       <c r="A176" t="s">
+        <v>310</v>
+      </c>
+      <c r="B176" t="s">
         <v>311</v>
-      </c>
-      <c r="B176" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="177" spans="1:2" hidden="1">
       <c r="A177" t="s">
+        <v>312</v>
+      </c>
+      <c r="B177" t="s">
         <v>313</v>
-      </c>
-      <c r="B177" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="178" spans="1:2" hidden="1">
       <c r="A178" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B178" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" spans="1:2" hidden="1">
       <c r="A179" t="s">
+        <v>315</v>
+      </c>
+      <c r="B179" t="s">
         <v>316</v>
-      </c>
-      <c r="B179" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="180" spans="1:2" hidden="1">
       <c r="A180" t="s">
+        <v>317</v>
+      </c>
+      <c r="B180" t="s">
         <v>318</v>
       </c>
-      <c r="B180" t="s">
+    </row>
+    <row r="181" spans="1:2" hidden="1">
+      <c r="A181" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
-      <c r="A181" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="182" spans="1:2" hidden="1">
       <c r="A182" t="s">
+        <v>320</v>
+      </c>
+      <c r="B182" t="s">
         <v>321</v>
-      </c>
-      <c r="B182" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="183" spans="1:2" hidden="1">
       <c r="A183" t="s">
+        <v>322</v>
+      </c>
+      <c r="B183" t="s">
         <v>323</v>
-      </c>
-      <c r="B183" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="184" spans="1:2" hidden="1">
       <c r="A184" t="s">
+        <v>324</v>
+      </c>
+      <c r="B184" t="s">
         <v>325</v>
-      </c>
-      <c r="B184" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="185" spans="1:2" hidden="1">
       <c r="A185" t="s">
+        <v>326</v>
+      </c>
+      <c r="B185" t="s">
         <v>327</v>
-      </c>
-      <c r="B185" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="186" spans="1:2" hidden="1">
       <c r="A186" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B186" t="s">
         <v>226</v>
@@ -3792,47 +3789,47 @@
     </row>
     <row r="187" spans="1:2" hidden="1">
       <c r="A187" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B187" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="188" spans="1:2" hidden="1">
       <c r="A188" t="s">
+        <v>330</v>
+      </c>
+      <c r="B188" t="s">
         <v>331</v>
-      </c>
-      <c r="B188" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="189" spans="1:2" hidden="1">
       <c r="A189" t="s">
+        <v>332</v>
+      </c>
+      <c r="B189" t="s">
         <v>333</v>
-      </c>
-      <c r="B189" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="190" spans="1:2" hidden="1">
       <c r="A190" t="s">
+        <v>334</v>
+      </c>
+      <c r="B190" t="s">
         <v>335</v>
       </c>
-      <c r="B190" t="s">
+    </row>
+    <row r="191" spans="1:2" hidden="1">
+      <c r="A191" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="191" spans="1:2">
-      <c r="A191" t="s">
-        <v>337</v>
-      </c>
       <c r="B191" s="10" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="192" spans="1:2" hidden="1">
       <c r="A192" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B192" t="s">
         <v>248</v>
@@ -3840,103 +3837,103 @@
     </row>
     <row r="193" spans="1:2" hidden="1">
       <c r="A193" t="s">
+        <v>338</v>
+      </c>
+      <c r="B193" t="s">
         <v>339</v>
-      </c>
-      <c r="B193" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="194" spans="1:2" hidden="1">
       <c r="A194" t="s">
+        <v>340</v>
+      </c>
+      <c r="B194" t="s">
         <v>341</v>
-      </c>
-      <c r="B194" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="195" spans="1:2" hidden="1">
       <c r="A195" t="s">
+        <v>342</v>
+      </c>
+      <c r="B195" t="s">
         <v>343</v>
-      </c>
-      <c r="B195" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="196" spans="1:2" hidden="1">
       <c r="A196" t="s">
+        <v>344</v>
+      </c>
+      <c r="B196" t="s">
         <v>345</v>
-      </c>
-      <c r="B196" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="197" spans="1:2" hidden="1">
       <c r="A197" t="s">
+        <v>346</v>
+      </c>
+      <c r="B197" t="s">
         <v>347</v>
-      </c>
-      <c r="B197" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="16.5" hidden="1">
       <c r="A198" t="s">
+        <v>348</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>349</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="199" spans="1:2" hidden="1">
       <c r="A199" t="s">
+        <v>350</v>
+      </c>
+      <c r="B199" t="s">
         <v>351</v>
-      </c>
-      <c r="B199" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="200" spans="1:2" hidden="1">
       <c r="A200" t="s">
+        <v>352</v>
+      </c>
+      <c r="B200" t="s">
         <v>353</v>
-      </c>
-      <c r="B200" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="201" spans="1:2" hidden="1">
       <c r="A201" t="s">
+        <v>354</v>
+      </c>
+      <c r="B201" t="s">
         <v>355</v>
-      </c>
-      <c r="B201" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="202" spans="1:2" hidden="1">
       <c r="A202" t="s">
+        <v>356</v>
+      </c>
+      <c r="B202" t="s">
         <v>357</v>
-      </c>
-      <c r="B202" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="203" spans="1:2" hidden="1">
       <c r="A203" t="s">
+        <v>358</v>
+      </c>
+      <c r="B203" t="s">
         <v>359</v>
-      </c>
-      <c r="B203" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="204" spans="1:2" hidden="1">
       <c r="A204" t="s">
+        <v>360</v>
+      </c>
+      <c r="B204" t="s">
         <v>361</v>
-      </c>
-      <c r="B204" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="205" spans="1:2" hidden="1">
       <c r="A205" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B205" t="s">
         <v>98</v>
@@ -3944,23 +3941,23 @@
     </row>
     <row r="206" spans="1:2" hidden="1">
       <c r="A206" t="s">
+        <v>363</v>
+      </c>
+      <c r="B206" t="s">
         <v>364</v>
-      </c>
-      <c r="B206" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="207" spans="1:2" hidden="1">
       <c r="A207" t="s">
+        <v>365</v>
+      </c>
+      <c r="B207" t="s">
         <v>366</v>
-      </c>
-      <c r="B207" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="208" spans="1:2" hidden="1">
       <c r="A208" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B208" t="s">
         <v>246</v>
@@ -3968,55 +3965,55 @@
     </row>
     <row r="209" spans="1:2" hidden="1">
       <c r="A209" t="s">
+        <v>367</v>
+      </c>
+      <c r="B209" t="s">
         <v>368</v>
-      </c>
-      <c r="B209" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="210" spans="1:2" hidden="1">
       <c r="A210" t="s">
+        <v>369</v>
+      </c>
+      <c r="B210" t="s">
         <v>370</v>
-      </c>
-      <c r="B210" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="211" spans="1:2" hidden="1">
       <c r="A211" t="s">
+        <v>371</v>
+      </c>
+      <c r="B211" t="s">
         <v>372</v>
-      </c>
-      <c r="B211" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="212" spans="1:2" hidden="1">
       <c r="A212" t="s">
+        <v>373</v>
+      </c>
+      <c r="B212" t="s">
         <v>374</v>
-      </c>
-      <c r="B212" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="213" spans="1:2" hidden="1">
       <c r="A213" t="s">
+        <v>375</v>
+      </c>
+      <c r="B213" t="s">
         <v>376</v>
-      </c>
-      <c r="B213" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="214" spans="1:2" hidden="1">
       <c r="A214" t="s">
+        <v>377</v>
+      </c>
+      <c r="B214" t="s">
         <v>378</v>
-      </c>
-      <c r="B214" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="215" spans="1:2" hidden="1">
       <c r="A215" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B215" t="s">
         <v>241</v>
@@ -4024,318 +4021,318 @@
     </row>
     <row r="216" spans="1:2" hidden="1">
       <c r="A216" t="s">
+        <v>380</v>
+      </c>
+      <c r="B216" t="s">
         <v>381</v>
-      </c>
-      <c r="B216" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="217" spans="1:2" hidden="1">
       <c r="A217" t="s">
+        <v>382</v>
+      </c>
+      <c r="B217" t="s">
         <v>383</v>
-      </c>
-      <c r="B217" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="218" spans="1:2" hidden="1">
       <c r="A218" t="s">
+        <v>384</v>
+      </c>
+      <c r="B218" t="s">
         <v>385</v>
-      </c>
-      <c r="B218" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="219" spans="1:2" hidden="1">
       <c r="A219" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B219" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" hidden="1">
       <c r="A220" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="221" spans="1:2" hidden="1">
       <c r="A221" t="s">
+        <v>388</v>
+      </c>
+      <c r="B221" t="s">
         <v>389</v>
-      </c>
-      <c r="B221" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="222" spans="1:2" hidden="1">
       <c r="A222" t="s">
+        <v>390</v>
+      </c>
+      <c r="B222" t="s">
         <v>391</v>
-      </c>
-      <c r="B222" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="223" spans="1:2" hidden="1">
       <c r="A223" t="s">
+        <v>392</v>
+      </c>
+      <c r="B223" t="s">
         <v>393</v>
-      </c>
-      <c r="B223" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="224" spans="1:2" hidden="1">
       <c r="A224" t="s">
+        <v>394</v>
+      </c>
+      <c r="B224" t="s">
         <v>395</v>
-      </c>
-      <c r="B224" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="225" spans="1:2" hidden="1">
       <c r="A225" t="s">
+        <v>396</v>
+      </c>
+      <c r="B225" t="s">
         <v>397</v>
-      </c>
-      <c r="B225" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="226" spans="1:2" hidden="1">
       <c r="A226" t="s">
+        <v>398</v>
+      </c>
+      <c r="B226" t="s">
         <v>399</v>
-      </c>
-      <c r="B226" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="227" spans="1:2" hidden="1">
       <c r="A227" t="s">
+        <v>400</v>
+      </c>
+      <c r="B227" t="s">
         <v>401</v>
-      </c>
-      <c r="B227" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="228" spans="1:2" hidden="1">
       <c r="A228" t="s">
+        <v>402</v>
+      </c>
+      <c r="B228" t="s">
         <v>403</v>
-      </c>
-      <c r="B228" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="229" spans="1:2" hidden="1">
       <c r="A229" t="s">
+        <v>404</v>
+      </c>
+      <c r="B229" t="s">
         <v>405</v>
-      </c>
-      <c r="B229" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="230" spans="1:2" hidden="1">
       <c r="A230" t="s">
+        <v>406</v>
+      </c>
+      <c r="B230" t="s">
         <v>407</v>
-      </c>
-      <c r="B230" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="231" spans="1:2" hidden="1">
       <c r="A231" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B231" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="232" spans="1:2" hidden="1">
       <c r="A232" t="s">
+        <v>409</v>
+      </c>
+      <c r="B232" t="s">
         <v>410</v>
-      </c>
-      <c r="B232" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="233" spans="1:2" hidden="1">
       <c r="A233" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B233" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="234" spans="1:2" hidden="1">
       <c r="A234" t="s">
+        <v>412</v>
+      </c>
+      <c r="B234" t="s">
         <v>413</v>
-      </c>
-      <c r="B234" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="235" spans="1:2" hidden="1">
       <c r="A235" t="s">
+        <v>414</v>
+      </c>
+      <c r="B235" t="s">
         <v>415</v>
-      </c>
-      <c r="B235" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="236" spans="1:2" hidden="1">
       <c r="A236" t="s">
+        <v>416</v>
+      </c>
+      <c r="B236" t="s">
         <v>417</v>
-      </c>
-      <c r="B236" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="237" spans="1:2" hidden="1">
       <c r="A237" t="s">
+        <v>418</v>
+      </c>
+      <c r="B237" t="s">
         <v>419</v>
-      </c>
-      <c r="B237" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="238" spans="1:2" hidden="1">
       <c r="A238" t="s">
+        <v>420</v>
+      </c>
+      <c r="B238" t="s">
         <v>421</v>
-      </c>
-      <c r="B238" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="239" spans="1:2" hidden="1">
       <c r="A239" t="s">
+        <v>422</v>
+      </c>
+      <c r="B239" t="s">
         <v>423</v>
-      </c>
-      <c r="B239" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="240" spans="1:2" hidden="1">
       <c r="A240" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B240" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="241" spans="1:2" hidden="1">
       <c r="A241" t="s">
+        <v>425</v>
+      </c>
+      <c r="B241" t="s">
         <v>426</v>
-      </c>
-      <c r="B241" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="242" spans="1:2" hidden="1">
       <c r="A242" t="s">
+        <v>427</v>
+      </c>
+      <c r="B242" t="s">
         <v>428</v>
       </c>
-      <c r="B242" t="s">
+    </row>
+    <row r="243" spans="1:2" hidden="1">
+      <c r="A243" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2">
-      <c r="A243" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="244" spans="1:2" hidden="1">
       <c r="A244" t="s">
+        <v>430</v>
+      </c>
+      <c r="B244" t="s">
         <v>431</v>
-      </c>
-      <c r="B244" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="245" spans="1:2" hidden="1">
       <c r="A245" t="s">
+        <v>432</v>
+      </c>
+      <c r="B245" t="s">
         <v>433</v>
-      </c>
-      <c r="B245" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="246" spans="1:2" hidden="1">
       <c r="A246" t="s">
+        <v>434</v>
+      </c>
+      <c r="B246" t="s">
         <v>435</v>
-      </c>
-      <c r="B246" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="247" spans="1:2" hidden="1">
       <c r="A247" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B247" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" hidden="1">
       <c r="A248" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="249" spans="1:2" hidden="1">
       <c r="A249" t="s">
+        <v>438</v>
+      </c>
+      <c r="B249" t="s">
         <v>439</v>
-      </c>
-      <c r="B249" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="250" spans="1:2" hidden="1">
       <c r="A250" t="s">
+        <v>440</v>
+      </c>
+      <c r="B250" t="s">
         <v>441</v>
-      </c>
-      <c r="B250" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="251" spans="1:2" hidden="1">
       <c r="A251" t="s">
+        <v>442</v>
+      </c>
+      <c r="B251" t="s">
         <v>443</v>
       </c>
-      <c r="B251" t="s">
+    </row>
+    <row r="252" spans="1:2" hidden="1">
+      <c r="A252" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2">
-      <c r="A252" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="253" spans="1:2" hidden="1">
       <c r="A253" t="s">
+        <v>445</v>
+      </c>
+      <c r="B253" t="s">
         <v>446</v>
       </c>
-      <c r="B253" t="s">
+    </row>
+    <row r="254" spans="1:2" hidden="1">
+      <c r="A254" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="254" spans="1:2">
-      <c r="A254" t="s">
+      <c r="B254" s="10" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" hidden="1">
+      <c r="A255" t="s">
         <v>448</v>
       </c>
-      <c r="B254" s="10" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2">
-      <c r="A255" t="s">
-        <v>449</v>
-      </c>
       <c r="B255" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="256" spans="1:2" hidden="1">
       <c r="A256" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B256" t="s">
         <v>238</v>
@@ -4343,95 +4340,95 @@
     </row>
     <row r="257" spans="1:2" hidden="1">
       <c r="A257" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B257" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="258" spans="1:2" hidden="1">
       <c r="A258" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B258" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="259" spans="1:2" hidden="1">
       <c r="A259" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="260" spans="1:2" hidden="1">
       <c r="A260" t="s">
+        <v>453</v>
+      </c>
+      <c r="B260" t="s">
         <v>454</v>
-      </c>
-      <c r="B260" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="261" spans="1:2" hidden="1">
       <c r="A261" t="s">
+        <v>455</v>
+      </c>
+      <c r="B261" t="s">
         <v>456</v>
-      </c>
-      <c r="B261" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="262" spans="1:2" hidden="1">
       <c r="A262" t="s">
+        <v>457</v>
+      </c>
+      <c r="B262" t="s">
         <v>458</v>
-      </c>
-      <c r="B262" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="263" spans="1:2" hidden="1">
       <c r="A263" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B263" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="264" spans="1:2" hidden="1">
       <c r="A264" t="s">
+        <v>460</v>
+      </c>
+      <c r="B264" t="s">
         <v>461</v>
-      </c>
-      <c r="B264" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="265" spans="1:2" hidden="1">
       <c r="A265" t="s">
+        <v>462</v>
+      </c>
+      <c r="B265" t="s">
         <v>463</v>
-      </c>
-      <c r="B265" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="266" spans="1:2" hidden="1">
       <c r="A266" t="s">
+        <v>464</v>
+      </c>
+      <c r="B266" t="s">
         <v>465</v>
-      </c>
-      <c r="B266" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="267" spans="1:2" hidden="1">
       <c r="A267" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B267" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="268" spans="1:2" hidden="1">
       <c r="A268" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B268" t="s">
         <v>250</v>
@@ -4439,83 +4436,83 @@
     </row>
     <row r="269" spans="1:2" hidden="1">
       <c r="A269" t="s">
+        <v>468</v>
+      </c>
+      <c r="B269" t="s">
         <v>469</v>
       </c>
-      <c r="B269" t="s">
+    </row>
+    <row r="270" spans="1:2" hidden="1">
+      <c r="A270" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
-      <c r="A270" t="s">
+    <row r="271" spans="1:2" hidden="1">
+      <c r="A271" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
-      <c r="A271" t="s">
+    <row r="272" spans="1:2" hidden="1">
+      <c r="A272" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="272" spans="1:2">
-      <c r="A272" t="s">
+      <c r="B272" s="10" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" hidden="1">
+      <c r="A273" t="s">
         <v>473</v>
-      </c>
-      <c r="B272" s="10" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2">
-      <c r="A273" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="274" spans="1:2" hidden="1">
       <c r="A274" t="s">
+        <v>474</v>
+      </c>
+      <c r="B274" t="s">
         <v>475</v>
-      </c>
-      <c r="B274" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="275" spans="1:2" hidden="1">
       <c r="A275" t="s">
+        <v>476</v>
+      </c>
+      <c r="B275" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" hidden="1">
+      <c r="A276" t="s">
         <v>477</v>
-      </c>
-      <c r="B275" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2">
-      <c r="A276" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="277" spans="1:2" hidden="1">
       <c r="A277" t="s">
+        <v>478</v>
+      </c>
+      <c r="B277" t="s">
         <v>479</v>
-      </c>
-      <c r="B277" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="278" spans="1:2" hidden="1">
       <c r="A278" t="s">
+        <v>480</v>
+      </c>
+      <c r="B278" t="s">
         <v>481</v>
-      </c>
-      <c r="B278" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="279" spans="1:2" hidden="1">
       <c r="A279" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B279" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="280" spans="1:2" hidden="1">
       <c r="A280" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B280" t="s">
         <v>136</v>
@@ -4523,15 +4520,15 @@
     </row>
     <row r="281" spans="1:2" hidden="1">
       <c r="A281" t="s">
+        <v>484</v>
+      </c>
+      <c r="B281" t="s">
         <v>485</v>
-      </c>
-      <c r="B281" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="282" spans="1:2" hidden="1">
       <c r="A282" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B282" t="s">
         <v>125</v>
@@ -4539,7 +4536,7 @@
     </row>
     <row r="283" spans="1:2" hidden="1">
       <c r="A283" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B283" t="s">
         <v>5</v>
@@ -4547,7 +4544,7 @@
     </row>
     <row r="284" spans="1:2" hidden="1">
       <c r="A284" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B284" t="s">
         <v>131</v>
@@ -4555,31 +4552,31 @@
     </row>
     <row r="285" spans="1:2" hidden="1">
       <c r="A285" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="286" spans="1:2" hidden="1">
       <c r="A286" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B286" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="287" spans="1:2" hidden="1">
       <c r="A287" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B287" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="288" spans="1:2" hidden="1">
       <c r="A288" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B288" t="s">
         <v>74</v>
@@ -4587,31 +4584,31 @@
     </row>
     <row r="289" spans="1:2" hidden="1">
       <c r="A289" t="s">
+        <v>493</v>
+      </c>
+      <c r="B289" t="s">
         <v>494</v>
-      </c>
-      <c r="B289" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="290" spans="1:2" hidden="1">
       <c r="A290" t="s">
+        <v>495</v>
+      </c>
+      <c r="B290" t="s">
         <v>496</v>
-      </c>
-      <c r="B290" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="291" spans="1:2" hidden="1">
       <c r="A291" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B291" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="292" spans="1:2" hidden="1">
       <c r="A292" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B292" t="s">
         <v>202</v>
@@ -4619,7 +4616,7 @@
     </row>
     <row r="293" spans="1:2" hidden="1">
       <c r="A293" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B293" t="s">
         <v>141</v>
@@ -4627,7 +4624,7 @@
     </row>
     <row r="294" spans="1:2" hidden="1">
       <c r="A294" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B294" t="s">
         <v>115</v>
@@ -4635,31 +4632,31 @@
     </row>
     <row r="295" spans="1:2" hidden="1">
       <c r="A295" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B295" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="296" spans="1:2" hidden="1">
       <c r="A296" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B296" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="297" spans="1:2" hidden="1">
       <c r="A297" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="298" spans="1:2" hidden="1">
       <c r="A298" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B298" t="s">
         <v>86</v>
@@ -4667,23 +4664,23 @@
     </row>
     <row r="299" spans="1:2" hidden="1">
       <c r="A299" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B299" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="300" spans="1:2" hidden="1">
       <c r="A300" t="s">
+        <v>506</v>
+      </c>
+      <c r="B300" t="s">
         <v>507</v>
-      </c>
-      <c r="B300" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="301" spans="1:2" hidden="1">
       <c r="A301" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B301" t="s">
         <v>206</v>
@@ -4691,28 +4688,28 @@
     </row>
     <row r="302" spans="1:2" hidden="1">
       <c r="A302" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B302" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" hidden="1">
       <c r="A303" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="304" spans="1:2" hidden="1">
       <c r="A304" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B304" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="305" spans="1:5" hidden="1">
       <c r="A305" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B305" t="s">
         <v>68</v>
@@ -4720,18 +4717,18 @@
     </row>
     <row r="306" spans="1:5" hidden="1">
       <c r="A306" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E306" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="307" spans="1:5" hidden="1">
       <c r="A307" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B307" t="s">
         <v>117</v>
@@ -4739,7 +4736,7 @@
     </row>
     <row r="308" spans="1:5" hidden="1">
       <c r="A308" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B308" t="s">
         <v>41</v>
@@ -4747,31 +4744,31 @@
     </row>
     <row r="309" spans="1:5" hidden="1">
       <c r="A309" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B309" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="310" spans="1:5" hidden="1">
       <c r="A310" t="s">
+        <v>517</v>
+      </c>
+      <c r="B310" t="s">
         <v>518</v>
-      </c>
-      <c r="B310" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="311" spans="1:5" hidden="1">
       <c r="A311" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B311" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="312" spans="1:5" hidden="1">
       <c r="A312" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B312" t="s">
         <v>113</v>
@@ -4779,68 +4776,68 @@
     </row>
     <row r="313" spans="1:5" hidden="1">
       <c r="A313" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B313" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="314" spans="1:5" hidden="1">
       <c r="A314" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B314" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="315" spans="1:5" hidden="1">
       <c r="A315" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B315" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="316" spans="1:5" hidden="1">
       <c r="A316" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B316" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="317" spans="1:5" hidden="1">
       <c r="A317" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B317" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="318" spans="1:5" hidden="1">
       <c r="A318" t="s">
+        <v>526</v>
+      </c>
+      <c r="B318" t="s">
         <v>527</v>
-      </c>
-      <c r="B318" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="319" spans="1:5" hidden="1">
       <c r="A319" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="320" spans="1:5">
+    <row r="320" spans="1:5" hidden="1">
       <c r="A320" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="321" spans="1:2" hidden="1">
       <c r="A321" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B321" t="s">
         <v>178</v>
@@ -4848,7 +4845,7 @@
     </row>
     <row r="322" spans="1:2" hidden="1">
       <c r="A322" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B322" t="s">
         <v>43</v>
@@ -4856,52 +4853,52 @@
     </row>
     <row r="323" spans="1:2" hidden="1">
       <c r="A323" t="s">
+        <v>532</v>
+      </c>
+      <c r="B323" t="s">
         <v>533</v>
-      </c>
-      <c r="B323" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="324" spans="1:2" hidden="1">
       <c r="A324" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B324" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="325" spans="1:2" hidden="1">
       <c r="A325" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B325" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="326" spans="1:2" hidden="1">
       <c r="A326" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B326" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" hidden="1">
       <c r="A327" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="328" spans="1:2" hidden="1">
       <c r="A328" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B328" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="329" spans="1:2" hidden="1">
       <c r="A329" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B329" t="s">
         <v>62</v>
@@ -4909,31 +4906,31 @@
     </row>
     <row r="330" spans="1:2" hidden="1">
       <c r="A330" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="B330" t="s">
         <v>540</v>
-      </c>
-      <c r="B330" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="331" spans="1:2" hidden="1">
       <c r="A331" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B331" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="332" spans="1:2" hidden="1">
       <c r="A332" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B332" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="333" spans="1:2" hidden="1">
       <c r="A333" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B333" t="s">
         <v>82</v>
@@ -4941,138 +4938,138 @@
     </row>
     <row r="334" spans="1:2" hidden="1">
       <c r="A334" t="s">
+        <v>544</v>
+      </c>
+      <c r="B334" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" hidden="1">
+      <c r="A335" t="s">
         <v>545</v>
       </c>
-      <c r="B334" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2">
-      <c r="A335" t="s">
-        <v>546</v>
-      </c>
       <c r="B335" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="336" spans="1:2" hidden="1">
       <c r="A336" t="s">
+        <v>546</v>
+      </c>
+      <c r="B336" t="s">
         <v>547</v>
-      </c>
-      <c r="B336" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="337" spans="1:7" hidden="1">
       <c r="A337" t="s">
+        <v>548</v>
+      </c>
+      <c r="B337" t="s">
         <v>549</v>
-      </c>
-      <c r="B337" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="338" spans="1:7" hidden="1">
       <c r="A338" t="s">
+        <v>550</v>
+      </c>
+      <c r="B338" t="s">
         <v>551</v>
-      </c>
-      <c r="B338" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="339" spans="1:7" hidden="1">
       <c r="A339" t="s">
+        <v>552</v>
+      </c>
+      <c r="B339" t="s">
         <v>553</v>
-      </c>
-      <c r="B339" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="340" spans="1:7" hidden="1">
       <c r="A340" t="s">
+        <v>554</v>
+      </c>
+      <c r="B340" t="s">
         <v>555</v>
-      </c>
-      <c r="B340" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="341" spans="1:7" hidden="1">
       <c r="A341" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B341" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="342" spans="1:7" hidden="1">
       <c r="A342" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="343" spans="1:7" hidden="1">
       <c r="A343" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B343" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="344" spans="1:7" hidden="1">
       <c r="A344" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B344" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="345" spans="1:7" hidden="1">
       <c r="A345" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="346" spans="1:7" hidden="1">
       <c r="A346" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="347" spans="1:7" hidden="1">
       <c r="A347" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B347" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="348" spans="1:7" hidden="1">
       <c r="A348" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="349" spans="1:7" hidden="1">
       <c r="A349" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B349" s="7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="17.25" hidden="1">
       <c r="A350" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B350" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D350" s="7"/>
       <c r="E350" s="7"/>
@@ -5081,31 +5078,31 @@
     </row>
     <row r="351" spans="1:7" hidden="1">
       <c r="A351" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B351" s="7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D351" s="7"/>
       <c r="E351" s="7"/>
       <c r="F351" s="7"/>
       <c r="G351" s="7"/>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" hidden="1">
       <c r="A352" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B352" s="7"/>
       <c r="E352" s="7"/>
       <c r="F352" s="7"/>
       <c r="G352" s="7"/>
     </row>
-    <row r="353" spans="1:7">
+    <row r="353" spans="1:7" hidden="1">
       <c r="A353" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B353" s="10" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
@@ -5113,10 +5110,10 @@
     </row>
     <row r="354" spans="1:7" hidden="1">
       <c r="A354" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B354" s="7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E354" s="7"/>
       <c r="F354" s="7"/>
@@ -5124,10 +5121,10 @@
     </row>
     <row r="355" spans="1:7" hidden="1">
       <c r="A355" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B355" s="7" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E355" s="7"/>
       <c r="F355" s="7"/>
@@ -5135,10 +5132,10 @@
     </row>
     <row r="356" spans="1:7" ht="19.5" hidden="1">
       <c r="A356" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D356" s="8"/>
       <c r="E356" s="7"/>
@@ -5147,10 +5144,10 @@
     </row>
     <row r="357" spans="1:7" hidden="1">
       <c r="A357" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B357" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D357" s="7"/>
       <c r="E357" s="7"/>
@@ -5159,10 +5156,10 @@
     </row>
     <row r="358" spans="1:7" hidden="1">
       <c r="A358" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E358" s="7"/>
       <c r="F358" s="7"/>
@@ -5170,34 +5167,34 @@
     </row>
     <row r="359" spans="1:7" hidden="1">
       <c r="A359" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E359" s="7"/>
       <c r="F359" s="7"/>
       <c r="G359" s="7"/>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" hidden="1">
       <c r="A360" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E360" s="7"/>
       <c r="F360" s="7"/>
       <c r="G360" s="7"/>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" hidden="1">
       <c r="A361" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E361" s="7"/>
       <c r="F361" s="7"/>
       <c r="G361" s="7"/>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" hidden="1">
       <c r="A362" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E362" s="7"/>
       <c r="F362" s="7"/>
@@ -5243,7 +5240,9 @@
   </sheetData>
   <autoFilter ref="A1:H362">
     <filterColumn colId="1">
-      <filters blank="1"/>
+      <filters>
+        <filter val="ri26hugy"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5455,18 +5454,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5489,18 +5488,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
user @GEDA9263 eingetargen agil + klassisch
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="613">
   <si>
     <t>Themen</t>
   </si>
@@ -1858,6 +1858,9 @@
   </si>
   <si>
     <t>hello-pukeko</t>
+  </si>
+  <si>
+    <t>GEDA9263</t>
   </si>
 </sst>
 </file>
@@ -2305,10 +2308,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2336,7 +2340,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2344,7 +2348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2361,7 +2365,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2369,7 +2373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2377,7 +2381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2393,7 +2397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2401,7 +2405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2409,7 +2413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2425,7 +2429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2433,7 +2437,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2449,7 +2453,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2457,7 +2461,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" hidden="1">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2465,7 +2469,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" hidden="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" hidden="1">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2481,7 +2485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" hidden="1">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2489,7 +2493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" hidden="1">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2497,7 +2501,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" hidden="1">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2505,7 +2509,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" hidden="1">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2513,7 +2517,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" hidden="1">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2521,7 +2525,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" hidden="1">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2529,7 +2533,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" hidden="1">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2537,7 +2541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" hidden="1">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2545,7 +2549,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" hidden="1">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2558,7 +2562,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" hidden="1">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2566,7 +2570,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" hidden="1">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2574,7 +2578,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" hidden="1">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2582,7 +2586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" hidden="1">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2606,7 +2610,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" hidden="1">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2614,7 +2618,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2627,7 +2631,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2643,7 +2647,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2668,7 +2672,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2677,7 +2681,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2685,7 +2689,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2693,7 +2697,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" hidden="1">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -2709,7 +2713,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" hidden="1">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -2717,7 +2721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" hidden="1">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -2725,7 +2729,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" hidden="1">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2733,7 +2737,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" hidden="1">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2741,7 +2745,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" hidden="1">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2749,7 +2753,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" hidden="1">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2757,7 +2761,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" hidden="1">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -2765,7 +2769,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" hidden="1">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2773,7 +2777,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" hidden="1">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2781,7 +2785,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" hidden="1">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" hidden="1">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2797,7 +2801,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" hidden="1">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2805,7 +2809,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" hidden="1">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -2813,7 +2817,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" hidden="1">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -2821,7 +2825,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" hidden="1">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -2829,7 +2833,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" hidden="1">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -2837,7 +2841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" hidden="1">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -2845,7 +2849,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" hidden="1">
       <c r="A66" t="s">
         <v>123</v>
       </c>
@@ -2853,7 +2857,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" hidden="1">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -2861,7 +2865,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -2869,7 +2873,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" hidden="1">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" hidden="1">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -2885,7 +2889,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" hidden="1">
       <c r="A71" t="s">
         <v>132</v>
       </c>
@@ -2893,7 +2897,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" hidden="1">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -2901,7 +2905,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" hidden="1">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -2909,7 +2913,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" hidden="1">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -2917,7 +2921,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" hidden="1">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -2925,7 +2929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" hidden="1">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -2933,7 +2937,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" hidden="1">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2941,7 +2945,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" hidden="1">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2949,7 +2953,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" hidden="1">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2957,7 +2961,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" hidden="1">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2965,7 +2969,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" hidden="1">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2973,7 +2977,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" hidden="1">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -2981,7 +2985,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" hidden="1">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -2989,7 +2993,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" hidden="1">
       <c r="A84" t="s">
         <v>155</v>
       </c>
@@ -2997,7 +3001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" hidden="1">
       <c r="A85" t="s">
         <v>156</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" hidden="1">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -3013,7 +3017,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" hidden="1">
       <c r="A87" t="s">
         <v>160</v>
       </c>
@@ -3021,7 +3025,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" hidden="1">
       <c r="A88" t="s">
         <v>162</v>
       </c>
@@ -3029,7 +3033,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" hidden="1">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -3037,7 +3041,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" hidden="1">
       <c r="A90" t="s">
         <v>165</v>
       </c>
@@ -3045,7 +3049,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" hidden="1">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -3053,7 +3057,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" hidden="1">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -3061,7 +3065,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" hidden="1">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -3069,7 +3073,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" hidden="1">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -3077,7 +3081,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" hidden="1">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -3085,7 +3089,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" hidden="1">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3093,7 +3097,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" hidden="1">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -3101,7 +3105,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" hidden="1">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -3109,7 +3113,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" hidden="1">
       <c r="A99" t="s">
         <v>183</v>
       </c>
@@ -3117,7 +3121,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" hidden="1">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -3125,7 +3129,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" hidden="1">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -3133,7 +3137,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" hidden="1">
       <c r="A102" t="s">
         <v>189</v>
       </c>
@@ -3141,7 +3145,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" hidden="1">
       <c r="A103" t="s">
         <v>191</v>
       </c>
@@ -3149,7 +3153,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" hidden="1">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -3157,7 +3161,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" hidden="1">
       <c r="A105" t="s">
         <v>195</v>
       </c>
@@ -3165,7 +3169,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" hidden="1">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -3174,7 +3178,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" hidden="1">
       <c r="A107" t="s">
         <v>197</v>
       </c>
@@ -3182,7 +3186,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" hidden="1">
       <c r="A108" t="s">
         <v>199</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" hidden="1">
       <c r="A109" t="s">
         <v>201</v>
       </c>
@@ -3198,7 +3202,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1">
       <c r="A110" t="s">
         <v>203</v>
       </c>
@@ -3206,7 +3210,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" hidden="1">
       <c r="A111" t="s">
         <v>205</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" hidden="1">
       <c r="A112" t="s">
         <v>207</v>
       </c>
@@ -3222,7 +3226,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" hidden="1">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -3230,7 +3234,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" hidden="1">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -3238,7 +3242,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" hidden="1">
       <c r="A115" t="s">
         <v>213</v>
       </c>
@@ -3246,7 +3250,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" hidden="1">
       <c r="A116" t="s">
         <v>215</v>
       </c>
@@ -3254,7 +3258,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" hidden="1">
       <c r="A117" t="s">
         <v>217</v>
       </c>
@@ -3262,7 +3266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" hidden="1">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3270,7 +3274,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" hidden="1">
       <c r="A119" t="s">
         <v>219</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" hidden="1">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -3286,7 +3290,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" hidden="1">
       <c r="A121" t="s">
         <v>223</v>
       </c>
@@ -3294,7 +3298,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" hidden="1">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -3302,7 +3306,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" hidden="1">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -3310,7 +3314,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" hidden="1">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -3318,7 +3322,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" hidden="1">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" hidden="1">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -3334,7 +3338,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" hidden="1">
       <c r="A127" t="s">
         <v>235</v>
       </c>
@@ -3342,7 +3346,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" hidden="1">
       <c r="A128" t="s">
         <v>236</v>
       </c>
@@ -3350,7 +3354,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="16.5">
+    <row r="129" spans="1:2" ht="16.5" hidden="1">
       <c r="A129" t="s">
         <v>237</v>
       </c>
@@ -3358,7 +3362,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" hidden="1">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -3366,7 +3370,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" hidden="1">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -3374,7 +3378,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" hidden="1">
       <c r="A132" t="s">
         <v>242</v>
       </c>
@@ -3382,7 +3386,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" hidden="1">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -3390,7 +3394,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" hidden="1">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -3398,7 +3402,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" hidden="1">
       <c r="A135" t="s">
         <v>247</v>
       </c>
@@ -3406,7 +3410,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" hidden="1">
       <c r="A136" t="s">
         <v>249</v>
       </c>
@@ -3414,7 +3418,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" hidden="1">
       <c r="A137" t="s">
         <v>251</v>
       </c>
@@ -3422,7 +3426,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" hidden="1">
       <c r="A138" t="s">
         <v>252</v>
       </c>
@@ -3430,7 +3434,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" hidden="1">
       <c r="A139" t="s">
         <v>254</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" hidden="1">
       <c r="A140" t="s">
         <v>255</v>
       </c>
@@ -3446,7 +3450,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" hidden="1">
       <c r="A141" t="s">
         <v>256</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" hidden="1">
       <c r="A142" t="s">
         <v>258</v>
       </c>
@@ -3462,7 +3466,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" hidden="1">
       <c r="A143" t="s">
         <v>259</v>
       </c>
@@ -3470,7 +3474,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" hidden="1">
       <c r="A144" t="s">
         <v>260</v>
       </c>
@@ -3478,7 +3482,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" hidden="1">
       <c r="A145" t="s">
         <v>262</v>
       </c>
@@ -3486,7 +3490,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" hidden="1">
       <c r="A146" t="s">
         <v>263</v>
       </c>
@@ -3494,7 +3498,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" hidden="1">
       <c r="A147" t="s">
         <v>264</v>
       </c>
@@ -3507,7 +3511,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" hidden="1">
       <c r="A149" t="s">
         <v>266</v>
       </c>
@@ -3515,7 +3519,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" hidden="1">
       <c r="A150" t="s">
         <v>268</v>
       </c>
@@ -3523,7 +3527,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" hidden="1">
       <c r="A151" t="s">
         <v>270</v>
       </c>
@@ -3531,7 +3535,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" hidden="1">
       <c r="A152" t="s">
         <v>272</v>
       </c>
@@ -3539,7 +3543,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" hidden="1">
       <c r="A153" t="s">
         <v>273</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" hidden="1">
       <c r="A154" t="s">
         <v>274</v>
       </c>
@@ -3555,7 +3559,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" hidden="1">
       <c r="A155" t="s">
         <v>275</v>
       </c>
@@ -3563,7 +3567,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" hidden="1">
       <c r="A156" t="s">
         <v>276</v>
       </c>
@@ -3571,7 +3575,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" hidden="1">
       <c r="A157" t="s">
         <v>277</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" hidden="1">
       <c r="A158" t="s">
         <v>278</v>
       </c>
@@ -3587,7 +3591,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" hidden="1">
       <c r="A159" t="s">
         <v>280</v>
       </c>
@@ -3595,7 +3599,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" hidden="1">
       <c r="A160" t="s">
         <v>282</v>
       </c>
@@ -3603,7 +3607,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" hidden="1">
       <c r="A161" t="s">
         <v>284</v>
       </c>
@@ -3611,7 +3615,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" hidden="1">
       <c r="A162" t="s">
         <v>286</v>
       </c>
@@ -3619,7 +3623,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" hidden="1">
       <c r="A163" s="4" t="s">
         <v>287</v>
       </c>
@@ -3627,7 +3631,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" hidden="1">
       <c r="A164" t="s">
         <v>289</v>
       </c>
@@ -3635,7 +3639,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" hidden="1">
       <c r="A165" t="s">
         <v>291</v>
       </c>
@@ -3643,7 +3647,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" hidden="1">
       <c r="A166" t="s">
         <v>292</v>
       </c>
@@ -3651,7 +3655,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" hidden="1">
       <c r="A167" t="s">
         <v>294</v>
       </c>
@@ -3659,7 +3663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" hidden="1">
       <c r="A168" t="s">
         <v>295</v>
       </c>
@@ -3667,7 +3671,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" hidden="1">
       <c r="A169" t="s">
         <v>296</v>
       </c>
@@ -3675,7 +3679,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" hidden="1">
       <c r="A170" t="s">
         <v>298</v>
       </c>
@@ -3683,7 +3687,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" hidden="1">
       <c r="A171" t="s">
         <v>300</v>
       </c>
@@ -3691,7 +3695,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" hidden="1">
       <c r="A172" t="s">
         <v>302</v>
       </c>
@@ -3699,7 +3703,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" hidden="1">
       <c r="A173" t="s">
         <v>303</v>
       </c>
@@ -3707,7 +3711,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" hidden="1">
       <c r="A174" t="s">
         <v>305</v>
       </c>
@@ -3715,7 +3719,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" hidden="1">
       <c r="A175" t="s">
         <v>307</v>
       </c>
@@ -3723,7 +3727,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" hidden="1">
       <c r="A176" t="s">
         <v>309</v>
       </c>
@@ -3731,7 +3735,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" hidden="1">
       <c r="A177" t="s">
         <v>311</v>
       </c>
@@ -3739,7 +3743,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" hidden="1">
       <c r="A178" t="s">
         <v>313</v>
       </c>
@@ -3747,7 +3751,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" hidden="1">
       <c r="A179" t="s">
         <v>314</v>
       </c>
@@ -3755,7 +3759,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" hidden="1">
       <c r="A180" t="s">
         <v>316</v>
       </c>
@@ -3768,7 +3772,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" hidden="1">
       <c r="A182" t="s">
         <v>319</v>
       </c>
@@ -3776,7 +3780,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" hidden="1">
       <c r="A183" t="s">
         <v>321</v>
       </c>
@@ -3784,7 +3788,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" hidden="1">
       <c r="A184" t="s">
         <v>323</v>
       </c>
@@ -3792,7 +3796,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" hidden="1">
       <c r="A185" t="s">
         <v>325</v>
       </c>
@@ -3800,7 +3804,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" hidden="1">
       <c r="A186" t="s">
         <v>327</v>
       </c>
@@ -3808,7 +3812,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" hidden="1">
       <c r="A187" t="s">
         <v>328</v>
       </c>
@@ -3816,7 +3820,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" hidden="1">
       <c r="A188" t="s">
         <v>329</v>
       </c>
@@ -3824,7 +3828,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" hidden="1">
       <c r="A189" t="s">
         <v>331</v>
       </c>
@@ -3832,7 +3836,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" hidden="1">
       <c r="A190" t="s">
         <v>333</v>
       </c>
@@ -3840,7 +3844,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" hidden="1">
       <c r="A191" t="s">
         <v>335</v>
       </c>
@@ -3848,7 +3852,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" hidden="1">
       <c r="A192" t="s">
         <v>336</v>
       </c>
@@ -3856,7 +3860,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" hidden="1">
       <c r="A193" t="s">
         <v>337</v>
       </c>
@@ -3864,7 +3868,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" hidden="1">
       <c r="A194" t="s">
         <v>339</v>
       </c>
@@ -3872,7 +3876,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" hidden="1">
       <c r="A195" t="s">
         <v>341</v>
       </c>
@@ -3880,7 +3884,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" hidden="1">
       <c r="A196" t="s">
         <v>343</v>
       </c>
@@ -3888,7 +3892,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" hidden="1">
       <c r="A197" t="s">
         <v>345</v>
       </c>
@@ -3896,7 +3900,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5">
+    <row r="198" spans="1:2" ht="16.5" hidden="1">
       <c r="A198" t="s">
         <v>347</v>
       </c>
@@ -3904,7 +3908,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" hidden="1">
       <c r="A199" t="s">
         <v>349</v>
       </c>
@@ -3912,7 +3916,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" hidden="1">
       <c r="A200" t="s">
         <v>351</v>
       </c>
@@ -3920,7 +3924,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" hidden="1">
       <c r="A201" t="s">
         <v>353</v>
       </c>
@@ -3928,7 +3932,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" hidden="1">
       <c r="A202" t="s">
         <v>355</v>
       </c>
@@ -3936,7 +3940,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" hidden="1">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -3944,7 +3948,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" hidden="1">
       <c r="A204" t="s">
         <v>359</v>
       </c>
@@ -3952,7 +3956,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" hidden="1">
       <c r="A205" t="s">
         <v>361</v>
       </c>
@@ -3960,7 +3964,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" hidden="1">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -3968,7 +3972,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" hidden="1">
       <c r="A207" t="s">
         <v>364</v>
       </c>
@@ -3976,7 +3980,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" hidden="1">
       <c r="A208" t="s">
         <v>555</v>
       </c>
@@ -3984,7 +3988,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" hidden="1">
       <c r="A209" t="s">
         <v>366</v>
       </c>
@@ -3992,7 +3996,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" hidden="1">
       <c r="A210" t="s">
         <v>368</v>
       </c>
@@ -4000,7 +4004,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" hidden="1">
       <c r="A211" t="s">
         <v>370</v>
       </c>
@@ -4008,7 +4012,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" hidden="1">
       <c r="A212" t="s">
         <v>372</v>
       </c>
@@ -4016,7 +4020,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" hidden="1">
       <c r="A213" t="s">
         <v>374</v>
       </c>
@@ -4024,7 +4028,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" hidden="1">
       <c r="A214" t="s">
         <v>376</v>
       </c>
@@ -4032,7 +4036,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" hidden="1">
       <c r="A215" t="s">
         <v>378</v>
       </c>
@@ -4040,7 +4044,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" hidden="1">
       <c r="A216" t="s">
         <v>379</v>
       </c>
@@ -4048,7 +4052,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" hidden="1">
       <c r="A217" t="s">
         <v>381</v>
       </c>
@@ -4060,9 +4064,11 @@
       <c r="A218" t="s">
         <v>383</v>
       </c>
-      <c r="B218" s="13"/>
-    </row>
-    <row r="219" spans="1:2">
+      <c r="B218" s="12" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" hidden="1">
       <c r="A219" t="s">
         <v>385</v>
       </c>
@@ -4070,7 +4076,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" hidden="1">
       <c r="A220" t="s">
         <v>386</v>
       </c>
@@ -4078,7 +4084,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" hidden="1">
       <c r="A221" t="s">
         <v>387</v>
       </c>
@@ -4086,7 +4092,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" hidden="1">
       <c r="A222" t="s">
         <v>389</v>
       </c>
@@ -4094,7 +4100,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" hidden="1">
       <c r="A223" t="s">
         <v>391</v>
       </c>
@@ -4102,7 +4108,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" hidden="1">
       <c r="A224" t="s">
         <v>393</v>
       </c>
@@ -4110,7 +4116,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" hidden="1">
       <c r="A225" t="s">
         <v>395</v>
       </c>
@@ -4118,7 +4124,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" hidden="1">
       <c r="A226" t="s">
         <v>397</v>
       </c>
@@ -4126,7 +4132,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" hidden="1">
       <c r="A227" t="s">
         <v>399</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" hidden="1">
       <c r="A228" t="s">
         <v>401</v>
       </c>
@@ -4142,7 +4148,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" hidden="1">
       <c r="A229" t="s">
         <v>403</v>
       </c>
@@ -4150,7 +4156,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" hidden="1">
       <c r="A230" t="s">
         <v>405</v>
       </c>
@@ -4158,7 +4164,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" hidden="1">
       <c r="A231" t="s">
         <v>407</v>
       </c>
@@ -4166,7 +4172,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" hidden="1">
       <c r="A232" t="s">
         <v>408</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" hidden="1">
       <c r="A233" t="s">
         <v>410</v>
       </c>
@@ -4182,7 +4188,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" hidden="1">
       <c r="A234" t="s">
         <v>411</v>
       </c>
@@ -4190,7 +4196,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" hidden="1">
       <c r="A235" t="s">
         <v>413</v>
       </c>
@@ -4198,7 +4204,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" hidden="1">
       <c r="A236" t="s">
         <v>414</v>
       </c>
@@ -4206,7 +4212,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" hidden="1">
       <c r="A237" t="s">
         <v>416</v>
       </c>
@@ -4214,7 +4220,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" hidden="1">
       <c r="A238" t="s">
         <v>418</v>
       </c>
@@ -4222,7 +4228,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" hidden="1">
       <c r="A239" t="s">
         <v>420</v>
       </c>
@@ -4235,7 +4241,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" hidden="1">
       <c r="A241" t="s">
         <v>423</v>
       </c>
@@ -4243,7 +4249,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" hidden="1">
       <c r="A242" t="s">
         <v>425</v>
       </c>
@@ -4251,7 +4257,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16.5">
+    <row r="243" spans="1:2" ht="16.5" hidden="1">
       <c r="A243" t="s">
         <v>427</v>
       </c>
@@ -4259,7 +4265,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" hidden="1">
       <c r="A244" t="s">
         <v>428</v>
       </c>
@@ -4267,7 +4273,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" hidden="1">
       <c r="A245" t="s">
         <v>430</v>
       </c>
@@ -4275,7 +4281,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" hidden="1">
       <c r="A246" t="s">
         <v>432</v>
       </c>
@@ -4283,7 +4289,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" hidden="1">
       <c r="A247" t="s">
         <v>434</v>
       </c>
@@ -4296,7 +4302,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" hidden="1">
       <c r="A249" t="s">
         <v>436</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" hidden="1">
       <c r="A250" t="s">
         <v>438</v>
       </c>
@@ -4312,7 +4318,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" hidden="1">
       <c r="A251" t="s">
         <v>440</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" hidden="1">
       <c r="A253" t="s">
         <v>443</v>
       </c>
@@ -4333,7 +4339,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" hidden="1">
       <c r="A254" t="s">
         <v>445</v>
       </c>
@@ -4341,7 +4347,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" hidden="1">
       <c r="A255" t="s">
         <v>446</v>
       </c>
@@ -4349,7 +4355,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" hidden="1">
       <c r="A256" t="s">
         <v>447</v>
       </c>
@@ -4357,12 +4363,15 @@
         <v>238</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" ht="16.5">
       <c r="A257" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="258" spans="1:2">
+      <c r="B257" s="12" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" hidden="1">
       <c r="A258" t="s">
         <v>449</v>
       </c>
@@ -4370,7 +4379,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" hidden="1">
       <c r="A259" t="s">
         <v>450</v>
       </c>
@@ -4378,7 +4387,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" hidden="1">
       <c r="A260" t="s">
         <v>451</v>
       </c>
@@ -4386,7 +4395,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" hidden="1">
       <c r="A261" t="s">
         <v>453</v>
       </c>
@@ -4394,7 +4403,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" hidden="1">
       <c r="A262" t="s">
         <v>455</v>
       </c>
@@ -4402,7 +4411,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" hidden="1">
       <c r="A263" t="s">
         <v>457</v>
       </c>
@@ -4410,7 +4419,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" hidden="1">
       <c r="A264" t="s">
         <v>458</v>
       </c>
@@ -4418,7 +4427,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" hidden="1">
       <c r="A265" t="s">
         <v>460</v>
       </c>
@@ -4426,7 +4435,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" hidden="1">
       <c r="A266" t="s">
         <v>462</v>
       </c>
@@ -4434,7 +4443,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" hidden="1">
       <c r="A267" t="s">
         <v>464</v>
       </c>
@@ -4442,7 +4451,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" hidden="1">
       <c r="A268" t="s">
         <v>465</v>
       </c>
@@ -4450,7 +4459,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" hidden="1">
       <c r="A269" t="s">
         <v>466</v>
       </c>
@@ -4468,7 +4477,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" hidden="1">
       <c r="A272" t="s">
         <v>470</v>
       </c>
@@ -4481,7 +4490,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" hidden="1">
       <c r="A274" t="s">
         <v>472</v>
       </c>
@@ -4489,7 +4498,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" hidden="1">
       <c r="A275" t="s">
         <v>474</v>
       </c>
@@ -4502,7 +4511,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" hidden="1">
       <c r="A277" t="s">
         <v>476</v>
       </c>
@@ -4510,7 +4519,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" hidden="1">
       <c r="A278" t="s">
         <v>478</v>
       </c>
@@ -4518,7 +4527,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" hidden="1">
       <c r="A279" t="s">
         <v>480</v>
       </c>
@@ -4526,7 +4535,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" hidden="1">
       <c r="A280" t="s">
         <v>481</v>
       </c>
@@ -4534,7 +4543,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" hidden="1">
       <c r="A281" t="s">
         <v>482</v>
       </c>
@@ -4542,7 +4551,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" hidden="1">
       <c r="A282" t="s">
         <v>484</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" hidden="1">
       <c r="A283" t="s">
         <v>485</v>
       </c>
@@ -4558,7 +4567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" hidden="1">
       <c r="A284" t="s">
         <v>486</v>
       </c>
@@ -4566,7 +4575,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" hidden="1">
       <c r="A285" t="s">
         <v>487</v>
       </c>
@@ -4574,7 +4583,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" hidden="1">
       <c r="A286" t="s">
         <v>488</v>
       </c>
@@ -4582,7 +4591,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" hidden="1">
       <c r="A287" t="s">
         <v>489</v>
       </c>
@@ -4590,7 +4599,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" hidden="1">
       <c r="A288" t="s">
         <v>490</v>
       </c>
@@ -4598,7 +4607,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="16.5">
+    <row r="289" spans="1:2" ht="16.5" hidden="1">
       <c r="A289" t="s">
         <v>491</v>
       </c>
@@ -4606,7 +4615,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" hidden="1">
       <c r="A290" t="s">
         <v>492</v>
       </c>
@@ -4614,7 +4623,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" hidden="1">
       <c r="A291" t="s">
         <v>494</v>
       </c>
@@ -4622,7 +4631,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" hidden="1">
       <c r="A292" t="s">
         <v>495</v>
       </c>
@@ -4630,7 +4639,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" hidden="1">
       <c r="A293" t="s">
         <v>496</v>
       </c>
@@ -4638,7 +4647,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" hidden="1">
       <c r="A294" t="s">
         <v>497</v>
       </c>
@@ -4646,7 +4655,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" hidden="1">
       <c r="A295" t="s">
         <v>498</v>
       </c>
@@ -4654,7 +4663,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" hidden="1">
       <c r="A296" t="s">
         <v>499</v>
       </c>
@@ -4662,7 +4671,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" hidden="1">
       <c r="A297" t="s">
         <v>500</v>
       </c>
@@ -4670,7 +4679,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" hidden="1">
       <c r="A298" t="s">
         <v>501</v>
       </c>
@@ -4678,7 +4687,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" hidden="1">
       <c r="A299" t="s">
         <v>502</v>
       </c>
@@ -4686,7 +4695,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" hidden="1">
       <c r="A300" t="s">
         <v>503</v>
       </c>
@@ -4694,7 +4703,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" hidden="1">
       <c r="A301" t="s">
         <v>505</v>
       </c>
@@ -4702,7 +4711,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" hidden="1">
       <c r="A302" t="s">
         <v>506</v>
       </c>
@@ -4715,7 +4724,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" hidden="1">
       <c r="A304" t="s">
         <v>508</v>
       </c>
@@ -4723,7 +4732,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:5" hidden="1">
       <c r="A305" t="s">
         <v>509</v>
       </c>
@@ -4731,7 +4740,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="306" spans="1:5">
+    <row r="306" spans="1:5" hidden="1">
       <c r="A306" t="s">
         <v>510</v>
       </c>
@@ -4742,7 +4751,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="307" spans="1:5">
+    <row r="307" spans="1:5" hidden="1">
       <c r="A307" t="s">
         <v>511</v>
       </c>
@@ -4750,7 +4759,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:5" hidden="1">
       <c r="A308" t="s">
         <v>512</v>
       </c>
@@ -4758,7 +4767,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:5">
+    <row r="309" spans="1:5" hidden="1">
       <c r="A309" t="s">
         <v>513</v>
       </c>
@@ -4766,7 +4775,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="310" spans="1:5">
+    <row r="310" spans="1:5" hidden="1">
       <c r="A310" t="s">
         <v>514</v>
       </c>
@@ -4774,7 +4783,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="311" spans="1:5">
+    <row r="311" spans="1:5" hidden="1">
       <c r="A311" t="s">
         <v>516</v>
       </c>
@@ -4782,7 +4791,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="312" spans="1:5">
+    <row r="312" spans="1:5" hidden="1">
       <c r="A312" t="s">
         <v>517</v>
       </c>
@@ -4790,7 +4799,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="313" spans="1:5">
+    <row r="313" spans="1:5" hidden="1">
       <c r="A313" t="s">
         <v>518</v>
       </c>
@@ -4798,7 +4807,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="314" spans="1:5">
+    <row r="314" spans="1:5" hidden="1">
       <c r="A314" t="s">
         <v>519</v>
       </c>
@@ -4806,7 +4815,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="315" spans="1:5">
+    <row r="315" spans="1:5" hidden="1">
       <c r="A315" t="s">
         <v>520</v>
       </c>
@@ -4819,7 +4828,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="317" spans="1:5">
+    <row r="317" spans="1:5" hidden="1">
       <c r="A317" t="s">
         <v>522</v>
       </c>
@@ -4827,7 +4836,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="318" spans="1:5">
+    <row r="318" spans="1:5" hidden="1">
       <c r="A318" t="s">
         <v>523</v>
       </c>
@@ -4835,7 +4844,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="319" spans="1:5">
+    <row r="319" spans="1:5" hidden="1">
       <c r="A319" t="s">
         <v>525</v>
       </c>
@@ -4843,7 +4852,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="16.5">
+    <row r="320" spans="1:5" ht="16.5" hidden="1">
       <c r="A320" t="s">
         <v>526</v>
       </c>
@@ -4851,7 +4860,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" hidden="1">
       <c r="A321" t="s">
         <v>527</v>
       </c>
@@ -4859,7 +4868,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" hidden="1">
       <c r="A322" t="s">
         <v>528</v>
       </c>
@@ -4867,7 +4876,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" hidden="1">
       <c r="A323" t="s">
         <v>529</v>
       </c>
@@ -4875,7 +4884,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" hidden="1">
       <c r="A324" t="s">
         <v>531</v>
       </c>
@@ -4883,7 +4892,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" hidden="1">
       <c r="A325" t="s">
         <v>532</v>
       </c>
@@ -4891,7 +4900,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" hidden="1">
       <c r="A326" t="s">
         <v>533</v>
       </c>
@@ -4904,7 +4913,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" hidden="1">
       <c r="A328" t="s">
         <v>534</v>
       </c>
@@ -4912,7 +4921,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" hidden="1">
       <c r="A329" t="s">
         <v>535</v>
       </c>
@@ -4920,7 +4929,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" hidden="1">
       <c r="A330" s="4" t="s">
         <v>536</v>
       </c>
@@ -4928,7 +4937,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" hidden="1">
       <c r="A331" s="4" t="s">
         <v>538</v>
       </c>
@@ -4936,7 +4945,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" hidden="1">
       <c r="A332" s="4" t="s">
         <v>539</v>
       </c>
@@ -4944,7 +4953,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" hidden="1">
       <c r="A333" t="s">
         <v>540</v>
       </c>
@@ -4952,7 +4961,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" hidden="1">
       <c r="A334" t="s">
         <v>541</v>
       </c>
@@ -4960,7 +4969,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="335" spans="1:2">
+    <row r="335" spans="1:2" hidden="1">
       <c r="A335" t="s">
         <v>542</v>
       </c>
@@ -4968,7 +4977,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="336" spans="1:2">
+    <row r="336" spans="1:2" hidden="1">
       <c r="A336" t="s">
         <v>543</v>
       </c>
@@ -4976,7 +4985,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1">
       <c r="A337" t="s">
         <v>545</v>
       </c>
@@ -4984,7 +4993,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" hidden="1">
       <c r="A338" t="s">
         <v>547</v>
       </c>
@@ -4992,7 +5001,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" t="s">
         <v>549</v>
       </c>
@@ -5000,7 +5009,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" t="s">
         <v>551</v>
       </c>
@@ -5008,7 +5017,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" t="s">
         <v>553</v>
       </c>
@@ -5016,7 +5025,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" t="s">
         <v>577</v>
       </c>
@@ -5024,7 +5033,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" t="s">
         <v>572</v>
       </c>
@@ -5032,7 +5041,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" t="s">
         <v>576</v>
       </c>
@@ -5040,7 +5049,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" t="s">
         <v>573</v>
       </c>
@@ -5048,7 +5057,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1">
       <c r="A346" t="s">
         <v>574</v>
       </c>
@@ -5056,7 +5065,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1">
       <c r="A347" t="s">
         <v>575</v>
       </c>
@@ -5064,7 +5073,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1">
       <c r="A348" t="s">
         <v>578</v>
       </c>
@@ -5072,7 +5081,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1">
       <c r="A349" t="s">
         <v>579</v>
       </c>
@@ -5080,7 +5089,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="17.25">
+    <row r="350" spans="1:7" ht="17.25" hidden="1">
       <c r="A350" t="s">
         <v>580</v>
       </c>
@@ -5092,7 +5101,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1">
       <c r="A351" t="s">
         <v>581</v>
       </c>
@@ -5113,7 +5122,7 @@
       <c r="F352" s="7"/>
       <c r="G352" s="7"/>
     </row>
-    <row r="353" spans="1:7">
+    <row r="353" spans="1:7" hidden="1">
       <c r="A353" t="s">
         <v>583</v>
       </c>
@@ -5124,7 +5133,7 @@
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7">
+    <row r="354" spans="1:7" hidden="1">
       <c r="A354" t="s">
         <v>584</v>
       </c>
@@ -5135,7 +5144,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7">
+    <row r="355" spans="1:7" hidden="1">
       <c r="A355" t="s">
         <v>585</v>
       </c>
@@ -5146,7 +5155,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5">
+    <row r="356" spans="1:7" ht="19.5" hidden="1">
       <c r="A356" t="s">
         <v>586</v>
       </c>
@@ -5158,7 +5167,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1">
       <c r="A357" t="s">
         <v>587</v>
       </c>
@@ -5170,7 +5179,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1">
       <c r="A358" t="s">
         <v>588</v>
       </c>
@@ -5181,7 +5190,7 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1">
       <c r="A359" t="s">
         <v>589</v>
       </c>
@@ -5200,7 +5209,7 @@
       <c r="F360" s="7"/>
       <c r="G360" s="7"/>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" hidden="1">
       <c r="A361" t="s">
         <v>592</v>
       </c>
@@ -5257,7 +5266,11 @@
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362"/>
+  <autoFilter ref="A1:H362">
+    <filterColumn colId="1">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5467,18 +5480,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5501,18 +5514,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Themen fuer @schooschef vergeben
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="616">
   <si>
     <t>Themen</t>
   </si>
@@ -1867,6 +1867,9 @@
   </si>
   <si>
     <t>ga88maby</t>
+  </si>
+  <si>
+    <t>schooschef</t>
   </si>
 </sst>
 </file>
@@ -2318,7 +2321,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B362" sqref="B362"/>
+      <selection activeCell="B352" sqref="B352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4835,9 +4838,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="316" spans="1:5">
+    <row r="316" spans="1:5" ht="16.5">
       <c r="A316" t="s">
         <v>521</v>
+      </c>
+      <c r="B316" s="13" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="317" spans="1:5" hidden="1">
@@ -4920,9 +4926,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" ht="16.5">
       <c r="A327" t="s">
         <v>554</v>
+      </c>
+      <c r="B327" s="13" t="s">
+        <v>615</v>
       </c>
     </row>
     <row r="328" spans="1:2" hidden="1">
@@ -5495,18 +5504,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5529,18 +5538,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Zweites Thema fuer @julianTR4 zugeordnet
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="616">
   <si>
     <t>Themen</t>
   </si>
@@ -2321,7 +2321,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B352" sqref="B352"/>
+      <selection activeCell="B349" sqref="B349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2566,7 +2566,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" hidden="1">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" hidden="1">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" hidden="1">
       <c r="A181" t="s">
         <v>318</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" hidden="1">
       <c r="A248" t="s">
         <v>435</v>
       </c>
@@ -4345,6 +4345,9 @@
       <c r="A252" t="s">
         <v>442</v>
       </c>
+      <c r="B252" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="253" spans="1:2" hidden="1">
       <c r="A253" t="s">
@@ -4482,12 +4485,12 @@
         <v>467</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" hidden="1">
       <c r="A270" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" hidden="1">
       <c r="A271" t="s">
         <v>469</v>
       </c>
@@ -4500,7 +4503,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" hidden="1">
       <c r="A273" t="s">
         <v>471</v>
       </c>
@@ -4521,7 +4524,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" hidden="1">
       <c r="A276" t="s">
         <v>475</v>
       </c>
@@ -4734,7 +4737,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" hidden="1">
       <c r="A303" t="s">
         <v>507</v>
       </c>
@@ -4838,7 +4841,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="16.5">
+    <row r="316" spans="1:5" ht="16.5" hidden="1">
       <c r="A316" t="s">
         <v>521</v>
       </c>
@@ -4926,7 +4929,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16.5">
+    <row r="327" spans="1:2" ht="16.5" hidden="1">
       <c r="A327" t="s">
         <v>554</v>
       </c>
@@ -5102,11 +5105,11 @@
         <v>560</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1">
+    <row r="349" spans="1:7">
       <c r="A349" t="s">
         <v>579</v>
       </c>
-      <c r="B349" s="7" t="s">
+      <c r="B349" t="s">
         <v>561</v>
       </c>
     </row>
@@ -5134,7 +5137,7 @@
       <c r="F351" s="7"/>
       <c r="G351" s="7"/>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" hidden="1">
       <c r="A352" t="s">
         <v>582</v>
       </c>
@@ -5222,7 +5225,7 @@
       <c r="F359" s="7"/>
       <c r="G359" s="7"/>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" hidden="1">
       <c r="A360" t="s">
         <v>590</v>
       </c>
@@ -5244,7 +5247,7 @@
       <c r="F361" s="7"/>
       <c r="G361" s="7"/>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" hidden="1">
       <c r="A362" t="s">
         <v>591</v>
       </c>
@@ -5292,7 +5295,9 @@
   </sheetData>
   <autoFilter ref="A1:H362">
     <filterColumn colId="1">
-      <filters blank="1"/>
+      <filters>
+        <filter val="julianTR4"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5504,18 +5509,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5538,18 +5543,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update jonaskarg187 pamerkl flxrbnk NinaNagel Tjara1
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0AEF53-44D2-47A3-9773-1AE996DF461B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="616">
   <si>
     <t>Themen</t>
   </si>
@@ -1875,8 +1876,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2316,24 +2317,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B349" sqref="B349"/>
+      <selection activeCell="C364" sqref="C364"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="83.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2349,7 +2350,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2374,7 +2375,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2422,7 +2423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2430,7 +2431,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2470,7 +2471,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2566,12 +2567,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2579,7 +2580,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -2587,7 +2588,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2595,7 +2596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2603,7 +2604,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -2619,7 +2620,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2635,12 +2636,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2656,7 +2657,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -2672,7 +2673,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -2681,7 +2682,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2690,7 +2691,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2706,7 +2707,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>90</v>
       </c>
@@ -2722,7 +2723,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -2730,7 +2731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -2738,7 +2739,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2746,7 +2747,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -2770,15 +2771,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>103</v>
       </c>
-      <c r="B55" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" hidden="1">
+    </row>
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2786,7 +2784,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2794,7 +2792,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2802,7 +2800,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2810,7 +2808,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2818,7 +2816,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -2826,7 +2824,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -2834,7 +2832,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -2842,7 +2840,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -2850,7 +2848,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -2858,7 +2856,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>123</v>
       </c>
@@ -2866,7 +2864,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>124</v>
       </c>
@@ -2874,7 +2872,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>126</v>
       </c>
@@ -2882,7 +2880,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>128</v>
       </c>
@@ -2890,7 +2888,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>130</v>
       </c>
@@ -2898,7 +2896,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>132</v>
       </c>
@@ -2906,7 +2904,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -2914,7 +2912,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -2922,7 +2920,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -2930,7 +2928,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -2938,7 +2936,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -2946,7 +2944,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>142</v>
       </c>
@@ -2954,7 +2952,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>143</v>
       </c>
@@ -2962,7 +2960,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>145</v>
       </c>
@@ -2970,7 +2968,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>147</v>
       </c>
@@ -2978,7 +2976,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -2986,7 +2984,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>151</v>
       </c>
@@ -2994,7 +2992,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>153</v>
       </c>
@@ -3002,15 +3000,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>155</v>
       </c>
-      <c r="B84" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" hidden="1">
+    </row>
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>156</v>
       </c>
@@ -3018,7 +3013,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -3026,7 +3021,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>160</v>
       </c>
@@ -3034,7 +3029,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>162</v>
       </c>
@@ -3042,7 +3037,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -3050,7 +3045,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>165</v>
       </c>
@@ -3058,7 +3053,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>167</v>
       </c>
@@ -3066,7 +3061,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>169</v>
       </c>
@@ -3074,7 +3069,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -3082,7 +3077,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>173</v>
       </c>
@@ -3090,7 +3085,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -3098,7 +3093,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3106,7 +3101,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>179</v>
       </c>
@@ -3114,7 +3109,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>181</v>
       </c>
@@ -3122,7 +3117,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>183</v>
       </c>
@@ -3130,7 +3125,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>185</v>
       </c>
@@ -3138,7 +3133,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -3146,7 +3141,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>189</v>
       </c>
@@ -3154,7 +3149,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>191</v>
       </c>
@@ -3162,7 +3157,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -3170,7 +3165,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>195</v>
       </c>
@@ -3178,7 +3173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -3187,7 +3182,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" hidden="1">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>197</v>
       </c>
@@ -3195,7 +3190,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>199</v>
       </c>
@@ -3203,7 +3198,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>201</v>
       </c>
@@ -3211,7 +3206,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>203</v>
       </c>
@@ -3219,7 +3214,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>205</v>
       </c>
@@ -3227,7 +3222,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>207</v>
       </c>
@@ -3235,7 +3230,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>209</v>
       </c>
@@ -3243,7 +3238,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>211</v>
       </c>
@@ -3251,7 +3246,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>213</v>
       </c>
@@ -3259,7 +3254,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>215</v>
       </c>
@@ -3267,7 +3262,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>217</v>
       </c>
@@ -3275,7 +3270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3283,7 +3278,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>219</v>
       </c>
@@ -3291,7 +3286,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>221</v>
       </c>
@@ -3299,7 +3294,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>223</v>
       </c>
@@ -3307,7 +3302,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -3315,7 +3310,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -3323,7 +3318,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -3331,7 +3326,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -3339,7 +3334,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -3347,7 +3342,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>235</v>
       </c>
@@ -3355,7 +3350,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>236</v>
       </c>
@@ -3363,7 +3358,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="16.5" hidden="1">
+    <row r="129" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>237</v>
       </c>
@@ -3371,7 +3366,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -3379,7 +3374,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -3387,7 +3382,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>242</v>
       </c>
@@ -3395,7 +3390,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -3403,7 +3398,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>245</v>
       </c>
@@ -3411,7 +3406,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>247</v>
       </c>
@@ -3419,7 +3414,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>249</v>
       </c>
@@ -3427,7 +3422,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>251</v>
       </c>
@@ -3435,7 +3430,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>252</v>
       </c>
@@ -3443,7 +3438,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>254</v>
       </c>
@@ -3451,7 +3446,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>255</v>
       </c>
@@ -3459,7 +3454,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>256</v>
       </c>
@@ -3467,7 +3462,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>258</v>
       </c>
@@ -3475,7 +3470,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>259</v>
       </c>
@@ -3483,7 +3478,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>260</v>
       </c>
@@ -3491,7 +3486,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>262</v>
       </c>
@@ -3499,7 +3494,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>263</v>
       </c>
@@ -3507,7 +3502,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>264</v>
       </c>
@@ -3515,7 +3510,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>265</v>
       </c>
@@ -3523,7 +3518,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>266</v>
       </c>
@@ -3531,7 +3526,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>268</v>
       </c>
@@ -3539,7 +3534,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>270</v>
       </c>
@@ -3547,7 +3542,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>272</v>
       </c>
@@ -3555,7 +3550,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>273</v>
       </c>
@@ -3563,7 +3558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>274</v>
       </c>
@@ -3571,7 +3566,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>275</v>
       </c>
@@ -3579,7 +3574,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>276</v>
       </c>
@@ -3587,7 +3582,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>277</v>
       </c>
@@ -3595,7 +3590,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>278</v>
       </c>
@@ -3603,7 +3598,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>280</v>
       </c>
@@ -3611,7 +3606,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>282</v>
       </c>
@@ -3619,7 +3614,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>284</v>
       </c>
@@ -3627,7 +3622,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>286</v>
       </c>
@@ -3635,7 +3630,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>287</v>
       </c>
@@ -3643,7 +3638,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>289</v>
       </c>
@@ -3651,7 +3646,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>291</v>
       </c>
@@ -3659,7 +3654,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>292</v>
       </c>
@@ -3667,7 +3662,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>294</v>
       </c>
@@ -3675,7 +3670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>295</v>
       </c>
@@ -3683,7 +3678,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>296</v>
       </c>
@@ -3691,7 +3686,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>298</v>
       </c>
@@ -3699,7 +3694,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>300</v>
       </c>
@@ -3707,7 +3702,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>302</v>
       </c>
@@ -3715,7 +3710,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>303</v>
       </c>
@@ -3723,7 +3718,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>305</v>
       </c>
@@ -3731,7 +3726,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>307</v>
       </c>
@@ -3739,7 +3734,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>309</v>
       </c>
@@ -3747,7 +3742,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>311</v>
       </c>
@@ -3755,7 +3750,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>313</v>
       </c>
@@ -3763,7 +3758,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>314</v>
       </c>
@@ -3771,7 +3766,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>316</v>
       </c>
@@ -3779,12 +3774,12 @@
         <v>317</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>319</v>
       </c>
@@ -3792,7 +3787,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>321</v>
       </c>
@@ -3800,7 +3795,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>323</v>
       </c>
@@ -3808,7 +3803,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>325</v>
       </c>
@@ -3816,7 +3811,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>327</v>
       </c>
@@ -3824,7 +3819,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>328</v>
       </c>
@@ -3832,7 +3827,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>329</v>
       </c>
@@ -3840,7 +3835,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>331</v>
       </c>
@@ -3848,7 +3843,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>333</v>
       </c>
@@ -3856,7 +3851,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>335</v>
       </c>
@@ -3864,7 +3859,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>336</v>
       </c>
@@ -3872,7 +3867,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>337</v>
       </c>
@@ -3880,7 +3875,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>339</v>
       </c>
@@ -3888,7 +3883,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>341</v>
       </c>
@@ -3896,7 +3891,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>343</v>
       </c>
@@ -3904,7 +3899,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>345</v>
       </c>
@@ -3912,7 +3907,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5" hidden="1">
+    <row r="198" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
         <v>347</v>
       </c>
@@ -3920,7 +3915,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>349</v>
       </c>
@@ -3928,7 +3923,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>351</v>
       </c>
@@ -3936,7 +3931,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>353</v>
       </c>
@@ -3944,7 +3939,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>355</v>
       </c>
@@ -3952,7 +3947,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>357</v>
       </c>
@@ -3960,7 +3955,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>359</v>
       </c>
@@ -3968,7 +3963,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>361</v>
       </c>
@@ -3976,7 +3971,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>362</v>
       </c>
@@ -3984,7 +3979,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>364</v>
       </c>
@@ -3992,7 +3987,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>555</v>
       </c>
@@ -4000,7 +3995,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>366</v>
       </c>
@@ -4008,7 +4003,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>368</v>
       </c>
@@ -4016,7 +4011,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>370</v>
       </c>
@@ -4024,7 +4019,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>372</v>
       </c>
@@ -4032,7 +4027,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>374</v>
       </c>
@@ -4040,7 +4035,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>376</v>
       </c>
@@ -4048,7 +4043,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>378</v>
       </c>
@@ -4056,7 +4051,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>379</v>
       </c>
@@ -4064,7 +4059,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>381</v>
       </c>
@@ -4072,7 +4067,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="16.5" hidden="1">
+    <row r="218" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>383</v>
       </c>
@@ -4080,7 +4075,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>385</v>
       </c>
@@ -4088,7 +4083,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>386</v>
       </c>
@@ -4096,7 +4091,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>387</v>
       </c>
@@ -4104,7 +4099,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>389</v>
       </c>
@@ -4112,7 +4107,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>391</v>
       </c>
@@ -4120,7 +4115,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>393</v>
       </c>
@@ -4128,7 +4123,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>395</v>
       </c>
@@ -4136,7 +4131,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>397</v>
       </c>
@@ -4144,7 +4139,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>399</v>
       </c>
@@ -4152,7 +4147,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>401</v>
       </c>
@@ -4160,7 +4155,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>403</v>
       </c>
@@ -4168,7 +4163,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>405</v>
       </c>
@@ -4176,7 +4171,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>407</v>
       </c>
@@ -4184,7 +4179,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>408</v>
       </c>
@@ -4192,7 +4187,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>410</v>
       </c>
@@ -4200,7 +4195,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>411</v>
       </c>
@@ -4208,7 +4203,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>413</v>
       </c>
@@ -4216,7 +4211,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>414</v>
       </c>
@@ -4224,7 +4219,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>416</v>
       </c>
@@ -4232,7 +4227,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>418</v>
       </c>
@@ -4240,7 +4235,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>420</v>
       </c>
@@ -4248,7 +4243,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="16.5" hidden="1">
+    <row r="240" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
         <v>422</v>
       </c>
@@ -4256,7 +4251,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>423</v>
       </c>
@@ -4264,7 +4259,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>425</v>
       </c>
@@ -4272,7 +4267,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16.5" hidden="1">
+    <row r="243" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
         <v>427</v>
       </c>
@@ -4280,7 +4275,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>428</v>
       </c>
@@ -4288,7 +4283,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>430</v>
       </c>
@@ -4296,7 +4291,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>432</v>
       </c>
@@ -4304,7 +4299,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>434</v>
       </c>
@@ -4312,12 +4307,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>436</v>
       </c>
@@ -4325,7 +4320,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>438</v>
       </c>
@@ -4333,7 +4328,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>440</v>
       </c>
@@ -4341,7 +4336,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>442</v>
       </c>
@@ -4349,7 +4344,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>443</v>
       </c>
@@ -4357,7 +4352,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>445</v>
       </c>
@@ -4365,7 +4360,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>446</v>
       </c>
@@ -4373,7 +4368,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>447</v>
       </c>
@@ -4381,7 +4376,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="16.5" hidden="1">
+    <row r="257" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>448</v>
       </c>
@@ -4389,7 +4384,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>449</v>
       </c>
@@ -4397,7 +4392,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>450</v>
       </c>
@@ -4405,7 +4400,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1">
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>451</v>
       </c>
@@ -4413,7 +4408,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>453</v>
       </c>
@@ -4421,7 +4416,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>455</v>
       </c>
@@ -4429,7 +4424,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>457</v>
       </c>
@@ -4437,7 +4432,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>458</v>
       </c>
@@ -4445,7 +4440,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>460</v>
       </c>
@@ -4453,7 +4448,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>462</v>
       </c>
@@ -4461,7 +4456,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>464</v>
       </c>
@@ -4469,7 +4464,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="268" spans="1:2" hidden="1">
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>465</v>
       </c>
@@ -4477,7 +4472,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1">
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>466</v>
       </c>
@@ -4485,17 +4480,17 @@
         <v>467</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>470</v>
       </c>
@@ -4503,12 +4498,12 @@
         <v>602</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>472</v>
       </c>
@@ -4516,7 +4511,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>474</v>
       </c>
@@ -4524,12 +4519,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="276" spans="1:2" hidden="1">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>476</v>
       </c>
@@ -4537,7 +4532,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>478</v>
       </c>
@@ -4545,7 +4540,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>480</v>
       </c>
@@ -4553,7 +4548,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>481</v>
       </c>
@@ -4561,7 +4556,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>482</v>
       </c>
@@ -4569,7 +4564,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>484</v>
       </c>
@@ -4577,7 +4572,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>485</v>
       </c>
@@ -4585,7 +4580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>486</v>
       </c>
@@ -4593,7 +4588,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1">
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>487</v>
       </c>
@@ -4601,7 +4596,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1">
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>488</v>
       </c>
@@ -4609,15 +4604,12 @@
         <v>352</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>489</v>
       </c>
-      <c r="B287" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" hidden="1">
+    </row>
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>490</v>
       </c>
@@ -4625,7 +4617,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="16.5" hidden="1">
+    <row r="289" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>491</v>
       </c>
@@ -4633,7 +4625,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1">
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>492</v>
       </c>
@@ -4641,7 +4633,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1">
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>494</v>
       </c>
@@ -4649,7 +4641,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="292" spans="1:2" hidden="1">
+    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>495</v>
       </c>
@@ -4657,7 +4649,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1">
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>496</v>
       </c>
@@ -4665,7 +4657,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>497</v>
       </c>
@@ -4673,7 +4665,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1">
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>498</v>
       </c>
@@ -4681,15 +4673,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>499</v>
       </c>
-      <c r="B296" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" hidden="1">
+    </row>
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>500</v>
       </c>
@@ -4697,7 +4686,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1">
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>501</v>
       </c>
@@ -4705,7 +4694,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1">
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>502</v>
       </c>
@@ -4713,7 +4702,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1">
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>503</v>
       </c>
@@ -4721,7 +4710,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1">
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>505</v>
       </c>
@@ -4729,7 +4718,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1">
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>506</v>
       </c>
@@ -4737,12 +4726,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1">
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>508</v>
       </c>
@@ -4750,7 +4739,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>509</v>
       </c>
@@ -4758,7 +4747,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>510</v>
       </c>
@@ -4769,7 +4758,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>511</v>
       </c>
@@ -4777,7 +4766,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>512</v>
       </c>
@@ -4785,7 +4774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>513</v>
       </c>
@@ -4793,7 +4782,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>514</v>
       </c>
@@ -4801,15 +4790,12 @@
         <v>515</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>516</v>
       </c>
-      <c r="B311" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5" hidden="1">
+    </row>
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>517</v>
       </c>
@@ -4817,7 +4803,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>518</v>
       </c>
@@ -4825,7 +4811,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1">
+    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>519</v>
       </c>
@@ -4833,7 +4819,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>520</v>
       </c>
@@ -4841,7 +4827,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="16.5" hidden="1">
+    <row r="316" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A316" t="s">
         <v>521</v>
       </c>
@@ -4849,7 +4835,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1">
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>522</v>
       </c>
@@ -4857,7 +4843,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>523</v>
       </c>
@@ -4865,7 +4851,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>525</v>
       </c>
@@ -4873,7 +4859,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="16.5" hidden="1">
+    <row r="320" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A320" t="s">
         <v>526</v>
       </c>
@@ -4881,7 +4867,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1">
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>527</v>
       </c>
@@ -4889,7 +4875,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1">
+    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>528</v>
       </c>
@@ -4897,7 +4883,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1">
+    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>529</v>
       </c>
@@ -4905,7 +4891,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1">
+    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>531</v>
       </c>
@@ -4913,7 +4899,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1">
+    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>532</v>
       </c>
@@ -4921,7 +4907,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1">
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>533</v>
       </c>
@@ -4929,7 +4915,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16.5" hidden="1">
+    <row r="327" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
         <v>554</v>
       </c>
@@ -4937,7 +4923,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1">
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>534</v>
       </c>
@@ -4945,7 +4931,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1">
+    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>535</v>
       </c>
@@ -4953,7 +4939,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1">
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
         <v>536</v>
       </c>
@@ -4961,7 +4947,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1">
+    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
         <v>538</v>
       </c>
@@ -4969,7 +4955,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="332" spans="1:2" hidden="1">
+    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
         <v>539</v>
       </c>
@@ -4977,7 +4963,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1">
+    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>540</v>
       </c>
@@ -4985,7 +4971,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="334" spans="1:2" hidden="1">
+    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>541</v>
       </c>
@@ -4993,7 +4979,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="335" spans="1:2" hidden="1">
+    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>542</v>
       </c>
@@ -5001,7 +4987,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="336" spans="1:2" hidden="1">
+    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>543</v>
       </c>
@@ -5009,7 +4995,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="337" spans="1:7" hidden="1">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>545</v>
       </c>
@@ -5017,7 +5003,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>547</v>
       </c>
@@ -5025,7 +5011,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="339" spans="1:7" hidden="1">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>549</v>
       </c>
@@ -5033,7 +5019,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="340" spans="1:7" hidden="1">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>551</v>
       </c>
@@ -5041,7 +5027,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="341" spans="1:7" hidden="1">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>553</v>
       </c>
@@ -5049,7 +5035,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>577</v>
       </c>
@@ -5057,7 +5043,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="343" spans="1:7" hidden="1">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>572</v>
       </c>
@@ -5065,7 +5051,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="344" spans="1:7" hidden="1">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>576</v>
       </c>
@@ -5073,7 +5059,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1">
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>573</v>
       </c>
@@ -5081,7 +5067,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1">
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>574</v>
       </c>
@@ -5089,7 +5075,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>575</v>
       </c>
@@ -5097,7 +5083,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1">
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>578</v>
       </c>
@@ -5105,7 +5091,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>579</v>
       </c>
@@ -5113,7 +5099,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="17.25" hidden="1">
+    <row r="350" spans="1:7" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>580</v>
       </c>
@@ -5125,7 +5111,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7" hidden="1">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>581</v>
       </c>
@@ -5137,7 +5123,7 @@
       <c r="F351" s="7"/>
       <c r="G351" s="7"/>
     </row>
-    <row r="352" spans="1:7" hidden="1">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>582</v>
       </c>
@@ -5146,7 +5132,7 @@
       <c r="F352" s="7"/>
       <c r="G352" s="7"/>
     </row>
-    <row r="353" spans="1:7" hidden="1">
+    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>583</v>
       </c>
@@ -5157,7 +5143,7 @@
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7" hidden="1">
+    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>584</v>
       </c>
@@ -5168,7 +5154,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7" hidden="1">
+    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>585</v>
       </c>
@@ -5179,7 +5165,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5" hidden="1">
+    <row r="356" spans="1:7" ht="19.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
         <v>586</v>
       </c>
@@ -5191,7 +5177,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7" hidden="1">
+    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>587</v>
       </c>
@@ -5203,7 +5189,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7" hidden="1">
+    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>588</v>
       </c>
@@ -5214,7 +5200,7 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7" hidden="1">
+    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>589</v>
       </c>
@@ -5225,7 +5211,7 @@
       <c r="F359" s="7"/>
       <c r="G359" s="7"/>
     </row>
-    <row r="360" spans="1:7" hidden="1">
+    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>590</v>
       </c>
@@ -5236,7 +5222,7 @@
       <c r="F360" s="7"/>
       <c r="G360" s="7"/>
     </row>
-    <row r="361" spans="1:7" hidden="1">
+    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>592</v>
       </c>
@@ -5247,7 +5233,7 @@
       <c r="F361" s="7"/>
       <c r="G361" s="7"/>
     </row>
-    <row r="362" spans="1:7" hidden="1">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>591</v>
       </c>
@@ -5255,48 +5241,48 @@
       <c r="F362" s="7"/>
       <c r="G362" s="7"/>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E363" s="7"/>
       <c r="F363" s="7"/>
       <c r="G363" s="7"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
       <c r="F364" s="7"/>
       <c r="G364" s="7"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E365" s="7"/>
       <c r="F365" s="7"/>
       <c r="G365" s="7"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E366" s="7"/>
       <c r="F366" s="7"/>
       <c r="G366" s="7"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E367" s="7"/>
       <c r="F367" s="7"/>
       <c r="G367" s="7"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E368" s="7"/>
       <c r="F368" s="7"/>
       <c r="G368" s="7"/>
     </row>
-    <row r="369" spans="4:7">
+    <row r="369" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
       <c r="F369" s="7"/>
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362">
+  <autoFilter ref="A1:H362" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
-      <filters>
-        <filter val="julianTR4"/>
+      <filters blank="1">
+        <filter val="flxrbnk"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5306,6 +5292,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CDD89E2A6189134493471C3B1248FFEC" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f8c835211e191b604f15d9c196fd702e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73be11ab-4534-422f-8ab6-049e22ac882d" xmlns:ns3="142bc323-bc41-43fc-a839-79fc38759c0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e35637ed6ab77bc02eb788b6a909f82" ns2:_="" ns3:_="">
     <xsd:import namespace="73be11ab-4534-422f-8ab6-049e22ac882d"/>
@@ -5508,22 +5509,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A5431A-F902-4554-AE88-9292CACE75EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5540,21 +5543,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
YeldaUzun ein thema ausgetragen
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="615">
   <si>
     <t>Themen</t>
   </si>
@@ -2318,7 +2318,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130"/>
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2759,7 +2759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" hidden="1">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" hidden="1">
       <c r="A130" t="s">
         <v>238</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1">
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>255</v>
       </c>
@@ -3809,12 +3809,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1">
+    <row r="187" spans="1:2">
       <c r="A187" t="s">
         <v>327</v>
-      </c>
-      <c r="B187" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="188" spans="1:2" hidden="1">
@@ -5272,7 +5269,7 @@
   <autoFilter ref="A1:H362">
     <filterColumn colId="1">
       <filters>
-        <filter val="aliciamiederer"/>
+        <filter val="YeldaUzun"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5291,6 +5288,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CDD89E2A6189134493471C3B1248FFEC" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f8c835211e191b604f15d9c196fd702e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73be11ab-4534-422f-8ab6-049e22ac882d" xmlns:ns3="142bc323-bc41-43fc-a839-79fc38759c0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e35637ed6ab77bc02eb788b6a909f82" ns2:_="" ns3:_="">
     <xsd:import namespace="73be11ab-4534-422f-8ab6-049e22ac882d"/>
@@ -5493,12 +5496,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
   <ds:schemaRefs>
@@ -5508,6 +5505,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A5431A-F902-4554-AE88-9292CACE75EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5524,13 +5530,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
@janetteschuller aus Brainwriting ausgetragen
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="615">
   <si>
     <t>Themen</t>
   </si>
@@ -2318,7 +2318,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B243" sqref="B243"/>
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3199,12 +3199,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>202</v>
-      </c>
-      <c r="B110" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:3" hidden="1">
@@ -4254,7 +4251,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16.5">
+    <row r="243" spans="1:2" ht="16.5" hidden="1">
       <c r="A243" t="s">
         <v>426</v>
       </c>
@@ -4843,7 +4840,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="16.5">
+    <row r="320" spans="1:5" ht="16.5" hidden="1">
       <c r="A320" t="s">
         <v>614</v>
       </c>
@@ -5264,9 +5261,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H362">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Vallejk"/>
+        <filter val="Brainwriting"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5285,12 +5282,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CDD89E2A6189134493471C3B1248FFEC" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f8c835211e191b604f15d9c196fd702e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73be11ab-4534-422f-8ab6-049e22ac882d" xmlns:ns3="142bc323-bc41-43fc-a839-79fc38759c0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e35637ed6ab77bc02eb788b6a909f82" ns2:_="" ns3:_="">
     <xsd:import namespace="73be11ab-4534-422f-8ab6-049e22ac882d"/>
@@ -5493,6 +5484,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
   <ds:schemaRefs>
@@ -5502,15 +5499,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A5431A-F902-4554-AE88-9292CACE75EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5527,4 +5515,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Themen gelöscht Narin, Armin, Luis, Andreas, Martina
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C31397-C271-4331-9BDF-08215218C345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="610">
   <si>
     <t>Themen</t>
   </si>
@@ -582,9 +583,6 @@
     <t>Brainstorming</t>
   </si>
   <si>
-    <t>DasKettchup</t>
-  </si>
-  <si>
     <t>Crystal_Methods</t>
   </si>
   <si>
@@ -1044,9 +1042,6 @@
     <t>Risikodimensionen</t>
   </si>
   <si>
-    <t>martina-bchtl</t>
-  </si>
-  <si>
     <t>Risikoanalyse_und_Visualisierung</t>
   </si>
   <si>
@@ -1198,9 +1193,6 @@
   </si>
   <si>
     <t>Projekt_Lebenszyklus</t>
-  </si>
-  <si>
-    <t>arminwelte</t>
   </si>
   <si>
     <t>Qualitaetssicherung</t>
@@ -1866,8 +1858,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2307,24 +2299,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="83.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2340,7 +2332,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2348,7 +2340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2356,7 +2348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2365,7 +2357,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2373,7 +2365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2381,7 +2373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2389,7 +2381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2397,7 +2389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2405,7 +2397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2413,7 +2405,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2421,7 +2413,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2429,7 +2421,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2437,7 +2429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -2453,7 +2445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2461,7 +2453,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +2461,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2477,7 +2469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2485,7 +2477,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2493,7 +2485,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2501,7 +2493,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2509,7 +2501,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2517,7 +2509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2525,7 +2517,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +2525,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -2541,7 +2533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2549,25 +2541,25 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" hidden="1">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -2575,7 +2567,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -2583,7 +2575,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2591,7 +2583,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2599,7 +2591,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -2607,7 +2599,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2615,7 +2607,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -2623,12 +2615,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -2636,7 +2628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -2644,7 +2636,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2652,15 +2644,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" hidden="1">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2669,7 +2661,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -2678,7 +2670,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -2686,7 +2678,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2694,15 +2686,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>88</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" hidden="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -2710,7 +2702,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -2718,7 +2710,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -2726,7 +2718,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -2734,7 +2726,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -2742,7 +2734,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -2750,17 +2742,17 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -2768,7 +2760,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>104</v>
       </c>
@@ -2776,7 +2768,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>106</v>
       </c>
@@ -2784,7 +2776,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>108</v>
       </c>
@@ -2792,7 +2784,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>110</v>
       </c>
@@ -2800,7 +2792,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>112</v>
       </c>
@@ -2808,7 +2800,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>114</v>
       </c>
@@ -2816,7 +2808,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>116</v>
       </c>
@@ -2824,7 +2816,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>118</v>
       </c>
@@ -2832,7 +2824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -2840,12 +2832,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -2853,7 +2845,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>124</v>
       </c>
@@ -2861,7 +2853,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -2869,7 +2861,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -2877,15 +2869,15 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>130</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" hidden="1">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>131</v>
       </c>
@@ -2893,7 +2885,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>133</v>
       </c>
@@ -2901,7 +2893,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>135</v>
       </c>
@@ -2909,7 +2901,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>137</v>
       </c>
@@ -2917,7 +2909,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>138</v>
       </c>
@@ -2925,7 +2917,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -2933,7 +2925,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>141</v>
       </c>
@@ -2941,7 +2933,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -2949,7 +2941,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>145</v>
       </c>
@@ -2957,7 +2949,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>147</v>
       </c>
@@ -2965,7 +2957,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>149</v>
       </c>
@@ -2973,7 +2965,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>151</v>
       </c>
@@ -2981,12 +2973,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>154</v>
       </c>
@@ -2994,7 +2986,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>156</v>
       </c>
@@ -3002,7 +2994,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>158</v>
       </c>
@@ -3010,7 +3002,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>160</v>
       </c>
@@ -3018,7 +3010,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>162</v>
       </c>
@@ -3026,7 +3018,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>163</v>
       </c>
@@ -3034,7 +3026,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>165</v>
       </c>
@@ -3042,7 +3034,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>167</v>
       </c>
@@ -3050,7 +3042,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>169</v>
       </c>
@@ -3058,7 +3050,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>171</v>
       </c>
@@ -3066,7 +3058,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>173</v>
       </c>
@@ -3074,7 +3066,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>175</v>
       </c>
@@ -3082,7 +3074,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>177</v>
       </c>
@@ -3090,7 +3082,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>179</v>
       </c>
@@ -3098,7 +3090,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>181</v>
       </c>
@@ -3106,7 +3098,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>183</v>
       </c>
@@ -3114,2138 +3106,2123 @@
         <v>184</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>185</v>
       </c>
-      <c r="B101" t="s">
+    </row>
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" hidden="1">
-      <c r="A102" t="s">
+      <c r="B102" t="s">
         <v>187</v>
       </c>
-      <c r="B102" t="s">
+    </row>
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" hidden="1">
-      <c r="A103" t="s">
+      <c r="B103" t="s">
         <v>189</v>
       </c>
-      <c r="B103" t="s">
+    </row>
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" hidden="1">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
         <v>191</v>
       </c>
-      <c r="B104" t="s">
+    </row>
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" hidden="1">
-      <c r="A105" t="s">
-        <v>193</v>
       </c>
       <c r="B105" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B106" s="3">
         <v>29834</v>
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" hidden="1">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>194</v>
+      </c>
+      <c r="B107" t="s">
         <v>195</v>
       </c>
-      <c r="B107" t="s">
+    </row>
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" hidden="1">
-      <c r="A108" t="s">
+      <c r="B108" t="s">
         <v>197</v>
       </c>
-      <c r="B108" t="s">
+    </row>
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" hidden="1">
-      <c r="A109" t="s">
+      <c r="B109" t="s">
         <v>199</v>
       </c>
-      <c r="B109" t="s">
+    </row>
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1">
-      <c r="A110" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" hidden="1">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>202</v>
+      </c>
+      <c r="B111" t="s">
         <v>203</v>
       </c>
-      <c r="B111" t="s">
+    </row>
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" hidden="1">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
         <v>205</v>
       </c>
-      <c r="B112" t="s">
+    </row>
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" hidden="1">
-      <c r="A113" t="s">
+      <c r="B113" t="s">
         <v>207</v>
       </c>
-      <c r="B113" t="s">
+    </row>
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" hidden="1">
-      <c r="A114" t="s">
+      <c r="B114" t="s">
         <v>209</v>
       </c>
-      <c r="B114" t="s">
+    </row>
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" hidden="1">
-      <c r="A115" t="s">
+      <c r="B115" t="s">
         <v>211</v>
       </c>
-      <c r="B115" t="s">
+    </row>
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" hidden="1">
-      <c r="A116" t="s">
+      <c r="B116" t="s">
         <v>213</v>
       </c>
-      <c r="B116" t="s">
+    </row>
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" hidden="1">
-      <c r="A117" t="s">
-        <v>215</v>
       </c>
       <c r="B117" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B118" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>216</v>
+      </c>
+      <c r="B119" t="s">
         <v>217</v>
       </c>
-      <c r="B119" t="s">
+    </row>
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" hidden="1">
-      <c r="A120" t="s">
+      <c r="B120" t="s">
         <v>219</v>
       </c>
-      <c r="B120" t="s">
+    </row>
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" hidden="1">
-      <c r="A121" t="s">
+      <c r="B121" t="s">
         <v>221</v>
       </c>
-      <c r="B121" t="s">
+    </row>
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" hidden="1">
-      <c r="A122" t="s">
+      <c r="B122" t="s">
         <v>223</v>
       </c>
-      <c r="B122" t="s">
+    </row>
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" hidden="1">
-      <c r="A123" t="s">
+      <c r="B123" t="s">
         <v>225</v>
       </c>
-      <c r="B123" t="s">
+    </row>
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" hidden="1">
-      <c r="A124" t="s">
+      <c r="B124" t="s">
         <v>227</v>
       </c>
-      <c r="B124" t="s">
+    </row>
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" hidden="1">
-      <c r="A125" t="s">
+      <c r="B125" t="s">
         <v>229</v>
       </c>
-      <c r="B125" t="s">
+    </row>
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" hidden="1">
-      <c r="A126" t="s">
+      <c r="B126" t="s">
         <v>231</v>
       </c>
-      <c r="B126" t="s">
+    </row>
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" hidden="1">
-      <c r="A127" t="s">
+      <c r="B127" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>233</v>
-      </c>
-      <c r="B127" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" hidden="1">
-      <c r="A128" t="s">
-        <v>234</v>
       </c>
       <c r="B128" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="16.5" hidden="1">
+    <row r="129" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" hidden="1">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" hidden="1">
-      <c r="A131" t="s">
+      <c r="B131" t="s">
         <v>238</v>
       </c>
-      <c r="B131" t="s">
+    </row>
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" hidden="1">
-      <c r="A132" t="s">
+      <c r="B132" t="s">
         <v>240</v>
       </c>
-      <c r="B132" t="s">
+    </row>
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" hidden="1">
-      <c r="A133" t="s">
-        <v>242</v>
       </c>
       <c r="B133" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>242</v>
+      </c>
+      <c r="B134" t="s">
         <v>243</v>
       </c>
-      <c r="B134" t="s">
+    </row>
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" hidden="1">
-      <c r="A135" t="s">
+      <c r="B135" t="s">
         <v>245</v>
       </c>
-      <c r="B135" t="s">
+    </row>
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" hidden="1">
-      <c r="A136" t="s">
+      <c r="B136" t="s">
         <v>247</v>
       </c>
-      <c r="B136" t="s">
+    </row>
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" hidden="1">
-      <c r="A137" t="s">
+      <c r="B137" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>249</v>
       </c>
-      <c r="B137" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" hidden="1">
-      <c r="A138" t="s">
+      <c r="B138" t="s">
         <v>250</v>
       </c>
-      <c r="B138" t="s">
+    </row>
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" hidden="1">
-      <c r="A139" t="s">
+      <c r="B139" s="10" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>252</v>
       </c>
-      <c r="B139" s="10" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" hidden="1">
-      <c r="A140" t="s">
+      <c r="B140" s="10" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>253</v>
       </c>
-      <c r="B140" s="10" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" hidden="1">
-      <c r="A141" t="s">
+      <c r="B141" t="s">
         <v>254</v>
       </c>
-      <c r="B141" t="s">
+    </row>
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1">
-      <c r="A142" t="s">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>256</v>
       </c>
-      <c r="B142" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" hidden="1">
-      <c r="A143" t="s">
+      <c r="B143" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>257</v>
       </c>
-      <c r="B143" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" hidden="1">
-      <c r="A144" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" hidden="1">
+    </row>
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" hidden="1">
-      <c r="A146" t="s">
-        <v>261</v>
       </c>
       <c r="B146" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>261</v>
+      </c>
+      <c r="B147" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>262</v>
       </c>
-      <c r="B147" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" hidden="1">
-      <c r="A148" t="s">
+      <c r="B148" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>263</v>
       </c>
-      <c r="B148" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" hidden="1">
-      <c r="A149" t="s">
+      <c r="B149" t="s">
         <v>264</v>
       </c>
-      <c r="B149" t="s">
+    </row>
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" hidden="1">
-      <c r="A150" t="s">
+      <c r="B150" t="s">
         <v>266</v>
       </c>
-      <c r="B150" t="s">
+    </row>
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" hidden="1">
-      <c r="A151" t="s">
+      <c r="B151" t="s">
         <v>268</v>
       </c>
-      <c r="B151" t="s">
+    </row>
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" hidden="1">
-      <c r="A152" t="s">
-        <v>270</v>
       </c>
       <c r="B152" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B153" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B154" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B155" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B156" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
+        <v>274</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>275</v>
       </c>
-      <c r="B157" s="10" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" hidden="1">
-      <c r="A158" t="s">
+      <c r="B158" t="s">
         <v>276</v>
       </c>
-      <c r="B158" t="s">
+    </row>
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" hidden="1">
-      <c r="A159" t="s">
+      <c r="B159" t="s">
         <v>278</v>
       </c>
-      <c r="B159" t="s">
+    </row>
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" hidden="1">
-      <c r="A160" t="s">
+      <c r="B160" t="s">
         <v>280</v>
       </c>
-      <c r="B160" t="s">
+    </row>
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" hidden="1">
-      <c r="A161" t="s">
+      <c r="B161" t="s">
         <v>282</v>
       </c>
-      <c r="B161" t="s">
+    </row>
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" hidden="1">
-      <c r="A162" t="s">
+      <c r="B162" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B162" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" hidden="1">
-      <c r="A163" s="4" t="s">
+      <c r="B163" t="s">
         <v>285</v>
       </c>
-      <c r="B163" t="s">
+    </row>
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" hidden="1">
-      <c r="A164" t="s">
+      <c r="B164" t="s">
         <v>287</v>
       </c>
-      <c r="B164" t="s">
+    </row>
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>288</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" hidden="1">
-      <c r="A165" t="s">
-        <v>289</v>
       </c>
       <c r="B165" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>289</v>
+      </c>
+      <c r="B166" t="s">
         <v>290</v>
       </c>
-      <c r="B166" t="s">
+    </row>
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" hidden="1">
-      <c r="A167" t="s">
-        <v>292</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
+        <v>292</v>
+      </c>
+      <c r="B168" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>293</v>
       </c>
-      <c r="B168" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" hidden="1">
-      <c r="A169" t="s">
+      <c r="B169" t="s">
         <v>294</v>
       </c>
-      <c r="B169" t="s">
+    </row>
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" hidden="1">
-      <c r="A170" t="s">
+      <c r="B170" t="s">
         <v>296</v>
       </c>
-      <c r="B170" t="s">
+    </row>
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" hidden="1">
-      <c r="A171" t="s">
+      <c r="B171" t="s">
         <v>298</v>
       </c>
-      <c r="B171" t="s">
+    </row>
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" hidden="1">
-      <c r="A172" t="s">
+      <c r="B172" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
         <v>300</v>
       </c>
-      <c r="B172" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" hidden="1">
-      <c r="A173" t="s">
+      <c r="B173" t="s">
         <v>301</v>
       </c>
-      <c r="B173" t="s">
+    </row>
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" hidden="1">
-      <c r="A174" t="s">
+      <c r="B174" t="s">
         <v>303</v>
       </c>
-      <c r="B174" t="s">
+    </row>
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" hidden="1">
-      <c r="A175" t="s">
+      <c r="B175" t="s">
         <v>305</v>
       </c>
-      <c r="B175" t="s">
+    </row>
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" hidden="1">
-      <c r="A176" t="s">
+      <c r="B176" t="s">
         <v>307</v>
       </c>
-      <c r="B176" t="s">
+    </row>
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" hidden="1">
-      <c r="A177" t="s">
+      <c r="B177" t="s">
         <v>309</v>
       </c>
-      <c r="B177" t="s">
+    </row>
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" hidden="1">
-      <c r="A178" t="s">
+      <c r="B178" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
         <v>311</v>
       </c>
-      <c r="B178" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" hidden="1">
-      <c r="A179" t="s">
+      <c r="B179" t="s">
         <v>312</v>
       </c>
-      <c r="B179" t="s">
+    </row>
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1">
-      <c r="A180" t="s">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1">
-      <c r="A181" t="s">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" hidden="1">
-      <c r="A182" t="s">
+      <c r="B182" t="s">
         <v>316</v>
       </c>
-      <c r="B182" t="s">
+    </row>
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" hidden="1">
-      <c r="A183" t="s">
+      <c r="B183" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
         <v>318</v>
       </c>
-      <c r="B183" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" hidden="1">
-      <c r="A184" t="s">
+      <c r="B184" t="s">
         <v>319</v>
       </c>
-      <c r="B184" t="s">
+    </row>
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" hidden="1">
-      <c r="A185" t="s">
+      <c r="B185" t="s">
         <v>321</v>
       </c>
-      <c r="B185" t="s">
+    </row>
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" hidden="1">
-      <c r="A186" t="s">
+      <c r="B186" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
         <v>323</v>
       </c>
-      <c r="B186" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" hidden="1">
-      <c r="A187" t="s">
+    </row>
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" hidden="1">
-      <c r="A188" t="s">
+      <c r="B188" t="s">
         <v>325</v>
       </c>
-      <c r="B188" t="s">
+    </row>
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" hidden="1">
-      <c r="A189" t="s">
+      <c r="B189" t="s">
         <v>327</v>
       </c>
-      <c r="B189" t="s">
+    </row>
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" hidden="1">
-      <c r="A190" t="s">
+      <c r="B190" t="s">
         <v>329</v>
       </c>
-      <c r="B190" t="s">
+    </row>
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" hidden="1">
-      <c r="A191" t="s">
+      <c r="B191" s="10" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
         <v>331</v>
       </c>
-      <c r="B191" s="10" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" hidden="1">
-      <c r="A192" t="s">
+      <c r="B192" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
         <v>332</v>
       </c>
-      <c r="B192" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" hidden="1">
-      <c r="A193" t="s">
+      <c r="B193" t="s">
         <v>333</v>
       </c>
-      <c r="B193" t="s">
+    </row>
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" hidden="1">
-      <c r="A194" t="s">
+      <c r="B194" t="s">
         <v>335</v>
       </c>
-      <c r="B194" t="s">
+    </row>
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" hidden="1">
-      <c r="A195" t="s">
+      <c r="B195" t="s">
         <v>337</v>
       </c>
-      <c r="B195" t="s">
+    </row>
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1">
-      <c r="A196" t="s">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
         <v>339</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B197" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1">
-      <c r="A197" t="s">
+    <row r="198" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
         <v>341</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B198" s="6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5" hidden="1">
-      <c r="A198" t="s">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
         <v>343</v>
       </c>
-      <c r="B198" s="6" t="s">
+      <c r="B199" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1">
-      <c r="A199" t="s">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
         <v>345</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B200" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1">
-      <c r="A200" t="s">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
         <v>347</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1">
-      <c r="A201" t="s">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
         <v>349</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B202" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1">
-      <c r="A202" t="s">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
         <v>351</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B203" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1">
-      <c r="A203" t="s">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
         <v>353</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B204" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1">
-      <c r="A204" t="s">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
         <v>355</v>
-      </c>
-      <c r="B204" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" hidden="1">
-      <c r="A205" t="s">
-        <v>357</v>
       </c>
       <c r="B205" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>356</v>
+      </c>
+      <c r="B206" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
         <v>358</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B207" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1">
-      <c r="A207" t="s">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>547</v>
+      </c>
+      <c r="B208" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
         <v>360</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B209" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1">
-      <c r="A208" t="s">
-        <v>550</v>
-      </c>
-      <c r="B208" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" hidden="1">
-      <c r="A209" t="s">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
         <v>362</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B210" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1">
-      <c r="A210" t="s">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
         <v>364</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B211" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1">
-      <c r="A211" t="s">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
         <v>366</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1">
-      <c r="A212" t="s">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
         <v>368</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B213" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1">
-      <c r="A213" t="s">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
         <v>370</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B214" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1">
-      <c r="A214" t="s">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
         <v>372</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B215" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" hidden="1">
-      <c r="A215" t="s">
+      <c r="B216" t="s">
         <v>374</v>
       </c>
-      <c r="B215" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" hidden="1">
-      <c r="A216" t="s">
+    </row>
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
         <v>375</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B217" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1">
-      <c r="A217" t="s">
+    <row r="218" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
         <v>377</v>
       </c>
-      <c r="B217" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="16.5" hidden="1">
-      <c r="A218" t="s">
+      <c r="B218" s="12" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
         <v>379</v>
-      </c>
-      <c r="B218" s="12" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" hidden="1">
-      <c r="A219" t="s">
-        <v>381</v>
       </c>
       <c r="B219" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
+        <v>380</v>
+      </c>
+      <c r="B220" s="10" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>381</v>
+      </c>
+      <c r="B221" t="s">
         <v>382</v>
       </c>
-      <c r="B220" s="10" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" hidden="1">
-      <c r="A221" t="s">
+    </row>
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
         <v>383</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B222" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1">
-      <c r="A222" t="s">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
         <v>385</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B223" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1">
-      <c r="A223" t="s">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
         <v>387</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B224" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1">
-      <c r="A224" t="s">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
         <v>389</v>
       </c>
-      <c r="B224" t="s">
+    </row>
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" hidden="1">
-      <c r="A225" t="s">
+      <c r="B226" t="s">
         <v>391</v>
       </c>
-      <c r="B225" t="s">
+    </row>
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" hidden="1">
-      <c r="A226" t="s">
+      <c r="B227" t="s">
         <v>393</v>
       </c>
-      <c r="B226" t="s">
+    </row>
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" hidden="1">
-      <c r="A227" t="s">
+      <c r="B228" t="s">
         <v>395</v>
       </c>
-      <c r="B227" t="s">
+    </row>
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" hidden="1">
-      <c r="A228" t="s">
+      <c r="B229" t="s">
         <v>397</v>
       </c>
-      <c r="B228" t="s">
+    </row>
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" hidden="1">
-      <c r="A229" t="s">
+      <c r="B230" t="s">
         <v>399</v>
       </c>
-      <c r="B229" t="s">
+    </row>
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" hidden="1">
-      <c r="A230" t="s">
+      <c r="B231" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
         <v>401</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B232" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1">
-      <c r="A231" t="s">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
         <v>403</v>
       </c>
-      <c r="B231" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" hidden="1">
-      <c r="A232" t="s">
+      <c r="B233" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
         <v>404</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B234" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1">
-      <c r="A233" t="s">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
         <v>406</v>
       </c>
-      <c r="B233" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" hidden="1">
-      <c r="A234" t="s">
+      <c r="B235" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
         <v>407</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B236" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1">
-      <c r="A235" t="s">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
         <v>409</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B237" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>411</v>
+      </c>
+      <c r="B238" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>413</v>
+      </c>
+      <c r="B239" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A240" t="s">
+        <v>415</v>
+      </c>
+      <c r="B240" s="13" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1">
-      <c r="A236" t="s">
-        <v>410</v>
-      </c>
-      <c r="B236" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" hidden="1">
-      <c r="A237" t="s">
-        <v>412</v>
-      </c>
-      <c r="B237" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" hidden="1">
-      <c r="A238" t="s">
-        <v>414</v>
-      </c>
-      <c r="B238" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" hidden="1">
-      <c r="A239" t="s">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
         <v>416</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B241" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="16.5" hidden="1">
-      <c r="A240" t="s">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
         <v>418</v>
       </c>
-      <c r="B240" s="13" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" hidden="1">
-      <c r="A241" t="s">
+      <c r="B242" t="s">
         <v>419</v>
       </c>
-      <c r="B241" t="s">
+    </row>
+    <row r="243" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A243" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" hidden="1">
-      <c r="A242" t="s">
+      <c r="B243" s="13" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
         <v>421</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B244" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16.5" hidden="1">
-      <c r="A243" t="s">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
         <v>423</v>
       </c>
-      <c r="B243" s="13" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" hidden="1">
-      <c r="A244" t="s">
+      <c r="B245" t="s">
         <v>424</v>
       </c>
-      <c r="B244" t="s">
+    </row>
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" hidden="1">
-      <c r="A245" t="s">
+      <c r="B246" t="s">
         <v>426</v>
       </c>
-      <c r="B245" t="s">
+    </row>
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" hidden="1">
-      <c r="A246" t="s">
-        <v>428</v>
-      </c>
-      <c r="B246" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" hidden="1">
-      <c r="A247" t="s">
-        <v>430</v>
       </c>
       <c r="B247" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>429</v>
+      </c>
+      <c r="B249" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" hidden="1">
-      <c r="A249" t="s">
+      <c r="B250" t="s">
         <v>432</v>
       </c>
-      <c r="B249" t="s">
+    </row>
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" hidden="1">
-      <c r="A250" t="s">
+      <c r="B251" t="s">
         <v>434</v>
       </c>
-      <c r="B250" t="s">
+    </row>
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" hidden="1">
-      <c r="A251" t="s">
+      <c r="B252" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
         <v>436</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B253" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1">
-      <c r="A252" t="s">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
         <v>438</v>
       </c>
-      <c r="B252" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" hidden="1">
-      <c r="A253" t="s">
+      <c r="B254" s="10" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
         <v>439</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B255" s="11" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" hidden="1">
-      <c r="A254" t="s">
+      <c r="B256" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
         <v>441</v>
       </c>
-      <c r="B254" s="10" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" hidden="1">
-      <c r="A255" t="s">
+      <c r="B257" s="12" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
         <v>442</v>
       </c>
-      <c r="B255" s="11" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" hidden="1">
-      <c r="A256" t="s">
+      <c r="B258" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
         <v>443</v>
       </c>
-      <c r="B256" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" ht="16.5" hidden="1">
-      <c r="A257" t="s">
+      <c r="B259" s="7" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
         <v>444</v>
       </c>
-      <c r="B257" s="12" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" hidden="1">
-      <c r="A258" t="s">
+      <c r="B260" t="s">
         <v>445</v>
       </c>
-      <c r="B258" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" hidden="1">
-      <c r="A259" t="s">
+    </row>
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
         <v>446</v>
       </c>
-      <c r="B259" s="7" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" hidden="1">
-      <c r="A260" t="s">
+      <c r="B261" t="s">
         <v>447</v>
       </c>
-      <c r="B260" t="s">
+    </row>
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" hidden="1">
-      <c r="A261" t="s">
+      <c r="B262" t="s">
         <v>449</v>
       </c>
-      <c r="B261" t="s">
+    </row>
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" hidden="1">
-      <c r="A262" t="s">
+      <c r="B263" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
         <v>451</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B264" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1">
-      <c r="A263" t="s">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
         <v>453</v>
       </c>
-      <c r="B263" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" hidden="1">
-      <c r="A264" t="s">
+      <c r="B265" t="s">
         <v>454</v>
       </c>
-      <c r="B264" t="s">
+    </row>
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" hidden="1">
-      <c r="A265" t="s">
+      <c r="B266" t="s">
         <v>456</v>
       </c>
-      <c r="B265" t="s">
+    </row>
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" hidden="1">
-      <c r="A266" t="s">
+      <c r="B267" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
         <v>458</v>
       </c>
-      <c r="B266" t="s">
+      <c r="B268" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" hidden="1">
-      <c r="A267" t="s">
+      <c r="B269" t="s">
         <v>460</v>
       </c>
-      <c r="B267" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" hidden="1">
-      <c r="A268" t="s">
+    </row>
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
         <v>461</v>
       </c>
-      <c r="B268" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" hidden="1">
-      <c r="A269" t="s">
+    </row>
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
         <v>462</v>
       </c>
-      <c r="B269" t="s">
+    </row>
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" hidden="1">
-      <c r="A270" t="s">
+      <c r="B272" s="10" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1">
-      <c r="A271" t="s">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" hidden="1">
-      <c r="A272" t="s">
+      <c r="B274" t="s">
         <v>466</v>
       </c>
-      <c r="B272" s="10" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" hidden="1">
-      <c r="A273" t="s">
+    </row>
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" hidden="1">
-      <c r="A274" t="s">
+      <c r="B275" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
         <v>468</v>
       </c>
-      <c r="B274" t="s">
+    </row>
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" hidden="1">
-      <c r="A275" t="s">
+      <c r="B277" t="s">
         <v>470</v>
       </c>
-      <c r="B275" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" hidden="1">
-      <c r="A276" t="s">
+    </row>
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" hidden="1">
-      <c r="A277" t="s">
+      <c r="B278" t="s">
         <v>472</v>
       </c>
-      <c r="B277" t="s">
+    </row>
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" hidden="1">
-      <c r="A278" t="s">
+      <c r="B279" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
         <v>474</v>
-      </c>
-      <c r="B278" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" hidden="1">
-      <c r="A279" t="s">
-        <v>476</v>
-      </c>
-      <c r="B279" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" hidden="1">
-      <c r="A280" t="s">
-        <v>477</v>
       </c>
       <c r="B280" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B281" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" hidden="1">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B282" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B283" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B284" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1">
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
+        <v>480</v>
+      </c>
+      <c r="B285" s="7" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>481</v>
+      </c>
+      <c r="B286" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
         <v>483</v>
       </c>
-      <c r="B285" s="7" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" hidden="1">
-      <c r="A286" t="s">
+    </row>
+    <row r="289" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
         <v>484</v>
       </c>
-      <c r="B286" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" hidden="1">
-      <c r="A287" t="s">
+      <c r="B289" s="12" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="288" spans="1:2" hidden="1">
-      <c r="A288" t="s">
+      <c r="B290" t="s">
         <v>486</v>
       </c>
-      <c r="B288" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" ht="16.5" hidden="1">
-      <c r="A289" t="s">
+    </row>
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
         <v>487</v>
       </c>
-      <c r="B289" s="12" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" hidden="1">
-      <c r="A290" t="s">
+      <c r="B291" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
         <v>488</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B292" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
         <v>489</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" hidden="1">
-      <c r="A291" t="s">
-        <v>490</v>
-      </c>
-      <c r="B291" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" hidden="1">
-      <c r="A292" t="s">
-        <v>491</v>
-      </c>
-      <c r="B292" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" hidden="1">
-      <c r="A293" t="s">
-        <v>492</v>
       </c>
       <c r="B293" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B294" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1">
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
+        <v>491</v>
+      </c>
+      <c r="B295" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>493</v>
+      </c>
+      <c r="B297" s="7" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
         <v>494</v>
-      </c>
-      <c r="B295" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" hidden="1">
-      <c r="A296" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" hidden="1">
-      <c r="A297" t="s">
-        <v>496</v>
-      </c>
-      <c r="B297" s="7" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" hidden="1">
-      <c r="A298" t="s">
-        <v>497</v>
       </c>
       <c r="B298" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1">
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
+        <v>495</v>
+      </c>
+      <c r="B299" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>496</v>
+      </c>
+      <c r="B300" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
         <v>498</v>
       </c>
-      <c r="B299" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" hidden="1">
-      <c r="A300" t="s">
+      <c r="B301" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
         <v>499</v>
-      </c>
-      <c r="B300" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" hidden="1">
-      <c r="A301" t="s">
-        <v>501</v>
-      </c>
-      <c r="B301" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" hidden="1">
-      <c r="A302" t="s">
-        <v>502</v>
       </c>
       <c r="B302" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1">
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" hidden="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B304" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="305" spans="1:5" hidden="1">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B305" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E306" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="307" spans="1:5" hidden="1">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B307" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B308" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
+        <v>506</v>
+      </c>
+      <c r="B309" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>507</v>
+      </c>
+      <c r="B310" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
         <v>509</v>
       </c>
-      <c r="B309" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="310" spans="1:5" hidden="1">
-      <c r="A310" t="s">
+    </row>
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
         <v>510</v>
-      </c>
-      <c r="B310" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="311" spans="1:5" hidden="1">
-      <c r="A311" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="312" spans="1:5" hidden="1">
-      <c r="A312" t="s">
-        <v>513</v>
       </c>
       <c r="B312" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
+        <v>511</v>
+      </c>
+      <c r="B313" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A314" t="s">
+        <v>512</v>
+      </c>
+      <c r="B314" s="13" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>513</v>
+      </c>
+      <c r="B315" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A316" t="s">
         <v>514</v>
       </c>
-      <c r="B313" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="314" spans="1:5" ht="16.5" hidden="1">
-      <c r="A314" t="s">
+      <c r="B316" s="13" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
         <v>515</v>
       </c>
-      <c r="B314" s="13" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="315" spans="1:5" hidden="1">
-      <c r="A315" t="s">
+      <c r="B317" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
         <v>516</v>
       </c>
-      <c r="B315" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="316" spans="1:5" ht="16.5" hidden="1">
-      <c r="A316" t="s">
+      <c r="B318" t="s">
         <v>517</v>
       </c>
-      <c r="B316" s="13" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="317" spans="1:5" hidden="1">
-      <c r="A317" t="s">
+    </row>
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
         <v>518</v>
-      </c>
-      <c r="B317" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="318" spans="1:5" hidden="1">
-      <c r="A318" t="s">
-        <v>519</v>
-      </c>
-      <c r="B318" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="319" spans="1:5" hidden="1">
-      <c r="A319" t="s">
-        <v>521</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="16.5" hidden="1">
+    <row r="320" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A320" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" hidden="1">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B321" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1">
+    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B322" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1">
+    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
+        <v>521</v>
+      </c>
+      <c r="B323" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>523</v>
+      </c>
+      <c r="B324" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
         <v>524</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B325" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" hidden="1">
-      <c r="A324" t="s">
-        <v>526</v>
-      </c>
-      <c r="B324" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" hidden="1">
-      <c r="A325" t="s">
-        <v>527</v>
-      </c>
-      <c r="B325" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" hidden="1">
-      <c r="A326" t="s">
-        <v>528</v>
       </c>
       <c r="B326" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16.5" hidden="1">
+    <row r="327" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" hidden="1">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B328" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" hidden="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B329" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1">
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="B330" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A331" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B331" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A332" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B332" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
         <v>532</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" hidden="1">
-      <c r="A331" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="B331" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" hidden="1">
-      <c r="A332" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="B332" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" hidden="1">
-      <c r="A333" t="s">
-        <v>535</v>
       </c>
       <c r="B333" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="334" spans="1:2" hidden="1">
+    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
+        <v>533</v>
+      </c>
+      <c r="B334" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>534</v>
+      </c>
+      <c r="B335" s="10" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>535</v>
+      </c>
+      <c r="B336" t="s">
         <v>536</v>
       </c>
-      <c r="B334" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" hidden="1">
-      <c r="A335" t="s">
+    </row>
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
         <v>537</v>
       </c>
-      <c r="B335" s="10" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" hidden="1">
-      <c r="A336" t="s">
+      <c r="B337" t="s">
         <v>538</v>
       </c>
-      <c r="B336" t="s">
+    </row>
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="337" spans="1:7" hidden="1">
-      <c r="A337" t="s">
+      <c r="B338" t="s">
         <v>540</v>
       </c>
-      <c r="B337" t="s">
+    </row>
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="338" spans="1:7" hidden="1">
-      <c r="A338" t="s">
+      <c r="B339" t="s">
         <v>542</v>
       </c>
-      <c r="B338" t="s">
+    </row>
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="339" spans="1:7" hidden="1">
-      <c r="A339" t="s">
+      <c r="B340" t="s">
         <v>544</v>
       </c>
-      <c r="B339" t="s">
+    </row>
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="340" spans="1:7" hidden="1">
-      <c r="A340" t="s">
-        <v>546</v>
-      </c>
-      <c r="B340" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="341" spans="1:7" hidden="1">
-      <c r="A341" t="s">
+      <c r="B341" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>569</v>
+      </c>
+      <c r="B342" s="7" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>564</v>
+      </c>
+      <c r="B343" s="7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>568</v>
+      </c>
+      <c r="B344" s="7" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>565</v>
+      </c>
+      <c r="B345" s="7" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>566</v>
+      </c>
+      <c r="B346" s="7" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>567</v>
+      </c>
+      <c r="B347" t="s">
         <v>548</v>
       </c>
-      <c r="B341" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="342" spans="1:7" hidden="1">
-      <c r="A342" t="s">
+    </row>
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>570</v>
+      </c>
+      <c r="B348" s="7" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>571</v>
+      </c>
+      <c r="B349" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A350" t="s">
         <v>572</v>
       </c>
-      <c r="B342" s="7" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="343" spans="1:7" hidden="1">
-      <c r="A343" t="s">
-        <v>567</v>
-      </c>
-      <c r="B343" s="7" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="344" spans="1:7" hidden="1">
-      <c r="A344" t="s">
-        <v>571</v>
-      </c>
-      <c r="B344" s="7" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="345" spans="1:7" hidden="1">
-      <c r="A345" t="s">
-        <v>568</v>
-      </c>
-      <c r="B345" s="7" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="346" spans="1:7" hidden="1">
-      <c r="A346" t="s">
-        <v>569</v>
-      </c>
-      <c r="B346" s="7" t="s">
+      <c r="B350" s="9" t="s">
         <v>554</v>
-      </c>
-    </row>
-    <row r="347" spans="1:7" hidden="1">
-      <c r="A347" t="s">
-        <v>570</v>
-      </c>
-      <c r="B347" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="348" spans="1:7" hidden="1">
-      <c r="A348" t="s">
-        <v>573</v>
-      </c>
-      <c r="B348" s="7" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="349" spans="1:7" hidden="1">
-      <c r="A349" t="s">
-        <v>574</v>
-      </c>
-      <c r="B349" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="350" spans="1:7" ht="17.25" hidden="1">
-      <c r="A350" t="s">
-        <v>575</v>
-      </c>
-      <c r="B350" s="9" t="s">
-        <v>557</v>
       </c>
       <c r="D350" s="7"/>
       <c r="E350" s="7"/>
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7" hidden="1">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B351" s="7" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D351" s="7"/>
       <c r="E351" s="7"/>
       <c r="F351" s="7"/>
       <c r="G351" s="7"/>
     </row>
-    <row r="352" spans="1:7" hidden="1">
+    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B352" s="7"/>
       <c r="E352" s="7"/>
       <c r="F352" s="7"/>
       <c r="G352" s="7"/>
     </row>
-    <row r="353" spans="1:7" hidden="1">
+    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B353" s="10" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7" hidden="1">
+    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B354" s="7" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E354" s="7"/>
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7" hidden="1">
+    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B355" s="7" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E355" s="7"/>
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5" hidden="1">
+    <row r="356" spans="1:7" ht="19.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D356" s="8"/>
       <c r="E356" s="7"/>
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7" hidden="1">
+    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B357" s="7" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D357" s="7"/>
       <c r="E357" s="7"/>
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7" hidden="1">
+    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E358" s="7"/>
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7" hidden="1">
+    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E359" s="7"/>
       <c r="F359" s="7"/>
       <c r="G359" s="7"/>
     </row>
-    <row r="360" spans="1:7" hidden="1">
+    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B360" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E360" s="7"/>
       <c r="F360" s="7"/>
       <c r="G360" s="7"/>
     </row>
-    <row r="361" spans="1:7" hidden="1">
+    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B361" s="10" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E361" s="7"/>
       <c r="F361" s="7"/>
       <c r="G361" s="7"/>
     </row>
-    <row r="362" spans="1:7" hidden="1">
+    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E362" s="7"/>
       <c r="F362" s="7"/>
       <c r="G362" s="7"/>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E363" s="7"/>
       <c r="F363" s="7"/>
       <c r="G363" s="7"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
       <c r="F364" s="7"/>
       <c r="G364" s="7"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E365" s="7"/>
       <c r="F365" s="7"/>
       <c r="G365" s="7"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E366" s="7"/>
       <c r="F366" s="7"/>
       <c r="G366" s="7"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E367" s="7"/>
       <c r="F367" s="7"/>
       <c r="G367" s="7"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E368" s="7"/>
       <c r="F368" s="7"/>
       <c r="G368" s="7"/>
     </row>
-    <row r="369" spans="4:7">
+    <row r="369" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
       <c r="F369" s="7"/>
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:H362" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="LauraMancini99"/>
+        <filter val="Brainstorming"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
@aculsalocin @phigeit Thema gelöscht
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swmaende\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570251A4-67E0-4C81-950B-683BF99E88CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="609">
   <si>
     <t>Themen</t>
   </si>
@@ -1854,8 +1855,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2295,24 +2296,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B175" sqref="B175"/>
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="83.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2328,7 +2329,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2353,7 +2354,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2361,7 +2362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2369,7 +2370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2385,12 +2386,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2422,7 +2423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -2430,7 +2431,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2470,7 +2471,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2534,17 +2535,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -2608,12 +2609,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -2629,7 +2630,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -2654,7 +2655,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -2663,7 +2664,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2679,7 +2680,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -2687,7 +2688,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -2711,7 +2712,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -2735,17 +2736,17 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -2761,7 +2762,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>105</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>107</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>111</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>113</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>115</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>117</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>118</v>
       </c>
@@ -2825,12 +2826,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>121</v>
       </c>
@@ -2838,7 +2839,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>123</v>
       </c>
@@ -2846,7 +2847,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>125</v>
       </c>
@@ -2854,7 +2855,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>127</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>129</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>130</v>
       </c>
@@ -2878,7 +2879,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>132</v>
       </c>
@@ -2886,7 +2887,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>134</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>137</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>139</v>
       </c>
@@ -2918,7 +2919,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>140</v>
       </c>
@@ -2926,7 +2927,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>142</v>
       </c>
@@ -2934,7 +2935,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>144</v>
       </c>
@@ -2942,7 +2943,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>146</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>148</v>
       </c>
@@ -2958,7 +2959,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>150</v>
       </c>
@@ -2966,12 +2967,12 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>153</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>155</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>157</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>159</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>161</v>
       </c>
@@ -3011,7 +3012,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>162</v>
       </c>
@@ -3019,7 +3020,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>164</v>
       </c>
@@ -3027,7 +3028,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>166</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>168</v>
       </c>
@@ -3043,7 +3044,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>170</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>172</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>174</v>
       </c>
@@ -3067,7 +3068,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>176</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>178</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>180</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>182</v>
       </c>
@@ -3099,12 +3100,12 @@
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>185</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>187</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>189</v>
       </c>
@@ -3128,7 +3129,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>191</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>192</v>
       </c>
@@ -3145,7 +3146,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" hidden="1">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>193</v>
       </c>
@@ -3153,7 +3154,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>195</v>
       </c>
@@ -3161,7 +3162,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>197</v>
       </c>
@@ -3169,12 +3170,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>201</v>
       </c>
@@ -3182,7 +3183,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>203</v>
       </c>
@@ -3190,7 +3191,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>205</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>207</v>
       </c>
@@ -3206,7 +3207,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>209</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>211</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>213</v>
       </c>
@@ -3230,7 +3231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>214</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>215</v>
       </c>
@@ -3246,7 +3247,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>217</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>219</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>221</v>
       </c>
@@ -3270,7 +3271,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>223</v>
       </c>
@@ -3278,7 +3279,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>225</v>
       </c>
@@ -3286,7 +3287,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>227</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>229</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>231</v>
       </c>
@@ -3310,15 +3311,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>232</v>
       </c>
-      <c r="B128" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="16.5" hidden="1">
+    </row>
+    <row r="129" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>233</v>
       </c>
@@ -3326,12 +3324,12 @@
         <v>602</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>236</v>
       </c>
@@ -3339,7 +3337,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>238</v>
       </c>
@@ -3347,7 +3345,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>240</v>
       </c>
@@ -3355,7 +3353,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>241</v>
       </c>
@@ -3363,7 +3361,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>243</v>
       </c>
@@ -3371,7 +3369,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>245</v>
       </c>
@@ -3379,7 +3377,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>247</v>
       </c>
@@ -3387,7 +3385,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>248</v>
       </c>
@@ -3395,7 +3393,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>250</v>
       </c>
@@ -3403,7 +3401,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>251</v>
       </c>
@@ -3411,7 +3409,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>252</v>
       </c>
@@ -3419,12 +3417,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>255</v>
       </c>
@@ -3432,17 +3430,17 @@
         <v>228</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>259</v>
       </c>
@@ -3450,7 +3448,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>260</v>
       </c>
@@ -3458,7 +3456,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>261</v>
       </c>
@@ -3466,7 +3464,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>262</v>
       </c>
@@ -3474,7 +3472,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>264</v>
       </c>
@@ -3482,7 +3480,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>266</v>
       </c>
@@ -3490,7 +3488,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>268</v>
       </c>
@@ -3498,20 +3496,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>270</v>
       </c>
-      <c r="B154" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" hidden="1">
+    </row>
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>271</v>
       </c>
@@ -3519,7 +3514,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>272</v>
       </c>
@@ -3527,7 +3522,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>273</v>
       </c>
@@ -3535,7 +3530,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>274</v>
       </c>
@@ -3543,7 +3538,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>276</v>
       </c>
@@ -3551,7 +3546,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>278</v>
       </c>
@@ -3559,7 +3554,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>280</v>
       </c>
@@ -3567,7 +3562,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>282</v>
       </c>
@@ -3575,7 +3570,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>283</v>
       </c>
@@ -3583,7 +3578,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>285</v>
       </c>
@@ -3591,7 +3586,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>287</v>
       </c>
@@ -3599,7 +3594,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>288</v>
       </c>
@@ -3607,7 +3602,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>290</v>
       </c>
@@ -3615,7 +3610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>291</v>
       </c>
@@ -3623,7 +3618,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>292</v>
       </c>
@@ -3631,7 +3626,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>294</v>
       </c>
@@ -3639,7 +3634,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>296</v>
       </c>
@@ -3647,7 +3642,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>298</v>
       </c>
@@ -3655,7 +3650,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>299</v>
       </c>
@@ -3663,7 +3658,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>301</v>
       </c>
@@ -3671,12 +3666,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>305</v>
       </c>
@@ -3684,7 +3679,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>307</v>
       </c>
@@ -3692,7 +3687,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>309</v>
       </c>
@@ -3700,7 +3695,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>310</v>
       </c>
@@ -3708,17 +3703,17 @@
         <v>311</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>314</v>
       </c>
@@ -3726,7 +3721,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>316</v>
       </c>
@@ -3734,7 +3729,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>317</v>
       </c>
@@ -3742,7 +3737,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>319</v>
       </c>
@@ -3750,7 +3745,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>321</v>
       </c>
@@ -3758,12 +3753,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>323</v>
       </c>
@@ -3771,7 +3766,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>325</v>
       </c>
@@ -3779,7 +3774,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>327</v>
       </c>
@@ -3787,7 +3782,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>329</v>
       </c>
@@ -3795,7 +3790,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>330</v>
       </c>
@@ -3803,7 +3798,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>331</v>
       </c>
@@ -3811,7 +3806,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>333</v>
       </c>
@@ -3819,7 +3814,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>335</v>
       </c>
@@ -3827,12 +3822,12 @@
         <v>336</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>338</v>
       </c>
@@ -3840,7 +3835,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.5" hidden="1">
+    <row r="198" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
         <v>340</v>
       </c>
@@ -3848,7 +3843,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>342</v>
       </c>
@@ -3856,7 +3851,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>344</v>
       </c>
@@ -3864,7 +3859,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>346</v>
       </c>
@@ -3872,7 +3867,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>348</v>
       </c>
@@ -3880,7 +3875,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>350</v>
       </c>
@@ -3888,7 +3883,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>352</v>
       </c>
@@ -3896,7 +3891,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>354</v>
       </c>
@@ -3904,7 +3899,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>355</v>
       </c>
@@ -3912,7 +3907,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -3920,7 +3915,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>546</v>
       </c>
@@ -3928,7 +3923,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>359</v>
       </c>
@@ -3936,7 +3931,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>361</v>
       </c>
@@ -3944,7 +3939,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>363</v>
       </c>
@@ -3952,7 +3947,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>365</v>
       </c>
@@ -3960,7 +3955,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>367</v>
       </c>
@@ -3968,7 +3963,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>369</v>
       </c>
@@ -3976,7 +3971,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>371</v>
       </c>
@@ -3984,7 +3979,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>372</v>
       </c>
@@ -3992,7 +3987,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>374</v>
       </c>
@@ -4000,7 +3995,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="16.5" hidden="1">
+    <row r="218" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>376</v>
       </c>
@@ -4008,7 +4003,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>378</v>
       </c>
@@ -4016,7 +4011,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>379</v>
       </c>
@@ -4024,7 +4019,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>380</v>
       </c>
@@ -4032,7 +4027,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>382</v>
       </c>
@@ -4040,7 +4035,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>384</v>
       </c>
@@ -4048,7 +4043,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>386</v>
       </c>
@@ -4056,12 +4051,12 @@
         <v>387</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>389</v>
       </c>
@@ -4069,7 +4064,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>391</v>
       </c>
@@ -4077,7 +4072,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>393</v>
       </c>
@@ -4085,7 +4080,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>395</v>
       </c>
@@ -4093,7 +4088,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>397</v>
       </c>
@@ -4101,7 +4096,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>399</v>
       </c>
@@ -4109,7 +4104,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>400</v>
       </c>
@@ -4117,7 +4112,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>402</v>
       </c>
@@ -4125,7 +4120,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>403</v>
       </c>
@@ -4133,7 +4128,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>405</v>
       </c>
@@ -4141,7 +4136,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>406</v>
       </c>
@@ -4149,7 +4144,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>408</v>
       </c>
@@ -4157,7 +4152,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>410</v>
       </c>
@@ -4165,7 +4160,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>412</v>
       </c>
@@ -4173,7 +4168,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="16.5" hidden="1">
+    <row r="240" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
         <v>414</v>
       </c>
@@ -4181,7 +4176,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>415</v>
       </c>
@@ -4189,7 +4184,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>417</v>
       </c>
@@ -4197,7 +4192,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16.5" hidden="1">
+    <row r="243" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
         <v>419</v>
       </c>
@@ -4205,7 +4200,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>420</v>
       </c>
@@ -4213,7 +4208,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>422</v>
       </c>
@@ -4221,7 +4216,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>424</v>
       </c>
@@ -4229,7 +4224,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>426</v>
       </c>
@@ -4237,12 +4232,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>428</v>
       </c>
@@ -4250,7 +4245,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>430</v>
       </c>
@@ -4258,7 +4253,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>432</v>
       </c>
@@ -4266,7 +4261,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>434</v>
       </c>
@@ -4274,7 +4269,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>435</v>
       </c>
@@ -4282,7 +4277,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>437</v>
       </c>
@@ -4290,7 +4285,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>438</v>
       </c>
@@ -4298,7 +4293,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>439</v>
       </c>
@@ -4306,7 +4301,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="16.5" hidden="1">
+    <row r="257" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>440</v>
       </c>
@@ -4314,7 +4309,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>441</v>
       </c>
@@ -4322,7 +4317,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>442</v>
       </c>
@@ -4330,7 +4325,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1">
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>443</v>
       </c>
@@ -4338,7 +4333,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>445</v>
       </c>
@@ -4346,7 +4341,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>447</v>
       </c>
@@ -4354,7 +4349,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>449</v>
       </c>
@@ -4362,7 +4357,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>450</v>
       </c>
@@ -4370,7 +4365,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>452</v>
       </c>
@@ -4378,7 +4373,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>454</v>
       </c>
@@ -4386,7 +4381,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>456</v>
       </c>
@@ -4394,7 +4389,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="268" spans="1:2" hidden="1">
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>457</v>
       </c>
@@ -4402,7 +4397,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1">
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>458</v>
       </c>
@@ -4410,17 +4405,17 @@
         <v>459</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>462</v>
       </c>
@@ -4428,12 +4423,12 @@
         <v>593</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1">
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>464</v>
       </c>
@@ -4441,7 +4436,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>466</v>
       </c>
@@ -4449,12 +4444,12 @@
         <v>304</v>
       </c>
     </row>
-    <row r="276" spans="1:2" hidden="1">
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>468</v>
       </c>
@@ -4462,7 +4457,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>470</v>
       </c>
@@ -4470,7 +4465,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>472</v>
       </c>
@@ -4478,7 +4473,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>473</v>
       </c>
@@ -4486,7 +4481,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>474</v>
       </c>
@@ -4494,7 +4489,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>476</v>
       </c>
@@ -4502,7 +4497,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>477</v>
       </c>
@@ -4510,7 +4505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>478</v>
       </c>
@@ -4518,7 +4513,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1">
+    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>479</v>
       </c>
@@ -4526,7 +4521,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1">
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>480</v>
       </c>
@@ -4534,17 +4529,17 @@
         <v>345</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1">
+    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1">
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="16.5" hidden="1">
+    <row r="289" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>483</v>
       </c>
@@ -4552,7 +4547,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1">
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>484</v>
       </c>
@@ -4560,7 +4555,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1">
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>486</v>
       </c>
@@ -4568,7 +4563,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="292" spans="1:2" hidden="1">
+    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>487</v>
       </c>
@@ -4576,7 +4571,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1">
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>488</v>
       </c>
@@ -4584,7 +4579,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>489</v>
       </c>
@@ -4592,7 +4587,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1">
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>490</v>
       </c>
@@ -4600,12 +4595,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1">
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1">
+    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>492</v>
       </c>
@@ -4613,7 +4608,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1">
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>493</v>
       </c>
@@ -4621,7 +4616,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1">
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>494</v>
       </c>
@@ -4629,7 +4624,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1">
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>495</v>
       </c>
@@ -4637,7 +4632,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1">
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>497</v>
       </c>
@@ -4645,7 +4640,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1">
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>498</v>
       </c>
@@ -4653,12 +4648,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1">
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1">
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>500</v>
       </c>
@@ -4666,7 +4661,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>501</v>
       </c>
@@ -4674,7 +4669,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>502</v>
       </c>
@@ -4685,7 +4680,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>503</v>
       </c>
@@ -4693,7 +4688,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>504</v>
       </c>
@@ -4701,7 +4696,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>505</v>
       </c>
@@ -4709,7 +4704,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>506</v>
       </c>
@@ -4717,12 +4712,12 @@
         <v>507</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>509</v>
       </c>
@@ -4730,7 +4725,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>510</v>
       </c>
@@ -4738,7 +4733,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="314" spans="1:5" ht="16.5" hidden="1">
+    <row r="314" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A314" t="s">
         <v>511</v>
       </c>
@@ -4746,7 +4741,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>512</v>
       </c>
@@ -4754,7 +4749,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="16.5" hidden="1">
+    <row r="316" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A316" t="s">
         <v>513</v>
       </c>
@@ -4762,7 +4757,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1">
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>514</v>
       </c>
@@ -4770,7 +4765,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>515</v>
       </c>
@@ -4778,7 +4773,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>517</v>
       </c>
@@ -4786,7 +4781,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="16.5" hidden="1">
+    <row r="320" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A320" t="s">
         <v>607</v>
       </c>
@@ -4794,7 +4789,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1">
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>518</v>
       </c>
@@ -4802,7 +4797,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1">
+    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>519</v>
       </c>
@@ -4810,7 +4805,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1">
+    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>520</v>
       </c>
@@ -4818,7 +4813,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1">
+    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>522</v>
       </c>
@@ -4826,7 +4821,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1">
+    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>523</v>
       </c>
@@ -4834,7 +4829,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1">
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>524</v>
       </c>
@@ -4842,7 +4837,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16.5" hidden="1">
+    <row r="327" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
         <v>545</v>
       </c>
@@ -4850,7 +4845,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1">
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>525</v>
       </c>
@@ -4858,7 +4853,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1">
+    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>526</v>
       </c>
@@ -4866,7 +4861,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1">
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
         <v>527</v>
       </c>
@@ -4874,7 +4869,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1">
+    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
         <v>529</v>
       </c>
@@ -4882,7 +4877,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="332" spans="1:2" hidden="1">
+    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
         <v>530</v>
       </c>
@@ -4890,7 +4885,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1">
+    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>531</v>
       </c>
@@ -4898,7 +4893,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="334" spans="1:2" hidden="1">
+    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>532</v>
       </c>
@@ -4906,7 +4901,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="335" spans="1:2" hidden="1">
+    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>533</v>
       </c>
@@ -4914,7 +4909,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="336" spans="1:2" hidden="1">
+    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>534</v>
       </c>
@@ -4922,7 +4917,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="337" spans="1:7" hidden="1">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>536</v>
       </c>
@@ -4930,7 +4925,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>538</v>
       </c>
@@ -4938,7 +4933,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="339" spans="1:7" hidden="1">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>540</v>
       </c>
@@ -4946,7 +4941,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="340" spans="1:7" hidden="1">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>542</v>
       </c>
@@ -4954,7 +4949,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="341" spans="1:7" hidden="1">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>544</v>
       </c>
@@ -4962,7 +4957,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>568</v>
       </c>
@@ -4970,7 +4965,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="343" spans="1:7" hidden="1">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>563</v>
       </c>
@@ -4978,7 +4973,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="344" spans="1:7" hidden="1">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>567</v>
       </c>
@@ -4986,7 +4981,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1">
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>564</v>
       </c>
@@ -4994,7 +4989,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1">
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>565</v>
       </c>
@@ -5002,7 +4997,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>566</v>
       </c>
@@ -5010,7 +5005,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1">
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>569</v>
       </c>
@@ -5018,7 +5013,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1">
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>570</v>
       </c>
@@ -5026,7 +5021,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="17.25" hidden="1">
+    <row r="350" spans="1:7" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>571</v>
       </c>
@@ -5038,7 +5033,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7" hidden="1">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>572</v>
       </c>
@@ -5050,7 +5045,7 @@
       <c r="F351" s="7"/>
       <c r="G351" s="7"/>
     </row>
-    <row r="352" spans="1:7" hidden="1">
+    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>573</v>
       </c>
@@ -5059,7 +5054,7 @@
       <c r="F352" s="7"/>
       <c r="G352" s="7"/>
     </row>
-    <row r="353" spans="1:7" hidden="1">
+    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>574</v>
       </c>
@@ -5070,7 +5065,7 @@
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7" hidden="1">
+    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>575</v>
       </c>
@@ -5081,7 +5076,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7" hidden="1">
+    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>576</v>
       </c>
@@ -5092,7 +5087,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.5" hidden="1">
+    <row r="356" spans="1:7" ht="19.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
         <v>577</v>
       </c>
@@ -5104,7 +5099,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7" hidden="1">
+    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>578</v>
       </c>
@@ -5116,7 +5111,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7" hidden="1">
+    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>579</v>
       </c>
@@ -5127,7 +5122,7 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7" hidden="1">
+    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>580</v>
       </c>
@@ -5138,7 +5133,7 @@
       <c r="F359" s="7"/>
       <c r="G359" s="7"/>
     </row>
-    <row r="360" spans="1:7" hidden="1">
+    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>581</v>
       </c>
@@ -5149,7 +5144,7 @@
       <c r="F360" s="7"/>
       <c r="G360" s="7"/>
     </row>
-    <row r="361" spans="1:7" hidden="1">
+    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>583</v>
       </c>
@@ -5160,7 +5155,7 @@
       <c r="F361" s="7"/>
       <c r="G361" s="7"/>
     </row>
-    <row r="362" spans="1:7" hidden="1">
+    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>582</v>
       </c>
@@ -5168,48 +5163,48 @@
       <c r="F362" s="7"/>
       <c r="G362" s="7"/>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E363" s="7"/>
       <c r="F363" s="7"/>
       <c r="G363" s="7"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
       <c r="F364" s="7"/>
       <c r="G364" s="7"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E365" s="7"/>
       <c r="F365" s="7"/>
       <c r="G365" s="7"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E366" s="7"/>
       <c r="F366" s="7"/>
       <c r="G366" s="7"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E367" s="7"/>
       <c r="F367" s="7"/>
       <c r="G367" s="7"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E368" s="7"/>
       <c r="F368" s="7"/>
       <c r="G368" s="7"/>
     </row>
-    <row r="369" spans="4:7">
+    <row r="369" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
       <c r="F369" s="7"/>
       <c r="G369" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H362">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:H362" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="ebressel"/>
+        <filter val="Compliance_im_Projektmanagment"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5219,9 +5214,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5428,19 +5426,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5465,9 +5459,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Leni2502, jessymrc, FAUdennis96, Christoph-Mantsch
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189E305-C67A-4D4B-925A-CE983FA1913D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B88B16D-643F-485A-B39C-3CA18DD037E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="608">
   <si>
     <t>Themen</t>
   </si>
@@ -914,9 +914,6 @@
   </si>
   <si>
     <t>Projektumfang</t>
-  </si>
-  <si>
-    <t>jessymrc</t>
   </si>
   <si>
     <t>Jour_Fixe</t>
@@ -2301,7 +2298,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B317" sqref="B317"/>
+      <selection activeCell="B366" sqref="B366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2550,7 +2547,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -2643,7 +2640,7 @@
         <v>79</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2685,7 +2682,7 @@
         <v>87</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2868,7 +2865,7 @@
         <v>129</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3316,7 +3313,7 @@
         <v>232</v>
       </c>
       <c r="B128" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
@@ -3324,7 +3321,7 @@
         <v>233</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3385,7 +3382,7 @@
         <v>247</v>
       </c>
       <c r="B137" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3401,7 +3398,7 @@
         <v>250</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3409,7 +3406,7 @@
         <v>251</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3456,7 +3453,7 @@
         <v>260</v>
       </c>
       <c r="B147" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3464,7 +3461,7 @@
         <v>261</v>
       </c>
       <c r="B148" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3530,7 +3527,7 @@
         <v>273</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3570,7 +3567,7 @@
         <v>282</v>
       </c>
       <c r="B162" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -3641,13 +3638,10 @@
       <c r="A171" t="s">
         <v>296</v>
       </c>
-      <c r="B171" t="s">
-        <v>297</v>
-      </c>
     </row>
     <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B172" t="s">
         <v>249</v>
@@ -3655,44 +3649,44 @@
     </row>
     <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>298</v>
+      </c>
+      <c r="B173" t="s">
         <v>299</v>
-      </c>
-      <c r="B173" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>300</v>
+      </c>
+      <c r="B174" t="s">
         <v>301</v>
-      </c>
-      <c r="B174" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
+        <v>304</v>
+      </c>
+      <c r="B176" t="s">
         <v>305</v>
-      </c>
-      <c r="B176" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>306</v>
+      </c>
+      <c r="B177" t="s">
         <v>307</v>
-      </c>
-      <c r="B177" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B178" t="s">
         <v>263</v>
@@ -3700,33 +3694,33 @@
     </row>
     <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>309</v>
+      </c>
+      <c r="B179" t="s">
         <v>310</v>
-      </c>
-      <c r="B179" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
+        <v>313</v>
+      </c>
+      <c r="B182" t="s">
         <v>314</v>
-      </c>
-      <c r="B182" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B183" t="s">
         <v>257</v>
@@ -3734,23 +3728,23 @@
     </row>
     <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>316</v>
+      </c>
+      <c r="B184" t="s">
         <v>317</v>
-      </c>
-      <c r="B184" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>318</v>
+      </c>
+      <c r="B185" t="s">
         <v>319</v>
-      </c>
-      <c r="B185" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B186" t="s">
         <v>222</v>
@@ -3758,44 +3752,44 @@
     </row>
     <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
+        <v>322</v>
+      </c>
+      <c r="B188" t="s">
         <v>323</v>
-      </c>
-      <c r="B188" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
+        <v>324</v>
+      </c>
+      <c r="B189" t="s">
         <v>325</v>
-      </c>
-      <c r="B189" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>326</v>
+      </c>
+      <c r="B190" t="s">
         <v>327</v>
-      </c>
-      <c r="B190" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B191" s="10" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B192" t="s">
         <v>244</v>
@@ -3803,100 +3797,100 @@
     </row>
     <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>330</v>
+      </c>
+      <c r="B193" t="s">
         <v>331</v>
-      </c>
-      <c r="B193" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
+        <v>332</v>
+      </c>
+      <c r="B194" t="s">
         <v>333</v>
-      </c>
-      <c r="B194" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>334</v>
+      </c>
+      <c r="B195" t="s">
         <v>335</v>
-      </c>
-      <c r="B195" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>337</v>
+      </c>
+      <c r="B197" t="s">
         <v>338</v>
-      </c>
-      <c r="B197" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
+        <v>339</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>340</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>341</v>
+      </c>
+      <c r="B199" t="s">
         <v>342</v>
-      </c>
-      <c r="B199" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
+        <v>343</v>
+      </c>
+      <c r="B200" t="s">
         <v>344</v>
-      </c>
-      <c r="B200" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>345</v>
+      </c>
+      <c r="B201" t="s">
         <v>346</v>
-      </c>
-      <c r="B201" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>347</v>
+      </c>
+      <c r="B202" t="s">
         <v>348</v>
-      </c>
-      <c r="B202" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
+        <v>349</v>
+      </c>
+      <c r="B203" t="s">
         <v>350</v>
-      </c>
-      <c r="B203" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>351</v>
+      </c>
+      <c r="B204" t="s">
         <v>352</v>
-      </c>
-      <c r="B204" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B205" t="s">
         <v>96</v>
@@ -3904,23 +3898,23 @@
     </row>
     <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>354</v>
+      </c>
+      <c r="B206" t="s">
         <v>355</v>
-      </c>
-      <c r="B206" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>356</v>
+      </c>
+      <c r="B207" t="s">
         <v>357</v>
-      </c>
-      <c r="B207" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B208" t="s">
         <v>242</v>
@@ -3928,55 +3922,55 @@
     </row>
     <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>358</v>
+      </c>
+      <c r="B209" t="s">
         <v>359</v>
-      </c>
-      <c r="B209" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>360</v>
+      </c>
+      <c r="B210" t="s">
         <v>361</v>
-      </c>
-      <c r="B210" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>362</v>
+      </c>
+      <c r="B211" t="s">
         <v>363</v>
-      </c>
-      <c r="B211" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
+        <v>364</v>
+      </c>
+      <c r="B212" t="s">
         <v>365</v>
-      </c>
-      <c r="B212" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
+        <v>366</v>
+      </c>
+      <c r="B213" t="s">
         <v>367</v>
-      </c>
-      <c r="B213" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
+        <v>368</v>
+      </c>
+      <c r="B214" t="s">
         <v>369</v>
-      </c>
-      <c r="B214" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B215" t="s">
         <v>237</v>
@@ -3984,31 +3978,31 @@
     </row>
     <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>371</v>
+      </c>
+      <c r="B216" t="s">
         <v>372</v>
-      </c>
-      <c r="B216" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
+        <v>373</v>
+      </c>
+      <c r="B217" t="s">
         <v>374</v>
-      </c>
-      <c r="B217" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B219" t="s">
         <v>177</v>
@@ -4016,220 +4010,220 @@
     </row>
     <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
+        <v>379</v>
+      </c>
+      <c r="B221" t="s">
         <v>380</v>
-      </c>
-      <c r="B221" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
+        <v>381</v>
+      </c>
+      <c r="B222" t="s">
         <v>382</v>
-      </c>
-      <c r="B222" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>383</v>
+      </c>
+      <c r="B223" t="s">
         <v>384</v>
-      </c>
-      <c r="B223" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>385</v>
+      </c>
+      <c r="B224" t="s">
         <v>386</v>
-      </c>
-      <c r="B224" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>388</v>
+      </c>
+      <c r="B226" t="s">
         <v>389</v>
-      </c>
-      <c r="B226" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>390</v>
+      </c>
+      <c r="B227" t="s">
         <v>391</v>
-      </c>
-      <c r="B227" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>392</v>
+      </c>
+      <c r="B228" t="s">
         <v>393</v>
-      </c>
-      <c r="B228" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>394</v>
+      </c>
+      <c r="B229" t="s">
         <v>395</v>
-      </c>
-      <c r="B229" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>396</v>
+      </c>
+      <c r="B230" t="s">
         <v>397</v>
-      </c>
-      <c r="B230" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B231" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>399</v>
+      </c>
+      <c r="B232" t="s">
         <v>400</v>
-      </c>
-      <c r="B232" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B233" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
+        <v>402</v>
+      </c>
+      <c r="B234" t="s">
         <v>403</v>
-      </c>
-      <c r="B234" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B235" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>405</v>
+      </c>
+      <c r="B236" t="s">
         <v>406</v>
-      </c>
-      <c r="B236" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
+        <v>407</v>
+      </c>
+      <c r="B237" t="s">
         <v>408</v>
-      </c>
-      <c r="B237" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>409</v>
+      </c>
+      <c r="B238" t="s">
         <v>410</v>
-      </c>
-      <c r="B238" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>411</v>
+      </c>
+      <c r="B239" t="s">
         <v>412</v>
-      </c>
-      <c r="B239" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
+        <v>414</v>
+      </c>
+      <c r="B241" t="s">
         <v>415</v>
-      </c>
-      <c r="B241" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>416</v>
+      </c>
+      <c r="B242" t="s">
         <v>417</v>
-      </c>
-      <c r="B242" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
+        <v>419</v>
+      </c>
+      <c r="B244" t="s">
         <v>420</v>
-      </c>
-      <c r="B244" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
+        <v>421</v>
+      </c>
+      <c r="B245" t="s">
         <v>422</v>
-      </c>
-      <c r="B245" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>423</v>
+      </c>
+      <c r="B246" t="s">
         <v>424</v>
-      </c>
-      <c r="B246" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B247" t="s">
         <v>36</v>
@@ -4237,68 +4231,68 @@
     </row>
     <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
+        <v>427</v>
+      </c>
+      <c r="B249" t="s">
         <v>428</v>
-      </c>
-      <c r="B249" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
+        <v>429</v>
+      </c>
+      <c r="B250" t="s">
         <v>430</v>
-      </c>
-      <c r="B250" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
+        <v>431</v>
+      </c>
+      <c r="B251" t="s">
         <v>432</v>
-      </c>
-      <c r="B251" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B252" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
+        <v>434</v>
+      </c>
+      <c r="B253" t="s">
         <v>435</v>
-      </c>
-      <c r="B253" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B254" s="10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B255" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B256" t="s">
         <v>234</v>
@@ -4306,92 +4300,92 @@
     </row>
     <row r="257" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B258" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
+        <v>442</v>
+      </c>
+      <c r="B260" t="s">
         <v>443</v>
-      </c>
-      <c r="B260" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
+        <v>444</v>
+      </c>
+      <c r="B261" t="s">
         <v>445</v>
-      </c>
-      <c r="B261" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
+        <v>446</v>
+      </c>
+      <c r="B262" t="s">
         <v>447</v>
-      </c>
-      <c r="B262" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B263" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
+        <v>450</v>
+      </c>
+      <c r="B265" t="s">
         <v>451</v>
-      </c>
-      <c r="B265" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
+        <v>452</v>
+      </c>
+      <c r="B266" t="s">
         <v>453</v>
-      </c>
-      <c r="B266" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B267" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B268" t="s">
         <v>246</v>
@@ -4399,75 +4393,75 @@
     </row>
     <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
+        <v>456</v>
+      </c>
+      <c r="B269" t="s">
         <v>457</v>
-      </c>
-      <c r="B269" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
+        <v>462</v>
+      </c>
+      <c r="B274" t="s">
         <v>463</v>
-      </c>
-      <c r="B274" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B275" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
+        <v>466</v>
+      </c>
+      <c r="B277" t="s">
         <v>467</v>
-      </c>
-      <c r="B277" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
+        <v>468</v>
+      </c>
+      <c r="B278" t="s">
         <v>469</v>
-      </c>
-      <c r="B278" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B279" t="s">
         <v>293</v>
@@ -4475,23 +4469,23 @@
     </row>
     <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B280" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
+        <v>472</v>
+      </c>
+      <c r="B281" t="s">
         <v>473</v>
-      </c>
-      <c r="B281" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B282" t="s">
         <v>122</v>
@@ -4499,7 +4493,7 @@
     </row>
     <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B283" t="s">
         <v>5</v>
@@ -4507,7 +4501,7 @@
     </row>
     <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B284" t="s">
         <v>128</v>
@@ -4515,57 +4509,57 @@
     </row>
     <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B286" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B289" s="12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
+        <v>482</v>
+      </c>
+      <c r="B290" t="s">
         <v>483</v>
-      </c>
-      <c r="B290" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B291" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B292" t="s">
         <v>198</v>
@@ -4573,15 +4567,12 @@
     </row>
     <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>487</v>
-      </c>
-      <c r="B293" t="s">
-        <v>138</v>
+        <v>486</v>
       </c>
     </row>
     <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B294" t="s">
         <v>112</v>
@@ -4589,28 +4580,28 @@
     </row>
     <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B295" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B298" t="s">
         <v>84</v>
@@ -4618,23 +4609,23 @@
     </row>
     <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B299" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
+        <v>493</v>
+      </c>
+      <c r="B300" t="s">
         <v>494</v>
-      </c>
-      <c r="B300" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B301" t="s">
         <v>202</v>
@@ -4642,7 +4633,7 @@
     </row>
     <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B302" t="s">
         <v>119</v>
@@ -4650,39 +4641,33 @@
     </row>
     <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>499</v>
-      </c>
-      <c r="B304" t="s">
-        <v>297</v>
+        <v>498</v>
       </c>
     </row>
     <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>500</v>
-      </c>
-      <c r="B305" t="s">
-        <v>66</v>
+        <v>499</v>
       </c>
     </row>
     <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E306" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B307" t="s">
         <v>114</v>
@@ -4690,7 +4675,7 @@
     </row>
     <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B308" t="s">
         <v>40</v>
@@ -4698,28 +4683,28 @@
     </row>
     <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B309" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
+        <v>504</v>
+      </c>
+      <c r="B310" t="s">
         <v>505</v>
-      </c>
-      <c r="B310" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B312" t="s">
         <v>110</v>
@@ -4727,23 +4712,23 @@
     </row>
     <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B313" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="314" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A314" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B315" t="s">
         <v>267</v>
@@ -4751,28 +4736,28 @@
     </row>
     <row r="316" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A316" t="s">
+        <v>511</v>
+      </c>
+      <c r="B316" s="13" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
         <v>512</v>
-      </c>
-      <c r="B316" s="13" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A317" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
+        <v>513</v>
+      </c>
+      <c r="B318" t="s">
         <v>514</v>
-      </c>
-      <c r="B318" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>151</v>
@@ -4780,15 +4765,15 @@
     </row>
     <row r="320" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A320" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B321" t="s">
         <v>175</v>
@@ -4796,7 +4781,7 @@
     </row>
     <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B322" t="s">
         <v>42</v>
@@ -4804,31 +4789,31 @@
     </row>
     <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
+        <v>518</v>
+      </c>
+      <c r="B323" t="s">
         <v>519</v>
-      </c>
-      <c r="B323" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B324" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B325" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B326" t="s">
         <v>135</v>
@@ -4836,23 +4821,23 @@
     </row>
     <row r="327" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B328" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B329" t="s">
         <v>60</v>
@@ -4860,31 +4845,31 @@
     </row>
     <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B330" t="s">
         <v>526</v>
-      </c>
-      <c r="B330" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B331" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B332" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B333" t="s">
         <v>80</v>
@@ -4892,138 +4877,136 @@
     </row>
     <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B334" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B335" s="10" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
+        <v>532</v>
+      </c>
+      <c r="B336" t="s">
         <v>533</v>
-      </c>
-      <c r="B336" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
+        <v>534</v>
+      </c>
+      <c r="B337" t="s">
         <v>535</v>
-      </c>
-      <c r="B337" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
+        <v>536</v>
+      </c>
+      <c r="B338" t="s">
         <v>537</v>
-      </c>
-      <c r="B338" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
+        <v>538</v>
+      </c>
+      <c r="B339" t="s">
         <v>539</v>
-      </c>
-      <c r="B339" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
+        <v>540</v>
+      </c>
+      <c r="B340" t="s">
         <v>541</v>
-      </c>
-      <c r="B340" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B341" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>562</v>
-      </c>
-      <c r="B343" s="7" t="s">
-        <v>474</v>
-      </c>
+        <v>561</v>
+      </c>
+      <c r="B343" s="7"/>
     </row>
     <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B344" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B347" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B349" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B350" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D350" s="7"/>
       <c r="E350" s="7"/>
@@ -5032,10 +5015,10 @@
     </row>
     <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B351" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D351" s="7"/>
       <c r="E351" s="7"/>
@@ -5044,7 +5027,7 @@
     </row>
     <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B352" s="7"/>
       <c r="E352" s="7"/>
@@ -5053,10 +5036,10 @@
     </row>
     <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B353" s="10" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
@@ -5064,10 +5047,10 @@
     </row>
     <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B354" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E354" s="7"/>
       <c r="F354" s="7"/>
@@ -5075,10 +5058,10 @@
     </row>
     <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B355" s="7" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E355" s="7"/>
       <c r="F355" s="7"/>
@@ -5086,10 +5069,10 @@
     </row>
     <row r="356" spans="1:7" ht="19.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D356" s="8"/>
       <c r="E356" s="7"/>
@@ -5098,10 +5081,10 @@
     </row>
     <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B357" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D357" s="7"/>
       <c r="E357" s="7"/>
@@ -5110,10 +5093,10 @@
     </row>
     <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E358" s="7"/>
       <c r="F358" s="7"/>
@@ -5121,10 +5104,10 @@
     </row>
     <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E359" s="7"/>
       <c r="F359" s="7"/>
@@ -5132,10 +5115,10 @@
     </row>
     <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B360" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="E360" s="7"/>
       <c r="F360" s="7"/>
@@ -5143,10 +5126,10 @@
     </row>
     <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B361" s="10" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E361" s="7"/>
       <c r="F361" s="7"/>
@@ -5154,7 +5137,7 @@
     </row>
     <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E362" s="7"/>
       <c r="F362" s="7"/>
@@ -5199,9 +5182,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H362" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
+    <filterColumn colId="1">
       <filters>
-        <filter val="Burndown_Chart"/>
+        <filter val="Leni2505"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5211,12 +5194,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5423,15 +5403,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5456,10 +5440,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
oh43ebet jy59zadi larass12 jackDS008
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE33690-9EA3-4611-A5B5-6E1F74C893B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85D04FE-7E19-4C25-A040-8A6C12EAC596}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="606">
   <si>
     <t>Themen</t>
   </si>
@@ -649,9 +649,6 @@
     <t>Bar_Camp</t>
   </si>
   <si>
-    <t>jackDS008</t>
-  </si>
-  <si>
     <t>Walt_Disney_Methode</t>
   </si>
   <si>
@@ -1232,9 +1229,6 @@
   </si>
   <si>
     <t>Project_Canvas</t>
-  </si>
-  <si>
-    <t>larass12</t>
   </si>
   <si>
     <t>Projektstrukturplan</t>
@@ -2307,7 +2301,7 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B365" sqref="B365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2351,7 +2345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2501,7 +2495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2553,7 +2547,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -2646,7 +2640,7 @@
         <v>79</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2688,7 +2682,7 @@
         <v>87</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2871,7 +2865,7 @@
         <v>129</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -2886,9 +2880,6 @@
       <c r="A73" t="s">
         <v>132</v>
       </c>
-      <c r="B73" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -3206,29 +3197,26 @@
       <c r="A114" t="s">
         <v>207</v>
       </c>
-      <c r="B114" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
+        <v>208</v>
+      </c>
+      <c r="B115" t="s">
         <v>209</v>
-      </c>
-      <c r="B115" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>210</v>
+      </c>
+      <c r="B116" t="s">
         <v>211</v>
-      </c>
-      <c r="B116" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B117" t="s">
         <v>20</v>
@@ -3236,7 +3224,7 @@
     </row>
     <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B118" t="s">
         <v>80</v>
@@ -3244,71 +3232,71 @@
     </row>
     <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>214</v>
+      </c>
+      <c r="B119" t="s">
         <v>215</v>
-      </c>
-      <c r="B119" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>216</v>
+      </c>
+      <c r="B120" t="s">
         <v>217</v>
-      </c>
-      <c r="B120" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>218</v>
+      </c>
+      <c r="B121" t="s">
         <v>219</v>
-      </c>
-      <c r="B121" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>220</v>
+      </c>
+      <c r="B122" t="s">
         <v>221</v>
-      </c>
-      <c r="B122" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B123" t="s">
         <v>223</v>
-      </c>
-      <c r="B123" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>224</v>
+      </c>
+      <c r="B124" t="s">
         <v>225</v>
-      </c>
-      <c r="B124" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>226</v>
+      </c>
+      <c r="B125" t="s">
         <v>227</v>
-      </c>
-      <c r="B125" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>228</v>
+      </c>
+      <c r="B126" t="s">
         <v>229</v>
-      </c>
-      <c r="B126" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B127" t="s">
         <v>200</v>
@@ -3316,136 +3304,136 @@
     </row>
     <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B128" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
+        <v>235</v>
+      </c>
+      <c r="B131" t="s">
         <v>236</v>
-      </c>
-      <c r="B131" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
+        <v>237</v>
+      </c>
+      <c r="B132" t="s">
         <v>238</v>
-      </c>
-      <c r="B132" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>240</v>
+      </c>
+      <c r="B134" t="s">
         <v>241</v>
-      </c>
-      <c r="B134" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
+        <v>242</v>
+      </c>
+      <c r="B135" t="s">
         <v>243</v>
-      </c>
-      <c r="B135" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>244</v>
+      </c>
+      <c r="B136" t="s">
         <v>245</v>
-      </c>
-      <c r="B136" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B137" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>247</v>
+      </c>
+      <c r="B138" t="s">
         <v>248</v>
-      </c>
-      <c r="B138" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>251</v>
+      </c>
+      <c r="B141" t="s">
         <v>252</v>
-      </c>
-      <c r="B141" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B143" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B146" t="s">
         <v>160</v>
@@ -3453,47 +3441,47 @@
     </row>
     <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B147" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B148" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>261</v>
+      </c>
+      <c r="B149" t="s">
         <v>262</v>
-      </c>
-      <c r="B149" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
+        <v>263</v>
+      </c>
+      <c r="B150" t="s">
         <v>264</v>
-      </c>
-      <c r="B150" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
+        <v>265</v>
+      </c>
+      <c r="B151" t="s">
         <v>266</v>
-      </c>
-      <c r="B151" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B152" t="s">
         <v>89</v>
@@ -3501,25 +3489,25 @@
     </row>
     <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B155" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B156" t="s">
         <v>44</v>
@@ -3527,71 +3515,71 @@
     </row>
     <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
+        <v>273</v>
+      </c>
+      <c r="B158" t="s">
         <v>274</v>
-      </c>
-      <c r="B158" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>275</v>
+      </c>
+      <c r="B159" t="s">
         <v>276</v>
-      </c>
-      <c r="B159" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>277</v>
+      </c>
+      <c r="B160" t="s">
         <v>278</v>
-      </c>
-      <c r="B160" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
+        <v>279</v>
+      </c>
+      <c r="B161" t="s">
         <v>280</v>
-      </c>
-      <c r="B161" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B162" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B163" t="s">
         <v>283</v>
-      </c>
-      <c r="B163" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>284</v>
+      </c>
+      <c r="B164" t="s">
         <v>285</v>
-      </c>
-      <c r="B164" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B165" t="s">
         <v>94</v>
@@ -3599,23 +3587,20 @@
     </row>
     <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>287</v>
+      </c>
+      <c r="B166" t="s">
         <v>288</v>
       </c>
-      <c r="B166" t="s">
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>290</v>
-      </c>
-      <c r="B167" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B168" t="s">
         <v>186</v>
@@ -3623,277 +3608,277 @@
     </row>
     <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>291</v>
+      </c>
+      <c r="B169" t="s">
         <v>292</v>
-      </c>
-      <c r="B169" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
+        <v>293</v>
+      </c>
+      <c r="B170" t="s">
         <v>294</v>
-      </c>
-      <c r="B170" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B172" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>297</v>
+      </c>
+      <c r="B173" t="s">
         <v>298</v>
-      </c>
-      <c r="B173" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
+        <v>299</v>
+      </c>
+      <c r="B174" t="s">
         <v>300</v>
-      </c>
-      <c r="B174" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
+        <v>303</v>
+      </c>
+      <c r="B176" t="s">
         <v>304</v>
-      </c>
-      <c r="B176" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>305</v>
+      </c>
+      <c r="B177" t="s">
         <v>306</v>
-      </c>
-      <c r="B177" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B178" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>308</v>
+      </c>
+      <c r="B179" t="s">
         <v>309</v>
-      </c>
-      <c r="B179" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
+        <v>312</v>
+      </c>
+      <c r="B182" t="s">
         <v>313</v>
-      </c>
-      <c r="B182" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B183" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>315</v>
+      </c>
+      <c r="B184" t="s">
         <v>316</v>
-      </c>
-      <c r="B184" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>317</v>
+      </c>
+      <c r="B185" t="s">
         <v>318</v>
-      </c>
-      <c r="B185" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B186" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
+        <v>321</v>
+      </c>
+      <c r="B188" t="s">
         <v>322</v>
-      </c>
-      <c r="B188" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
+        <v>323</v>
+      </c>
+      <c r="B189" t="s">
         <v>324</v>
-      </c>
-      <c r="B189" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>325</v>
+      </c>
+      <c r="B190" t="s">
         <v>326</v>
-      </c>
-      <c r="B190" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B191" s="10" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B192" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>329</v>
+      </c>
+      <c r="B193" t="s">
         <v>330</v>
-      </c>
-      <c r="B193" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
+        <v>331</v>
+      </c>
+      <c r="B194" t="s">
         <v>332</v>
-      </c>
-      <c r="B194" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
+        <v>333</v>
+      </c>
+      <c r="B195" t="s">
         <v>334</v>
-      </c>
-      <c r="B195" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>336</v>
+      </c>
+      <c r="B197" t="s">
         <v>337</v>
-      </c>
-      <c r="B197" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
+        <v>338</v>
+      </c>
+      <c r="B198" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>340</v>
+      </c>
+      <c r="B199" t="s">
         <v>341</v>
-      </c>
-      <c r="B199" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
+        <v>342</v>
+      </c>
+      <c r="B200" t="s">
         <v>343</v>
-      </c>
-      <c r="B200" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>344</v>
+      </c>
+      <c r="B201" t="s">
         <v>345</v>
-      </c>
-      <c r="B201" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
+        <v>346</v>
+      </c>
+      <c r="B202" t="s">
         <v>347</v>
-      </c>
-      <c r="B202" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
+        <v>348</v>
+      </c>
+      <c r="B203" t="s">
         <v>349</v>
-      </c>
-      <c r="B203" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>350</v>
+      </c>
+      <c r="B204" t="s">
         <v>351</v>
-      </c>
-      <c r="B204" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B205" t="s">
         <v>96</v>
@@ -3901,111 +3886,111 @@
     </row>
     <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>353</v>
+      </c>
+      <c r="B206" t="s">
         <v>354</v>
-      </c>
-      <c r="B206" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>355</v>
+      </c>
+      <c r="B207" t="s">
         <v>356</v>
-      </c>
-      <c r="B207" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B208" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>357</v>
+      </c>
+      <c r="B209" t="s">
         <v>358</v>
-      </c>
-      <c r="B209" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>359</v>
+      </c>
+      <c r="B210" t="s">
         <v>360</v>
-      </c>
-      <c r="B210" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>361</v>
+      </c>
+      <c r="B211" t="s">
         <v>362</v>
-      </c>
-      <c r="B211" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
+        <v>363</v>
+      </c>
+      <c r="B212" t="s">
         <v>364</v>
-      </c>
-      <c r="B212" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
+        <v>365</v>
+      </c>
+      <c r="B213" t="s">
         <v>366</v>
-      </c>
-      <c r="B213" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
+        <v>367</v>
+      </c>
+      <c r="B214" t="s">
         <v>368</v>
-      </c>
-      <c r="B214" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B215" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>370</v>
+      </c>
+      <c r="B216" t="s">
         <v>371</v>
-      </c>
-      <c r="B216" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
+        <v>372</v>
+      </c>
+      <c r="B217" t="s">
         <v>373</v>
-      </c>
-      <c r="B217" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B219" t="s">
         <v>177</v>
@@ -4013,220 +3998,217 @@
     </row>
     <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B220" s="10" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
+        <v>378</v>
+      </c>
+      <c r="B221" t="s">
         <v>379</v>
-      </c>
-      <c r="B221" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
+        <v>380</v>
+      </c>
+      <c r="B222" t="s">
         <v>381</v>
-      </c>
-      <c r="B222" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
+        <v>382</v>
+      </c>
+      <c r="B223" t="s">
         <v>383</v>
-      </c>
-      <c r="B223" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
+        <v>384</v>
+      </c>
+      <c r="B224" t="s">
         <v>385</v>
-      </c>
-      <c r="B224" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
+        <v>387</v>
+      </c>
+      <c r="B226" t="s">
         <v>388</v>
-      </c>
-      <c r="B226" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
+        <v>389</v>
+      </c>
+      <c r="B227" t="s">
         <v>390</v>
-      </c>
-      <c r="B227" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
+        <v>391</v>
+      </c>
+      <c r="B228" t="s">
         <v>392</v>
-      </c>
-      <c r="B228" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
+        <v>393</v>
+      </c>
+      <c r="B229" t="s">
         <v>394</v>
-      </c>
-      <c r="B229" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
+        <v>395</v>
+      </c>
+      <c r="B230" t="s">
         <v>396</v>
-      </c>
-      <c r="B230" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B231" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
+        <v>398</v>
+      </c>
+      <c r="B232" t="s">
         <v>399</v>
-      </c>
-      <c r="B232" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B233" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>402</v>
-      </c>
-      <c r="B234" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B235" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B236" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B237" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B238" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B239" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B241" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B242" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B244" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B245" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B246" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B247" t="s">
         <v>36</v>
@@ -4234,245 +4216,245 @@
     </row>
     <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B249" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B250" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B251" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B252" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B253" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B254" s="10" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B255" s="11" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B256" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B258" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B260" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B261" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B262" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B263" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B265" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B266" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B267" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B268" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B269" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B272" s="10" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B274" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B275" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B277" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B278" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B279" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B280" t="s">
         <v>133</v>
@@ -4480,15 +4462,15 @@
     </row>
     <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B281" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B282" t="s">
         <v>122</v>
@@ -4496,7 +4478,7 @@
     </row>
     <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B283" t="s">
         <v>5</v>
@@ -4504,7 +4486,7 @@
     </row>
     <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B284" t="s">
         <v>128</v>
@@ -4512,54 +4494,54 @@
     </row>
     <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B285" s="7" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B289" s="12" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B290" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B291" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B292" t="s">
         <v>198</v>
@@ -4567,7 +4549,7 @@
     </row>
     <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B293" s="14" t="s">
         <v>173</v>
@@ -4575,33 +4557,33 @@
     </row>
     <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B295" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B297" s="7" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B298" t="s">
         <v>84</v>
@@ -4609,23 +4591,23 @@
     </row>
     <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B299" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B300" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B301" t="s">
         <v>202</v>
@@ -4633,7 +4615,7 @@
     </row>
     <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B302" t="s">
         <v>119</v>
@@ -4641,33 +4623,33 @@
     </row>
     <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E306" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B307" t="s">
         <v>114</v>
@@ -4675,7 +4657,7 @@
     </row>
     <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B308" t="s">
         <v>40</v>
@@ -4683,23 +4665,23 @@
     </row>
     <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B309" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B310" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B311" s="14" t="s">
         <v>46</v>
@@ -4707,7 +4689,7 @@
     </row>
     <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B312" t="s">
         <v>110</v>
@@ -4715,52 +4697,52 @@
     </row>
     <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B313" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="314" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A314" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B315" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="316" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A316" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B318" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>151</v>
@@ -4768,20 +4750,20 @@
     </row>
     <row r="320" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A320" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B322" t="s">
         <v>42</v>
@@ -4789,31 +4771,31 @@
     </row>
     <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B323" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B324" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B325" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B326" t="s">
         <v>135</v>
@@ -4821,23 +4803,23 @@
     </row>
     <row r="327" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B328" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B329" t="s">
         <v>60</v>
@@ -4845,31 +4827,31 @@
     </row>
     <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B330" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B331" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B332" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B333" t="s">
         <v>80</v>
@@ -4877,136 +4859,136 @@
     </row>
     <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B334" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B335" s="10" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B336" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B337" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B338" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B339" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B340" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B341" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B343" s="7"/>
     </row>
     <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B344" s="7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B347" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B348" s="7" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B349" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="350" spans="1:7" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B350" s="9" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D350" s="7"/>
       <c r="E350" s="7"/>
@@ -5015,10 +4997,10 @@
     </row>
     <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B351" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D351" s="7"/>
       <c r="E351" s="7"/>
@@ -5027,7 +5009,7 @@
     </row>
     <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B352" s="7"/>
       <c r="E352" s="7"/>
@@ -5036,10 +5018,10 @@
     </row>
     <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B353" s="10" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E353" s="7"/>
       <c r="F353" s="7"/>
@@ -5047,10 +5029,10 @@
     </row>
     <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B354" s="7" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E354" s="7"/>
       <c r="F354" s="7"/>
@@ -5058,10 +5040,10 @@
     </row>
     <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B355" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E355" s="7"/>
       <c r="F355" s="7"/>
@@ -5069,10 +5051,10 @@
     </row>
     <row r="356" spans="1:7" ht="19.8" hidden="1" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B356" s="7" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D356" s="8"/>
       <c r="E356" s="7"/>
@@ -5081,10 +5063,10 @@
     </row>
     <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B357" s="7" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D357" s="7"/>
       <c r="E357" s="7"/>
@@ -5093,10 +5075,10 @@
     </row>
     <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E358" s="7"/>
       <c r="F358" s="7"/>
@@ -5104,10 +5086,10 @@
     </row>
     <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E359" s="7"/>
       <c r="F359" s="7"/>
@@ -5115,10 +5097,10 @@
     </row>
     <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B360" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E360" s="7"/>
       <c r="F360" s="7"/>
@@ -5126,10 +5108,10 @@
     </row>
     <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B361" s="10" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="E361" s="7"/>
       <c r="F361" s="7"/>
@@ -5137,7 +5119,7 @@
     </row>
     <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E362" s="7"/>
       <c r="F362" s="7"/>
@@ -5184,7 +5166,7 @@
   <autoFilter ref="A1:H362" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="AlperK61"/>
+        <filter val="jy59zadi"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5194,12 +5176,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5406,15 +5385,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5439,10 +5422,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Luca, Corinna, Philipp ausgetragen
</commit_message>
<xml_diff>
--- a/Verwaltung/2021-10-26_Themenzuordnung.xlsx
+++ b/Verwaltung/2021-10-26_Themenzuordnung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\va60moli\Documents\GitHub\ManagingProjectsSuccessfully.github.io\Verwaltung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177DDD0A-4122-4367-B258-D0F2B2C19996}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1196D5E-BDEA-41F7-B395-19BF5217F8A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="7260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="604">
   <si>
     <t>Themen</t>
   </si>
@@ -2295,19 +2295,19 @@
   <dimension ref="A1:H369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="83.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="1" max="1" width="83.6328125" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2323,7 +2323,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -2380,12 +2380,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2489,12 +2489,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -2526,17 +2526,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2560,12 +2560,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2581,7 +2581,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -2597,12 +2597,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -2660,12 +2660,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -2721,17 +2721,17 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>98</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>100</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>102</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>104</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>108</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>110</v>
       </c>
@@ -2787,15 +2787,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>112</v>
       </c>
-      <c r="B63" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>114</v>
       </c>
@@ -2803,7 +2800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>115</v>
       </c>
@@ -2811,12 +2808,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>118</v>
       </c>
@@ -2824,7 +2821,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>120</v>
       </c>
@@ -2832,7 +2829,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>122</v>
       </c>
@@ -2840,7 +2837,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>124</v>
       </c>
@@ -2848,7 +2845,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>126</v>
       </c>
@@ -2856,7 +2853,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>127</v>
       </c>
@@ -2864,12 +2861,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>131</v>
       </c>
@@ -2877,7 +2874,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>133</v>
       </c>
@@ -2885,7 +2882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>134</v>
       </c>
@@ -2893,7 +2890,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>136</v>
       </c>
@@ -2901,7 +2898,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>137</v>
       </c>
@@ -2909,7 +2906,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>139</v>
       </c>
@@ -2917,7 +2914,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>141</v>
       </c>
@@ -2925,7 +2922,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>143</v>
       </c>
@@ -2933,7 +2930,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>145</v>
       </c>
@@ -2941,7 +2938,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>147</v>
       </c>
@@ -2949,12 +2946,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>150</v>
       </c>
@@ -2962,7 +2959,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>152</v>
       </c>
@@ -2970,7 +2967,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>154</v>
       </c>
@@ -2978,7 +2975,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>156</v>
       </c>
@@ -2986,7 +2983,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>158</v>
       </c>
@@ -2994,7 +2991,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>159</v>
       </c>
@@ -3002,7 +2999,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>161</v>
       </c>
@@ -3010,7 +3007,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>163</v>
       </c>
@@ -3018,7 +3015,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>165</v>
       </c>
@@ -3026,7 +3023,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>167</v>
       </c>
@@ -3034,7 +3031,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>169</v>
       </c>
@@ -3042,7 +3039,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>171</v>
       </c>
@@ -3050,7 +3047,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>173</v>
       </c>
@@ -3058,7 +3055,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>175</v>
       </c>
@@ -3066,7 +3063,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>177</v>
       </c>
@@ -3074,7 +3071,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>179</v>
       </c>
@@ -3082,12 +3079,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>182</v>
       </c>
@@ -3095,7 +3092,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>184</v>
       </c>
@@ -3103,7 +3100,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>186</v>
       </c>
@@ -3111,7 +3108,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>188</v>
       </c>
@@ -3119,7 +3116,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>189</v>
       </c>
@@ -3128,7 +3125,7 @@
       </c>
       <c r="C106" s="3"/>
     </row>
-    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>190</v>
       </c>
@@ -3136,7 +3133,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>192</v>
       </c>
@@ -3144,7 +3141,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>194</v>
       </c>
@@ -3152,12 +3149,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>198</v>
       </c>
@@ -3165,7 +3162,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>200</v>
       </c>
@@ -3173,7 +3170,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>202</v>
       </c>
@@ -3181,12 +3178,12 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>205</v>
       </c>
@@ -3194,7 +3191,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>207</v>
       </c>
@@ -3202,7 +3199,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>209</v>
       </c>
@@ -3210,7 +3207,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>210</v>
       </c>
@@ -3218,7 +3215,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>211</v>
       </c>
@@ -3226,7 +3223,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>213</v>
       </c>
@@ -3234,7 +3231,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>215</v>
       </c>
@@ -3242,7 +3239,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>217</v>
       </c>
@@ -3250,7 +3247,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>219</v>
       </c>
@@ -3258,7 +3255,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>221</v>
       </c>
@@ -3266,7 +3263,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>223</v>
       </c>
@@ -3274,7 +3271,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>225</v>
       </c>
@@ -3282,7 +3279,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>227</v>
       </c>
@@ -3290,7 +3287,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>228</v>
       </c>
@@ -3298,7 +3295,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>229</v>
       </c>
@@ -3306,12 +3303,12 @@
         <v>595</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>232</v>
       </c>
@@ -3319,7 +3316,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>234</v>
       </c>
@@ -3327,12 +3324,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>237</v>
       </c>
@@ -3340,7 +3337,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>239</v>
       </c>
@@ -3348,7 +3345,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>241</v>
       </c>
@@ -3356,7 +3353,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>243</v>
       </c>
@@ -3364,7 +3361,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>244</v>
       </c>
@@ -3372,7 +3369,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>246</v>
       </c>
@@ -3380,7 +3377,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>247</v>
       </c>
@@ -3388,7 +3385,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>248</v>
       </c>
@@ -3396,12 +3393,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>251</v>
       </c>
@@ -3409,17 +3406,17 @@
         <v>224</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>255</v>
       </c>
@@ -3427,7 +3424,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>256</v>
       </c>
@@ -3435,7 +3432,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>257</v>
       </c>
@@ -3443,7 +3440,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>258</v>
       </c>
@@ -3451,7 +3448,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>260</v>
       </c>
@@ -3459,7 +3456,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>262</v>
       </c>
@@ -3467,7 +3464,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>264</v>
       </c>
@@ -3475,17 +3472,17 @@
         <v>86</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>267</v>
       </c>
@@ -3493,7 +3490,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>268</v>
       </c>
@@ -3501,7 +3498,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>269</v>
       </c>
@@ -3509,7 +3506,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>270</v>
       </c>
@@ -3517,7 +3514,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>272</v>
       </c>
@@ -3525,7 +3522,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>274</v>
       </c>
@@ -3533,7 +3530,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>276</v>
       </c>
@@ -3541,7 +3538,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>278</v>
       </c>
@@ -3549,7 +3546,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="4" t="s">
         <v>279</v>
       </c>
@@ -3557,7 +3554,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>281</v>
       </c>
@@ -3565,7 +3562,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>283</v>
       </c>
@@ -3573,7 +3570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>284</v>
       </c>
@@ -3581,12 +3578,12 @@
         <v>285</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>287</v>
       </c>
@@ -3594,7 +3591,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>288</v>
       </c>
@@ -3602,7 +3599,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>290</v>
       </c>
@@ -3610,12 +3607,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>293</v>
       </c>
@@ -3623,7 +3620,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>294</v>
       </c>
@@ -3631,7 +3628,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>296</v>
       </c>
@@ -3639,12 +3636,12 @@
         <v>297</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>300</v>
       </c>
@@ -3652,7 +3649,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>302</v>
       </c>
@@ -3660,7 +3657,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>304</v>
       </c>
@@ -3668,7 +3665,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>305</v>
       </c>
@@ -3676,17 +3673,17 @@
         <v>306</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>309</v>
       </c>
@@ -3694,7 +3691,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>311</v>
       </c>
@@ -3702,7 +3699,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>312</v>
       </c>
@@ -3710,7 +3707,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>314</v>
       </c>
@@ -3718,20 +3715,17 @@
         <v>315</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>316</v>
       </c>
-      <c r="B186" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>318</v>
       </c>
@@ -3739,7 +3733,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>320</v>
       </c>
@@ -3747,7 +3741,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>322</v>
       </c>
@@ -3755,7 +3749,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>324</v>
       </c>
@@ -3763,7 +3757,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>325</v>
       </c>
@@ -3771,7 +3765,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>326</v>
       </c>
@@ -3779,7 +3773,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>328</v>
       </c>
@@ -3787,7 +3781,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>330</v>
       </c>
@@ -3795,12 +3789,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>333</v>
       </c>
@@ -3808,7 +3802,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>335</v>
       </c>
@@ -3816,7 +3810,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>337</v>
       </c>
@@ -3824,7 +3818,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>339</v>
       </c>
@@ -3832,7 +3826,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>341</v>
       </c>
@@ -3840,7 +3834,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>343</v>
       </c>
@@ -3848,7 +3842,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>345</v>
       </c>
@@ -3856,7 +3850,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>347</v>
       </c>
@@ -3864,7 +3858,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>349</v>
       </c>
@@ -3872,7 +3866,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>350</v>
       </c>
@@ -3880,7 +3874,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>352</v>
       </c>
@@ -3888,7 +3882,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>539</v>
       </c>
@@ -3896,7 +3890,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>354</v>
       </c>
@@ -3904,7 +3898,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>356</v>
       </c>
@@ -3912,7 +3906,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>358</v>
       </c>
@@ -3920,7 +3914,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>360</v>
       </c>
@@ -3928,7 +3922,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>362</v>
       </c>
@@ -3936,7 +3930,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>364</v>
       </c>
@@ -3944,7 +3938,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>366</v>
       </c>
@@ -3952,7 +3946,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>367</v>
       </c>
@@ -3960,7 +3954,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>369</v>
       </c>
@@ -3968,7 +3962,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>371</v>
       </c>
@@ -3976,7 +3970,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>373</v>
       </c>
@@ -3984,7 +3978,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>374</v>
       </c>
@@ -3992,7 +3986,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>375</v>
       </c>
@@ -4000,7 +3994,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>377</v>
       </c>
@@ -4008,7 +4002,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>379</v>
       </c>
@@ -4016,7 +4010,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>381</v>
       </c>
@@ -4024,12 +4018,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>384</v>
       </c>
@@ -4037,7 +4031,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>386</v>
       </c>
@@ -4045,7 +4039,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>388</v>
       </c>
@@ -4053,7 +4047,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>390</v>
       </c>
@@ -4061,7 +4055,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>392</v>
       </c>
@@ -4069,7 +4063,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>394</v>
       </c>
@@ -4077,7 +4071,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>395</v>
       </c>
@@ -4085,7 +4079,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>397</v>
       </c>
@@ -4093,12 +4087,12 @@
         <v>327</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>399</v>
       </c>
@@ -4106,7 +4100,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>400</v>
       </c>
@@ -4114,7 +4108,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>402</v>
       </c>
@@ -4122,7 +4116,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>404</v>
       </c>
@@ -4130,7 +4124,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>406</v>
       </c>
@@ -4138,7 +4132,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>408</v>
       </c>
@@ -4146,7 +4140,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>409</v>
       </c>
@@ -4154,7 +4148,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>411</v>
       </c>
@@ -4162,7 +4156,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>413</v>
       </c>
@@ -4170,7 +4164,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>414</v>
       </c>
@@ -4178,7 +4172,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>416</v>
       </c>
@@ -4186,7 +4180,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>418</v>
       </c>
@@ -4194,7 +4188,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>420</v>
       </c>
@@ -4202,12 +4196,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>422</v>
       </c>
@@ -4215,7 +4209,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>424</v>
       </c>
@@ -4223,7 +4217,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>426</v>
       </c>
@@ -4231,7 +4225,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>428</v>
       </c>
@@ -4239,7 +4233,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>429</v>
       </c>
@@ -4247,7 +4241,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>431</v>
       </c>
@@ -4255,7 +4249,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>432</v>
       </c>
@@ -4263,7 +4257,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>433</v>
       </c>
@@ -4271,7 +4265,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>434</v>
       </c>
@@ -4279,7 +4273,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>435</v>
       </c>
@@ -4287,7 +4281,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>436</v>
       </c>
@@ -4295,7 +4289,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>437</v>
       </c>
@@ -4303,7 +4297,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>439</v>
       </c>
@@ -4311,7 +4305,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>441</v>
       </c>
@@ -4319,7 +4313,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>443</v>
       </c>
@@ -4327,12 +4321,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>445</v>
       </c>
@@ -4340,7 +4334,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>447</v>
       </c>
@@ -4348,7 +4342,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>449</v>
       </c>
@@ -4356,7 +4350,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>450</v>
       </c>
@@ -4364,7 +4358,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>451</v>
       </c>
@@ -4372,17 +4366,17 @@
         <v>452</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>455</v>
       </c>
@@ -4390,12 +4384,12 @@
         <v>586</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>457</v>
       </c>
@@ -4403,7 +4397,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>459</v>
       </c>
@@ -4411,12 +4405,12 @@
         <v>299</v>
       </c>
     </row>
-    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>461</v>
       </c>
@@ -4424,7 +4418,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>463</v>
       </c>
@@ -4432,7 +4426,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>465</v>
       </c>
@@ -4440,7 +4434,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>466</v>
       </c>
@@ -4448,7 +4442,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>467</v>
       </c>
@@ -4456,7 +4450,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>469</v>
       </c>
@@ -4464,7 +4458,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>470</v>
       </c>
@@ -4472,7 +4466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>471</v>
       </c>
@@ -4480,7 +4474,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>472</v>
       </c>
@@ -4488,22 +4482,22 @@
         <v>552</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>476</v>
       </c>
@@ -4511,7 +4505,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>477</v>
       </c>
@@ -4519,7 +4513,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>479</v>
       </c>
@@ -4527,7 +4521,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>480</v>
       </c>
@@ -4535,7 +4529,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>481</v>
       </c>
@@ -4543,12 +4537,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>483</v>
       </c>
@@ -4556,12 +4550,12 @@
         <v>306</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>485</v>
       </c>
@@ -4569,7 +4563,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>486</v>
       </c>
@@ -4577,7 +4571,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>487</v>
       </c>
@@ -4585,7 +4579,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>488</v>
       </c>
@@ -4593,7 +4587,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>490</v>
       </c>
@@ -4601,7 +4595,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>491</v>
       </c>
@@ -4609,22 +4603,22 @@
         <v>116</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>495</v>
       </c>
@@ -4635,7 +4629,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>496</v>
       </c>
@@ -4643,7 +4637,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>497</v>
       </c>
@@ -4651,7 +4645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>498</v>
       </c>
@@ -4659,7 +4653,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>499</v>
       </c>
@@ -4667,7 +4661,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>501</v>
       </c>
@@ -4675,7 +4669,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>502</v>
       </c>
@@ -4683,7 +4677,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>503</v>
       </c>
@@ -4691,7 +4685,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="314" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>504</v>
       </c>
@@ -4699,7 +4693,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>505</v>
       </c>
@@ -4707,7 +4701,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="316" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>506</v>
       </c>
@@ -4715,12 +4709,12 @@
         <v>599</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>508</v>
       </c>
@@ -4728,7 +4722,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>510</v>
       </c>
@@ -4736,7 +4730,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="320" spans="1:5" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:5" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>600</v>
       </c>
@@ -4744,12 +4738,12 @@
         <v>593</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>512</v>
       </c>
@@ -4757,7 +4751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>513</v>
       </c>
@@ -4765,7 +4759,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>515</v>
       </c>
@@ -4773,7 +4767,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>516</v>
       </c>
@@ -4781,7 +4775,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>517</v>
       </c>
@@ -4789,7 +4783,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="16.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:2" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>538</v>
       </c>
@@ -4797,7 +4791,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>518</v>
       </c>
@@ -4805,7 +4799,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>519</v>
       </c>
@@ -4813,7 +4807,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A330" s="4" t="s">
         <v>520</v>
       </c>
@@ -4821,7 +4815,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A331" s="4" t="s">
         <v>522</v>
       </c>
@@ -4829,7 +4823,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A332" s="4" t="s">
         <v>523</v>
       </c>
@@ -4837,7 +4831,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>524</v>
       </c>
@@ -4845,7 +4839,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>525</v>
       </c>
@@ -4853,7 +4847,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>526</v>
       </c>
@@ -4861,7 +4855,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>527</v>
       </c>
@@ -4869,7 +4863,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>529</v>
       </c>
@@ -4877,7 +4871,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>531</v>
       </c>
@@ -4885,7 +4879,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>533</v>
       </c>
@@ -4893,7 +4887,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>535</v>
       </c>
@@ -4901,7 +4895,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>537</v>
       </c>
@@ -4909,7 +4903,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>561</v>
       </c>
@@ -4917,13 +4911,13 @@
         <v>544</v>
       </c>
     </row>
-    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>556</v>
       </c>
       <c r="B343" s="7"/>
     </row>
-    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>560</v>
       </c>
@@ -4931,7 +4925,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>557</v>
       </c>
@@ -4939,7 +4933,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>558</v>
       </c>
@@ -4947,7 +4941,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>559</v>
       </c>
@@ -4955,7 +4949,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>562</v>
       </c>
@@ -4963,7 +4957,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>563</v>
       </c>
@@ -4971,7 +4965,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="19.2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:7" ht="17.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>564</v>
       </c>
@@ -4983,7 +4977,7 @@
       <c r="F350" s="7"/>
       <c r="G350" s="7"/>
     </row>
-    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>565</v>
       </c>
@@ -4995,7 +4989,7 @@
       <c r="F351" s="7"/>
       <c r="G351" s="7"/>
     </row>
-    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>566</v>
       </c>
@@ -5004,7 +4998,7 @@
       <c r="F352" s="7"/>
       <c r="G352" s="7"/>
     </row>
-    <row r="353" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>567</v>
       </c>
@@ -5015,7 +5009,7 @@
       <c r="F353" s="7"/>
       <c r="G353" s="7"/>
     </row>
-    <row r="354" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A354" t="s">
         <v>568</v>
       </c>
@@ -5026,7 +5020,7 @@
       <c r="F354" s="7"/>
       <c r="G354" s="7"/>
     </row>
-    <row r="355" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>569</v>
       </c>
@@ -5037,7 +5031,7 @@
       <c r="F355" s="7"/>
       <c r="G355" s="7"/>
     </row>
-    <row r="356" spans="1:7" ht="19.8" hidden="1" x14ac:dyDescent="0.4">
+    <row r="356" spans="1:7" ht="19.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
         <v>570</v>
       </c>
@@ -5049,7 +5043,7 @@
       <c r="F356" s="7"/>
       <c r="G356" s="7"/>
     </row>
-    <row r="357" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>571</v>
       </c>
@@ -5061,7 +5055,7 @@
       <c r="F357" s="7"/>
       <c r="G357" s="7"/>
     </row>
-    <row r="358" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>572</v>
       </c>
@@ -5072,18 +5066,16 @@
       <c r="F358" s="7"/>
       <c r="G358" s="7"/>
     </row>
-    <row r="359" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>573</v>
       </c>
-      <c r="B359" s="7" t="s">
-        <v>551</v>
-      </c>
+      <c r="B359" s="7"/>
       <c r="E359" s="7"/>
       <c r="F359" s="7"/>
       <c r="G359" s="7"/>
     </row>
-    <row r="360" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A360" t="s">
         <v>574</v>
       </c>
@@ -5094,7 +5086,7 @@
       <c r="F360" s="7"/>
       <c r="G360" s="7"/>
     </row>
-    <row r="361" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>576</v>
       </c>
@@ -5105,7 +5097,7 @@
       <c r="F361" s="7"/>
       <c r="G361" s="7"/>
     </row>
-    <row r="362" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>575</v>
       </c>
@@ -5113,38 +5105,38 @@
       <c r="F362" s="7"/>
       <c r="G362" s="7"/>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="E363" s="7"/>
       <c r="F363" s="7"/>
       <c r="G363" s="7"/>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
       <c r="F364" s="7"/>
       <c r="G364" s="7"/>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="E365" s="7"/>
       <c r="F365" s="7"/>
       <c r="G365" s="7"/>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="E366" s="7"/>
       <c r="F366" s="7"/>
       <c r="G366" s="7"/>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="E367" s="7"/>
       <c r="F367" s="7"/>
       <c r="G367" s="7"/>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="E368" s="7"/>
       <c r="F368" s="7"/>
       <c r="G368" s="7"/>
     </row>
-    <row r="369" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="369" spans="4:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
       <c r="F369" s="7"/>
@@ -5152,9 +5144,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H362" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
+    <filterColumn colId="0">
       <filters>
-        <filter val="BraNico"/>
+        <filter val="Leuchtturmprojekt"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5164,12 +5156,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5376,15 +5365,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5409,10 +5402,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDF2884C-80D2-4D39-BE35-36A86E185C63}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{197517D7-00A0-46DC-8AA3-E9140408A107}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>